<commit_message>
Solved problem 2785 (medium)
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="20"/>
+    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3343" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="1543">
   <si>
     <t>Date</t>
   </si>
@@ -3618,6 +3618,9 @@
   </si>
   <si>
     <t>Remove Letter To Equalize Frequency</t>
+  </si>
+  <si>
+    <t>Sort Vowels in a String</t>
   </si>
   <si>
     <t>Split Strings by Separator</t>
@@ -25233,8 +25236,8 @@
   <sheetPr/>
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="E199" sqref="E199"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -27996,8 +27999,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
-      <c r="A208" s="35"/>
+    <row r="208" spans="1:4">
+      <c r="A208" s="38">
+        <v>45133</v>
+      </c>
+      <c r="B208" s="1">
+        <v>2785</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="38">
@@ -28007,7 +28021,7 @@
         <v>2788</v>
       </c>
       <c r="C209" s="16" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>11</v>
@@ -28853,7 +28867,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -28876,7 +28890,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -28896,7 +28910,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -28916,7 +28930,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -28936,7 +28950,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -28954,7 +28968,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -28972,7 +28986,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -28990,7 +29004,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -29010,7 +29024,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -29028,7 +29042,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -29046,7 +29060,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -29064,7 +29078,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -29082,7 +29096,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -29156,7 +29170,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -29174,7 +29188,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -29194,7 +29208,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -29206,7 +29220,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -29219,7 +29233,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -29239,7 +29253,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -29262,7 +29276,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -29283,7 +29297,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -29304,7 +29318,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -29324,7 +29338,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -29342,7 +29356,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -29360,7 +29374,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -29378,7 +29392,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -29396,7 +29410,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -29432,7 +29446,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -29452,7 +29466,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -29461,7 +29475,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -29472,7 +29486,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -29490,7 +29504,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -29512,7 +29526,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -29521,7 +29535,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -29537,7 +29551,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -29563,7 +29577,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -29578,7 +29592,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -29592,7 +29606,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -29606,7 +29620,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -29618,7 +29632,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -29632,7 +29646,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -29644,7 +29658,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -29656,7 +29670,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -29670,7 +29684,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -29684,7 +29698,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -30985,7 +30999,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -31003,7 +31017,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -31025,7 +31039,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -31045,7 +31059,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31065,7 +31079,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31083,7 +31097,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -31101,7 +31115,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -31119,7 +31133,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -31135,7 +31149,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32576,7 +32590,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -32597,7 +32611,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -32615,7 +32629,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -32633,7 +32647,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32651,7 +32665,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -32672,7 +32686,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -32683,7 +32697,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -32693,7 +32707,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -32714,7 +32728,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -32732,7 +32746,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32750,7 +32764,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -32768,7 +32782,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -32786,7 +32800,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -32804,7 +32818,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -32824,7 +32838,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -32845,7 +32859,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -32864,7 +32878,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -32885,7 +32899,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -32905,7 +32919,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -32923,7 +32937,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -32943,7 +32957,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -32963,7 +32977,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -33013,7 +33027,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -33033,7 +33047,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -33051,7 +33065,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -33069,7 +33083,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -33087,7 +33101,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -33107,7 +33121,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -33125,7 +33139,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -33143,7 +33157,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -33161,7 +33175,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -33179,7 +33193,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -33197,7 +33211,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -33215,7 +33229,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -33233,7 +33247,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -33253,7 +33267,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -33271,7 +33285,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -33289,7 +33303,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -33307,7 +33321,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -33327,7 +33341,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -33347,7 +33361,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -33368,7 +33382,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -33388,7 +33402,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -33406,7 +33420,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -33426,7 +33440,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -34676,7 +34690,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -34694,7 +34708,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34714,7 +34728,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -34729,7 +34743,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -34744,7 +34758,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -34759,7 +34773,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -34768,10 +34782,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34783,14 +34797,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="29"/>
       <c r="I8" s="29" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34801,7 +34815,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -34821,7 +34835,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -34839,7 +34853,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -34857,7 +34871,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34877,7 +34891,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34897,7 +34911,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -34933,7 +34947,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -34951,7 +34965,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34969,7 +34983,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -34987,7 +35001,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -35027,7 +35041,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35045,7 +35059,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35065,7 +35079,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -35083,7 +35097,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -35106,7 +35120,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35127,7 +35141,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35146,7 +35160,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -35166,7 +35180,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35188,7 +35202,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -35224,7 +35238,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -35244,7 +35258,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -35264,7 +35278,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -35282,7 +35296,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -35300,7 +35314,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35318,7 +35332,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -35338,7 +35352,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -35358,7 +35372,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35378,7 +35392,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -35387,10 +35401,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -35402,7 +35416,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35420,7 +35434,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -35432,7 +35446,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -35444,7 +35458,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -35459,7 +35473,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -35483,7 +35497,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -35497,7 +35511,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -35509,7 +35523,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -35523,7 +35537,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -35537,7 +35551,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -35549,7 +35563,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -35561,7 +35575,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -35573,7 +35587,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -35585,7 +35599,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -35597,7 +35611,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -35609,7 +35623,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -35621,7 +35635,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -35635,7 +35649,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -35647,7 +35661,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -35659,7 +35673,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -35673,7 +35687,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -35685,7 +35699,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -35697,7 +35711,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -35709,7 +35723,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -35721,7 +35735,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -35772,7 +35786,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -35823,7 +35837,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -35876,7 +35890,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -35929,7 +35943,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -35980,7 +35994,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -36031,7 +36045,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -36082,7 +36096,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -36135,7 +36149,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -36186,7 +36200,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -36239,7 +36253,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -36290,7 +36304,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -36341,7 +36355,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -36394,7 +36408,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -36445,7 +36459,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -36498,7 +36512,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -36600,7 +36614,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -36704,7 +36718,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -36862,7 +36876,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -36915,7 +36929,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -37017,7 +37031,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -37070,7 +37084,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -37079,7 +37093,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -37179,7 +37193,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -37230,7 +37244,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -37283,7 +37297,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -37336,7 +37350,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -37440,7 +37454,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -37538,7 +37552,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -40717,7 +40731,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -40734,7 +40748,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -40751,7 +40765,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -40768,7 +40782,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -40787,7 +40801,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -40804,7 +40818,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -40821,7 +40835,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -40838,7 +40852,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -40857,7 +40871,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -40874,7 +40888,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -40891,7 +40905,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -40908,7 +40922,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -40925,7 +40939,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -40944,7 +40958,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -40961,7 +40975,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -40978,7 +40992,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -41511,7 +41525,7 @@
   <sheetPr/>
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
@@ -41563,14 +41577,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -41583,17 +41597,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -41603,7 +41617,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -41621,7 +41635,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -41637,7 +41651,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -41653,7 +41667,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -41669,7 +41683,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -41685,7 +41699,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -41703,17 +41717,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -41723,7 +41737,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -41741,17 +41755,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -41763,17 +41777,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -41785,7 +41799,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -41793,7 +41807,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="28"/>
       <c r="H14" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -41803,7 +41817,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -41820,7 +41834,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -41837,7 +41851,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -41856,7 +41870,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -41874,14 +41888,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -41894,14 +41908,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -41912,7 +41926,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -41928,14 +41942,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="28" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -41946,7 +41960,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -41964,7 +41978,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -41973,7 +41987,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -41984,7 +41998,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -42000,7 +42014,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -42016,7 +42030,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -42032,7 +42046,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -42048,7 +42062,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -42066,7 +42080,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -42082,7 +42096,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -42098,7 +42112,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -42114,7 +42128,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -42130,7 +42144,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -42164,14 +42178,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="28" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -42184,7 +42198,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -42200,7 +42214,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -42216,7 +42230,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -42250,7 +42264,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -42266,7 +42280,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -42284,7 +42298,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -42302,7 +42316,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -42320,13 +42334,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42337,7 +42351,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -42351,7 +42365,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -42365,7 +42379,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -42379,7 +42393,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -42391,7 +42405,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -42405,7 +42419,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -42419,7 +42433,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -42433,7 +42447,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -42447,7 +42461,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -42461,7 +42475,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -42473,7 +42487,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -42490,7 +42504,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -42502,7 +42516,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -42516,7 +42530,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -42533,7 +42547,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -42550,13 +42564,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42565,7 +42579,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -42579,7 +42593,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -42597,7 +42611,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -42611,13 +42625,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42628,7 +42642,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -42642,7 +42656,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -42656,7 +42670,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -42670,7 +42684,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -42682,7 +42696,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -42700,7 +42714,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -42714,13 +42728,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42731,7 +42745,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -42743,7 +42757,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -42757,13 +42771,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42772,7 +42786,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -42784,7 +42798,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -42798,7 +42812,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -42810,7 +42824,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -42822,7 +42836,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -42834,7 +42848,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -42848,13 +42862,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42865,7 +42879,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -42879,7 +42893,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -42893,7 +42907,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -42931,7 +42945,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -42945,7 +42959,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -42959,7 +42973,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -42989,7 +43003,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -43003,7 +43017,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -43017,7 +43031,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -43031,7 +43045,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -43045,7 +43059,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -43059,7 +43073,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -43073,7 +43087,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -43087,13 +43101,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43104,7 +43118,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -43118,7 +43132,7 @@
         <v>2739</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -43449,7 +43463,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43681,7 +43695,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43698,7 +43712,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43717,7 +43731,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43736,7 +43750,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43756,7 +43770,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43776,7 +43790,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -43797,7 +43811,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -43817,7 +43831,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -43827,10 +43841,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -43862,7 +43876,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -43882,7 +43896,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -43902,7 +43916,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -43925,7 +43939,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -43945,7 +43959,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -43965,19 +43979,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -43991,7 +44005,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44009,7 +44023,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44029,7 +44043,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44038,7 +44052,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44052,7 +44066,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44072,7 +44086,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44090,7 +44104,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44110,7 +44124,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44119,10 +44133,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44134,7 +44148,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44154,7 +44168,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44172,7 +44186,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44255,7 +44269,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44275,7 +44289,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44295,7 +44309,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44305,7 +44319,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44317,7 +44331,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44337,7 +44351,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44471,7 +44485,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44485,7 +44499,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44499,7 +44513,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44513,13 +44527,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
@@ -44716,7 +44730,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44738,13 +44752,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44758,13 +44772,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44775,7 +44789,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44789,7 +44803,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -44803,7 +44817,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44817,7 +44831,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -44840,7 +44854,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44849,7 +44863,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -44900,7 +44914,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44921,14 +44935,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -44944,7 +44958,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -44979,7 +44993,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -44988,7 +45002,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45025,7 +45039,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45046,7 +45060,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45056,7 +45070,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46515,7 +46529,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46530,13 +46544,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46577,7 +46591,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46592,7 +46606,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46652,7 +46666,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46665,7 +46679,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46690,7 +46704,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46703,7 +46717,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46716,7 +46730,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46729,7 +46743,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46744,7 +46758,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46759,7 +46773,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46772,7 +46786,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46787,7 +46801,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2744 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="13"/>
+    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3347" uniqueCount="1544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3349" uniqueCount="1545">
   <si>
     <t>Date</t>
   </si>
@@ -3621,6 +3621,9 @@
   </si>
   <si>
     <t>Remove Letter To Equalize Frequency</t>
+  </si>
+  <si>
+    <t>Find Maximum Number of String Pairs</t>
   </si>
   <si>
     <t>Sort Vowels in a String</t>
@@ -13726,7 +13729,7 @@
   <sheetPr/>
   <dimension ref="A1:AV281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+    <sheetView topLeftCell="A246" workbookViewId="0">
       <selection activeCell="E273" sqref="E273"/>
     </sheetView>
   </sheetViews>
@@ -25251,10 +25254,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I210"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C218" sqref="C218"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -28018,34 +28021,48 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="38">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B208" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>1147</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="38">
+        <v>45133</v>
+      </c>
+      <c r="B209" s="1">
+        <v>2785</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="38">
         <v>45131</v>
       </c>
-      <c r="B209" s="1">
+      <c r="B210" s="1">
         <v>2788</v>
       </c>
-      <c r="C209" s="16" t="s">
-        <v>1148</v>
-      </c>
-      <c r="D209" s="1" t="s">
+      <c r="C210" s="16" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
-      <c r="A210" s="35"/>
+    <row r="211" spans="1:1">
+      <c r="A211" s="35"/>
     </row>
   </sheetData>
   <sortState ref="A5:I62">
@@ -28333,262 +28350,262 @@
       <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A207">
+  <conditionalFormatting sqref="F209">
+    <cfRule type="containsText" dxfId="5" priority="27" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="35" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="43" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="51" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="75" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="83" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="91" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D210">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210">
+    <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="34" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="42" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="66" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="74" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="82" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="90" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F211">
+    <cfRule type="containsText" dxfId="5" priority="25" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="41" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="49" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="73" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="81" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="89" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A207:A208">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
-    <cfRule type="cellIs" dxfId="3" priority="19" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="18" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
+  <conditionalFormatting sqref="E45:E47">
+    <cfRule type="cellIs" dxfId="0" priority="192" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:F47">
+    <cfRule type="cellIs" dxfId="0" priority="185" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F207:F208">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="12" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="14" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="18" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 A212:E1048576 G212:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="191" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="193" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="194" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="195" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="196" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F212:F1048576">
+    <cfRule type="containsText" dxfId="5" priority="180" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="181" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="182" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="12" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="11" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F208">
-    <cfRule type="cellIs" dxfId="3" priority="91" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="83" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="75" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="67" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="59" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="51" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="43" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="35" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="27" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D209">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F209">
-    <cfRule type="cellIs" dxfId="3" priority="90" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="82" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="74" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="66" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="58" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="50" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="42" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="34" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
-    <cfRule type="cellIs" dxfId="3" priority="89" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="81" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="73" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="65" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="57" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="49" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="41" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="25" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:E47">
-    <cfRule type="cellIs" dxfId="0" priority="192" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:F47">
-    <cfRule type="cellIs" dxfId="0" priority="185" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 G211:XFD1048576 A196:B196 D196:E196 A197:E202 A211:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="191" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="193" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="194" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="195" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="196" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F211:F1048576">
-    <cfRule type="containsText" dxfId="5" priority="180" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="181" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="184" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="186" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="187" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="188" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="189" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="183" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="182" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="184" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="186" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="187" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="188" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="189" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:XFD187 A187:E187">
@@ -28723,92 +28740,92 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:XFD207 B207:E207">
+  <conditionalFormatting sqref="G207:XFD208 B207:E208">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="22" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="23" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="24" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="23" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="22" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="20" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G208:XFD208 A208:E208">
+  <conditionalFormatting sqref="G209:XFD209 A209:E209">
+    <cfRule type="cellIs" dxfId="0" priority="99" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="107" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="115" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="123" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="131" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="123" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="115" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="107" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="99" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:XFD209 A209:C209 E209">
+  <conditionalFormatting sqref="G210:XFD210 E210 A210:C210">
+    <cfRule type="cellIs" dxfId="0" priority="98" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="106" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="114" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="122" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="130" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="122" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="114" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="106" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="98" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G210:XFD210 A210:E210">
+  <conditionalFormatting sqref="G211:XFD211 A211:E211">
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="113" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="121" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="129" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="121" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="113" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="105" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="97" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -28884,7 +28901,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -28907,7 +28924,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -28927,7 +28944,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -28947,7 +28964,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -28967,7 +28984,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -28985,7 +29002,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -29003,7 +29020,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -29021,7 +29038,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -29041,7 +29058,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -29059,7 +29076,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -29077,7 +29094,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -29095,7 +29112,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -29113,7 +29130,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -29187,7 +29204,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -29205,7 +29222,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -29225,7 +29242,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -29237,7 +29254,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -29250,7 +29267,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -29270,7 +29287,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -29293,7 +29310,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -29314,7 +29331,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -29335,7 +29352,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -29355,7 +29372,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -29373,7 +29390,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -29391,7 +29408,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -29409,7 +29426,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -29427,7 +29444,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -29463,7 +29480,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -29483,7 +29500,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -29492,7 +29509,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -29503,7 +29520,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -29521,7 +29538,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -29543,7 +29560,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -29552,7 +29569,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -29568,7 +29585,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -29594,7 +29611,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -29609,7 +29626,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -29623,7 +29640,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -29637,7 +29654,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -29649,7 +29666,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -29663,7 +29680,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -29675,7 +29692,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -29687,7 +29704,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -29701,7 +29718,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -29715,7 +29732,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -31016,7 +31033,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -31034,7 +31051,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -31056,7 +31073,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -31076,7 +31093,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31096,7 +31113,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31114,7 +31131,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -31132,7 +31149,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -31150,7 +31167,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -31166,7 +31183,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32607,7 +32624,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -32628,7 +32645,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -32646,7 +32663,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -32664,7 +32681,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32682,7 +32699,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -32703,7 +32720,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -32714,7 +32731,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -32724,7 +32741,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -32745,7 +32762,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -32763,7 +32780,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32781,7 +32798,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -32799,7 +32816,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -32817,7 +32834,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -32835,7 +32852,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -32855,7 +32872,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -32876,7 +32893,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -32895,7 +32912,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -32916,7 +32933,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -32936,7 +32953,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -32954,7 +32971,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -32974,7 +32991,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -32994,7 +33011,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -33044,7 +33061,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -33064,7 +33081,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -33082,7 +33099,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -33100,7 +33117,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -33118,7 +33135,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -33138,7 +33155,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -33156,7 +33173,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -33174,7 +33191,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -33192,7 +33209,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -33210,7 +33227,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -33228,7 +33245,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -33246,7 +33263,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -33264,7 +33281,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -33284,7 +33301,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -33302,7 +33319,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -33320,7 +33337,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -33338,7 +33355,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -33358,7 +33375,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -33378,7 +33395,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -33399,7 +33416,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -33419,7 +33436,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -33437,7 +33454,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -33457,7 +33474,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -34707,7 +34724,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -34725,7 +34742,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34745,7 +34762,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -34760,7 +34777,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -34775,7 +34792,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -34790,7 +34807,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -34799,10 +34816,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34814,14 +34831,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="29"/>
       <c r="I8" s="29" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34832,7 +34849,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -34852,7 +34869,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -34870,7 +34887,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -34888,7 +34905,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34908,7 +34925,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34928,7 +34945,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -34964,7 +34981,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -34982,7 +34999,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -35000,7 +35017,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -35018,7 +35035,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -35058,7 +35075,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35076,7 +35093,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35096,7 +35113,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -35114,7 +35131,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -35137,7 +35154,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35158,7 +35175,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35177,7 +35194,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -35197,7 +35214,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35219,7 +35236,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -35255,7 +35272,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -35275,7 +35292,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -35295,7 +35312,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -35313,7 +35330,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -35331,7 +35348,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35349,7 +35366,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -35369,7 +35386,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -35389,7 +35406,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35409,7 +35426,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -35418,10 +35435,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -35433,7 +35450,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35451,7 +35468,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -35463,7 +35480,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -35475,7 +35492,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -35490,7 +35507,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -35514,7 +35531,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -35528,7 +35545,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -35540,7 +35557,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -35554,7 +35571,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -35568,7 +35585,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -35580,7 +35597,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -35592,7 +35609,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -35604,7 +35621,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -35616,7 +35633,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -35628,7 +35645,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -35640,7 +35657,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -35652,7 +35669,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -35666,7 +35683,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -35678,7 +35695,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -35690,7 +35707,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -35704,7 +35721,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -35716,7 +35733,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -35728,7 +35745,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -35740,7 +35757,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -35752,7 +35769,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -35803,7 +35820,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -35854,7 +35871,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -35907,7 +35924,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -35960,7 +35977,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -36011,7 +36028,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -36062,7 +36079,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -36113,7 +36130,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -36166,7 +36183,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -36217,7 +36234,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -36270,7 +36287,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -36321,7 +36338,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -36372,7 +36389,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -36425,7 +36442,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -36476,7 +36493,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -36529,7 +36546,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -36631,7 +36648,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -36735,7 +36752,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -36893,7 +36910,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -36946,7 +36963,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -37048,7 +37065,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -37101,7 +37118,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -37110,7 +37127,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -37210,7 +37227,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -37261,7 +37278,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -37314,7 +37331,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -37367,7 +37384,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -37471,7 +37488,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -37569,7 +37586,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -40748,7 +40765,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -40765,7 +40782,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -40782,7 +40799,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -40799,7 +40816,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -40818,7 +40835,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -40835,7 +40852,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -40852,7 +40869,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -40869,7 +40886,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -40888,7 +40905,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -40905,7 +40922,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -40922,7 +40939,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -40939,7 +40956,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -40956,7 +40973,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -40975,7 +40992,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -40992,7 +41009,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -41009,7 +41026,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -41594,14 +41611,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -41614,17 +41631,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -41634,7 +41651,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -41652,7 +41669,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -41668,7 +41685,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -41684,7 +41701,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -41700,7 +41717,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -41716,7 +41733,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -41734,17 +41751,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -41754,7 +41771,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -41772,17 +41789,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -41794,17 +41811,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -41816,7 +41833,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -41824,7 +41841,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="28"/>
       <c r="H14" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -41834,7 +41851,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -41851,7 +41868,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -41868,7 +41885,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -41887,7 +41904,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -41905,14 +41922,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -41925,14 +41942,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -41943,7 +41960,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -41959,14 +41976,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="28" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -41977,7 +41994,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -41995,7 +42012,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -42004,7 +42021,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -42015,7 +42032,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -42031,7 +42048,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -42047,7 +42064,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -42063,7 +42080,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -42079,7 +42096,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -42097,7 +42114,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -42113,7 +42130,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -42129,7 +42146,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -42145,7 +42162,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -42161,7 +42178,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -42195,14 +42212,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="28" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -42215,7 +42232,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -42231,7 +42248,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -42247,7 +42264,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -42281,7 +42298,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -42297,7 +42314,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -42315,7 +42332,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -42333,7 +42350,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -42351,13 +42368,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42368,7 +42385,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -42382,7 +42399,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -42396,7 +42413,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -42410,7 +42427,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -42422,7 +42439,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -42436,7 +42453,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -42450,7 +42467,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -42464,7 +42481,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -42478,7 +42495,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -42492,7 +42509,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -42504,7 +42521,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -42521,7 +42538,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -42533,7 +42550,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -42547,7 +42564,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -42564,7 +42581,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -42581,13 +42598,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42596,7 +42613,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -42610,7 +42627,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -42628,7 +42645,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -42642,13 +42659,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42659,7 +42676,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -42673,7 +42690,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -42687,7 +42704,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -42701,7 +42718,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -42713,7 +42730,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -42731,7 +42748,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -42745,13 +42762,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42762,7 +42779,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -42774,7 +42791,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -42788,13 +42805,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42803,7 +42820,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -42815,7 +42832,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -42829,7 +42846,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -42841,7 +42858,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -42853,7 +42870,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -42865,7 +42882,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -42879,13 +42896,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42896,7 +42913,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -42910,7 +42927,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -42924,7 +42941,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -42962,7 +42979,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -42976,7 +42993,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -42990,7 +43007,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -43020,7 +43037,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -43034,7 +43051,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -43048,7 +43065,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -43062,7 +43079,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -43076,7 +43093,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -43090,7 +43107,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -43104,7 +43121,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -43118,13 +43135,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43135,7 +43152,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -43149,7 +43166,7 @@
         <v>2739</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -43480,7 +43497,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43712,7 +43729,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43729,7 +43746,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43748,7 +43765,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43767,7 +43784,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43787,7 +43804,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43807,7 +43824,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -43828,7 +43845,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -43848,7 +43865,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -43858,10 +43875,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -43893,7 +43910,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -43913,7 +43930,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -43933,7 +43950,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -43956,7 +43973,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -43976,7 +43993,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -43996,19 +44013,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44022,7 +44039,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44040,7 +44057,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44060,7 +44077,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44069,7 +44086,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44083,7 +44100,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44103,7 +44120,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44121,7 +44138,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44141,7 +44158,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44150,10 +44167,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44165,7 +44182,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44185,7 +44202,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44203,7 +44220,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44286,7 +44303,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44306,7 +44323,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44326,7 +44343,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44336,7 +44353,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44348,7 +44365,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44368,7 +44385,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44502,7 +44519,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44516,7 +44533,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44530,7 +44547,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44544,13 +44561,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
@@ -44747,7 +44764,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44769,13 +44786,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44789,13 +44806,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44806,7 +44823,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44820,7 +44837,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -44834,7 +44851,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44848,7 +44865,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -44871,7 +44888,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44880,7 +44897,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -44931,7 +44948,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44952,14 +44969,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -44975,7 +44992,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45010,7 +45027,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45019,7 +45036,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45056,7 +45073,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45077,7 +45094,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45087,7 +45104,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46546,7 +46563,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46561,13 +46578,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46608,7 +46625,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46623,7 +46640,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46683,7 +46700,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46696,7 +46713,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46721,7 +46738,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46734,7 +46751,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46747,7 +46764,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46760,7 +46777,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46775,7 +46792,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46790,7 +46807,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46803,7 +46820,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46818,7 +46835,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2678 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="20"/>
+    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3351" uniqueCount="1546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="1547">
   <si>
     <t>Date</t>
   </si>
@@ -3621,6 +3621,9 @@
   </si>
   <si>
     <t>Remove Letter To Equalize Frequency</t>
+  </si>
+  <si>
+    <t>Number of Senior Citizens</t>
   </si>
   <si>
     <t>Find Maximum Number of String Pairs</t>
@@ -25260,10 +25263,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I211"/>
+  <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -28027,10 +28030,10 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="39">
-        <v>45134</v>
+        <v>45135</v>
       </c>
       <c r="B208" s="1">
-        <v>2744</v>
+        <v>2678</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>1147</v>
@@ -28041,34 +28044,48 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B209" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>1148</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
+        <v>45133</v>
+      </c>
+      <c r="B210" s="1">
+        <v>2785</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="39">
         <v>45131</v>
       </c>
-      <c r="B210" s="1">
+      <c r="B211" s="1">
         <v>2788</v>
       </c>
-      <c r="C210" s="16" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D210" s="1" t="s">
+      <c r="C211" s="16" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="36"/>
+    <row r="212" spans="1:1">
+      <c r="A212" s="36"/>
     </row>
   </sheetData>
   <sortState ref="A5:I62">
@@ -28356,12 +28373,12 @@
       <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209">
+  <conditionalFormatting sqref="F210">
     <cfRule type="containsText" dxfId="5" priority="27" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="35" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="43" operator="between">
       <formula>"Amazon"</formula>
@@ -28392,7 +28409,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D210">
+  <conditionalFormatting sqref="D211">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28414,12 +28431,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
+  <conditionalFormatting sqref="F211">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="34" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="42" operator="between">
       <formula>"Amazon"</formula>
@@ -28450,12 +28467,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F211">
+  <conditionalFormatting sqref="F212">
     <cfRule type="containsText" dxfId="5" priority="25" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="33" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="41" operator="between">
       <formula>"Amazon"</formula>
@@ -28486,7 +28503,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A207:A208">
+  <conditionalFormatting sqref="A207:A209">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28520,7 +28537,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207:F208">
+  <conditionalFormatting sqref="F207:F209">
     <cfRule type="containsText" dxfId="5" priority="11" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
@@ -28556,7 +28573,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 A212:E1048576 G212:XFD1048576">
+  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 G213:XFD1048576 A213:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="191" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28578,7 +28595,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F212:F1048576">
+  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F213:F1048576">
     <cfRule type="containsText" dxfId="5" priority="180" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -28746,7 +28763,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:XFD208 B207:E208">
+  <conditionalFormatting sqref="G207:XFD209 B207:E209">
     <cfRule type="cellIs" dxfId="0" priority="20" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28768,7 +28785,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:XFD209 A209:E209">
+  <conditionalFormatting sqref="G210:XFD210 A210:E210">
     <cfRule type="cellIs" dxfId="0" priority="99" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28790,7 +28807,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G210:XFD210 E210 A210:C210">
+  <conditionalFormatting sqref="G211:XFD211 A211:C211 E211">
     <cfRule type="cellIs" dxfId="0" priority="98" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28812,7 +28829,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G211:XFD211 A211:E211">
+  <conditionalFormatting sqref="G212:XFD212 A212:E212">
     <cfRule type="cellIs" dxfId="0" priority="97" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28907,7 +28924,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -28930,7 +28947,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -28950,7 +28967,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -28970,7 +28987,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -28990,7 +29007,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -29008,7 +29025,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -29026,7 +29043,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -29044,7 +29061,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -29064,7 +29081,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -29082,7 +29099,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -29100,7 +29117,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -29118,7 +29135,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -29136,7 +29153,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -29210,7 +29227,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -29228,7 +29245,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -29248,7 +29265,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -29260,7 +29277,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -29273,7 +29290,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -29293,7 +29310,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -29316,7 +29333,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -29337,7 +29354,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -29358,7 +29375,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -29378,7 +29395,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -29396,7 +29413,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -29414,7 +29431,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -29432,7 +29449,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -29450,7 +29467,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -29486,7 +29503,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -29506,7 +29523,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -29515,7 +29532,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -29526,7 +29543,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -29544,7 +29561,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -29566,7 +29583,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -29575,7 +29592,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -29591,7 +29608,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -29617,7 +29634,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -29632,7 +29649,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -29646,7 +29663,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -29660,7 +29677,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -29672,7 +29689,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -29686,7 +29703,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -29698,7 +29715,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -29710,7 +29727,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -29724,7 +29741,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -29738,7 +29755,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -31039,7 +31056,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -31057,7 +31074,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -31079,7 +31096,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -31099,7 +31116,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31119,7 +31136,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31137,7 +31154,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -31155,7 +31172,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -31173,7 +31190,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -31189,7 +31206,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32630,7 +32647,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -32651,7 +32668,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -32669,7 +32686,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -32687,7 +32704,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32705,7 +32722,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -32726,7 +32743,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -32737,7 +32754,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -32747,7 +32764,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -32768,7 +32785,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -32786,7 +32803,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32804,7 +32821,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -32822,7 +32839,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -32840,7 +32857,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -32858,7 +32875,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -32878,7 +32895,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -32899,7 +32916,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -32918,7 +32935,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -32939,7 +32956,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -32959,7 +32976,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -32977,7 +32994,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -32997,7 +33014,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -33017,7 +33034,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -33067,7 +33084,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -33087,7 +33104,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -33105,7 +33122,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -33123,7 +33140,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -33141,7 +33158,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -33161,7 +33178,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -33179,7 +33196,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -33197,7 +33214,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -33215,7 +33232,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -33233,7 +33250,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -33251,7 +33268,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -33269,7 +33286,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -33287,7 +33304,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -33307,7 +33324,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -33325,7 +33342,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -33343,7 +33360,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -33361,7 +33378,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -33381,7 +33398,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -33401,7 +33418,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -33422,7 +33439,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -33442,7 +33459,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -33460,7 +33477,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -33480,7 +33497,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -34730,7 +34747,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -34748,7 +34765,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34768,7 +34785,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -34783,7 +34800,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -34798,7 +34815,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -34813,7 +34830,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -34822,10 +34839,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34837,14 +34854,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34855,7 +34872,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -34875,7 +34892,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -34893,7 +34910,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -34911,7 +34928,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34931,7 +34948,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34951,7 +34968,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -34987,7 +35004,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -35005,7 +35022,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -35023,7 +35040,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -35041,7 +35058,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -35081,7 +35098,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35099,7 +35116,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35119,7 +35136,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -35137,7 +35154,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -35160,7 +35177,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35181,7 +35198,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35200,7 +35217,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -35220,7 +35237,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35242,7 +35259,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -35278,7 +35295,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -35298,7 +35315,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -35318,7 +35335,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -35336,7 +35353,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -35354,7 +35371,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35372,7 +35389,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -35392,7 +35409,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -35412,7 +35429,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35432,7 +35449,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -35441,10 +35458,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -35456,7 +35473,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35474,7 +35491,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -35486,7 +35503,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -35498,7 +35515,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -35513,7 +35530,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -35537,7 +35554,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -35551,7 +35568,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -35563,7 +35580,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -35577,7 +35594,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -35591,7 +35608,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -35603,7 +35620,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -35615,7 +35632,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -35627,7 +35644,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -35639,7 +35656,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -35651,7 +35668,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -35663,7 +35680,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -35675,7 +35692,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -35689,7 +35706,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -35701,7 +35718,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -35713,7 +35730,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -35727,7 +35744,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -35739,7 +35756,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -35751,7 +35768,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -35763,7 +35780,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -35775,7 +35792,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -35826,7 +35843,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -35877,7 +35894,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -35930,7 +35947,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -35983,7 +36000,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -36034,7 +36051,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -36085,7 +36102,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -36136,7 +36153,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -36189,7 +36206,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -36240,7 +36257,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -36293,7 +36310,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -36344,7 +36361,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -36395,7 +36412,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -36448,7 +36465,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -36499,7 +36516,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -36552,7 +36569,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -36654,7 +36671,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -36758,7 +36775,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -36916,7 +36933,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -36969,7 +36986,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -37071,7 +37088,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -37124,7 +37141,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -37133,7 +37150,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -37233,7 +37250,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -37284,7 +37301,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -37337,7 +37354,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -37390,7 +37407,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -37494,7 +37511,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -37592,7 +37609,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -40771,7 +40788,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -40788,7 +40805,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -40805,7 +40822,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -40822,7 +40839,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -40841,7 +40858,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -40858,7 +40875,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -40875,7 +40892,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -40892,7 +40909,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -40911,7 +40928,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -40928,7 +40945,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -40945,7 +40962,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -40962,7 +40979,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -40979,7 +40996,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -40998,7 +41015,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -41015,7 +41032,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -41032,7 +41049,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -41565,7 +41582,7 @@
   <sheetPr/>
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
@@ -41617,14 +41634,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -41637,17 +41654,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -41657,7 +41674,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -41675,7 +41692,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -41691,7 +41708,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -41707,7 +41724,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -41723,7 +41740,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -41739,7 +41756,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -41757,17 +41774,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -41777,7 +41794,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -41795,17 +41812,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -41817,17 +41834,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -41839,7 +41856,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -41847,7 +41864,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="28"/>
       <c r="H14" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -41857,7 +41874,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -41874,7 +41891,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -41891,7 +41908,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -41910,7 +41927,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -41928,14 +41945,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -41948,14 +41965,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -41966,7 +41983,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -41982,14 +41999,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="28" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -42000,7 +42017,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -42018,7 +42035,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -42027,7 +42044,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -42038,7 +42055,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -42054,7 +42071,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -42070,7 +42087,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -42086,7 +42103,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -42102,7 +42119,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -42120,7 +42137,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -42136,7 +42153,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -42152,7 +42169,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -42168,7 +42185,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -42184,7 +42201,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -42218,14 +42235,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="28" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -42238,7 +42255,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -42254,7 +42271,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -42270,7 +42287,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -42304,7 +42321,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -42320,7 +42337,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -42338,7 +42355,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -42356,7 +42373,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -42374,13 +42391,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42391,7 +42408,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -42405,7 +42422,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -42419,7 +42436,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -42433,7 +42450,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -42445,7 +42462,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -42459,7 +42476,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -42473,7 +42490,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -42487,7 +42504,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -42501,7 +42518,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -42515,7 +42532,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -42527,7 +42544,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -42544,7 +42561,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -42556,7 +42573,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -42570,7 +42587,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -42587,7 +42604,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -42604,13 +42621,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42619,7 +42636,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -42633,7 +42650,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -42651,7 +42668,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -42665,13 +42682,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42682,7 +42699,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -42696,7 +42713,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -42710,7 +42727,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -42724,7 +42741,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -42736,7 +42753,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -42754,7 +42771,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -42768,13 +42785,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42785,7 +42802,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -42797,7 +42814,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -42811,13 +42828,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42826,7 +42843,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -42838,7 +42855,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -42852,7 +42869,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -42864,7 +42881,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -42876,7 +42893,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -42888,7 +42905,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -42902,13 +42919,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42919,7 +42936,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -42933,7 +42950,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -42947,7 +42964,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -42985,7 +43002,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -42999,7 +43016,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -43013,7 +43030,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -43043,7 +43060,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -43057,7 +43074,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -43071,7 +43088,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -43085,7 +43102,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -43099,7 +43116,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -43113,7 +43130,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -43127,7 +43144,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -43141,13 +43158,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43158,7 +43175,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -43172,7 +43189,7 @@
         <v>2739</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -43186,7 +43203,7 @@
         <v>2745</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -43513,7 +43530,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43745,7 +43762,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43762,7 +43779,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43781,7 +43798,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43800,7 +43817,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43820,7 +43837,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43840,7 +43857,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -43861,7 +43878,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -43881,7 +43898,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -43891,10 +43908,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -43926,7 +43943,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -43946,7 +43963,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -43966,7 +43983,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -43989,7 +44006,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44009,7 +44026,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44029,19 +44046,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44055,7 +44072,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44073,7 +44090,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44093,7 +44110,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44102,7 +44119,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44116,7 +44133,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44136,7 +44153,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44154,7 +44171,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44174,7 +44191,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44183,10 +44200,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44198,7 +44215,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44218,7 +44235,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44236,7 +44253,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44319,7 +44336,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44339,7 +44356,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44359,7 +44376,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44369,7 +44386,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44381,7 +44398,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44401,7 +44418,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44535,7 +44552,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44549,7 +44566,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44563,7 +44580,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44577,13 +44594,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
@@ -44780,7 +44797,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44802,13 +44819,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44822,13 +44839,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44839,7 +44856,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44853,7 +44870,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -44867,7 +44884,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44881,7 +44898,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -44904,7 +44921,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44913,7 +44930,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -44964,7 +44981,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44985,14 +45002,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45008,7 +45025,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45043,7 +45060,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45052,7 +45069,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45089,7 +45106,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45110,7 +45127,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45120,7 +45137,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46579,7 +46596,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46594,13 +46611,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46641,7 +46658,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46656,7 +46673,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46716,7 +46733,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46729,7 +46746,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46754,7 +46771,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46767,7 +46784,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46780,7 +46797,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46793,7 +46810,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46808,7 +46825,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46823,7 +46840,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46836,7 +46853,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46851,7 +46868,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2740 Category: Sort Difficulty: Medium
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="5" activeTab="14"/>
+    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="8" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3355" uniqueCount="1548">
   <si>
     <t>Date</t>
   </si>
@@ -4750,6 +4750,9 @@
   </si>
   <si>
     <t>to_string</t>
+  </si>
+  <si>
+    <t>Find the Value of the Partition</t>
   </si>
   <si>
     <t>Range Sum Query - Immutable</t>
@@ -5645,12 +5648,12 @@
     <xf numFmtId="58" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -25265,7 +25268,7 @@
   <sheetPr/>
   <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+    <sheetView topLeftCell="A197" workbookViewId="0">
       <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
@@ -41588,7 +41591,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
   <cols>
-    <col min="1" max="1" width="11.4414414414414" style="27"/>
+    <col min="1" max="1" width="11.4414414414414" style="28"/>
     <col min="2" max="2" width="14.8918918918919" style="25" customWidth="1"/>
     <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
     <col min="4" max="4" width="9.10810810810811" style="8"/>
@@ -41862,7 +41865,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="14"/>
-      <c r="G14" s="28"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
         <v>1379</v>
       </c>
@@ -41881,7 +41884,7 @@
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="14"/>
       <c r="I15" s="19"/>
     </row>
@@ -41898,7 +41901,7 @@
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="28"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="14"/>
       <c r="I16" s="19"/>
     </row>
@@ -41917,7 +41920,7 @@
         <v>24</v>
       </c>
       <c r="F17" s="17"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="14"/>
       <c r="I17" s="19"/>
     </row>
@@ -41933,7 +41936,7 @@
         <v>11</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="G18" s="28"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="14"/>
       <c r="I18" s="19"/>
     </row>
@@ -42005,7 +42008,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="29" t="s">
         <v>1390</v>
       </c>
       <c r="H22" s="24"/>
@@ -42023,7 +42026,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="14"/>
-      <c r="G23" s="28"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="24"/>
       <c r="I23" s="19"/>
     </row>
@@ -42041,7 +42044,7 @@
         <v>13</v>
       </c>
       <c r="E24" s="14"/>
-      <c r="G24" s="28"/>
+      <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
         <v>1393</v>
@@ -42061,7 +42064,7 @@
         <v>13</v>
       </c>
       <c r="E25" s="14"/>
-      <c r="G25" s="28"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="24"/>
       <c r="I25" s="19"/>
     </row>
@@ -42077,7 +42080,7 @@
         <v>13</v>
       </c>
       <c r="E26" s="14"/>
-      <c r="G26" s="28"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="24"/>
       <c r="I26" s="19"/>
     </row>
@@ -42093,7 +42096,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="14"/>
-      <c r="G27" s="28"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="24"/>
       <c r="I27" s="19"/>
     </row>
@@ -42109,7 +42112,7 @@
         <v>13</v>
       </c>
       <c r="E28" s="14"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="24"/>
       <c r="I28" s="19"/>
     </row>
@@ -42125,7 +42128,7 @@
         <v>13</v>
       </c>
       <c r="E29" s="14"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="24"/>
       <c r="I29" s="19"/>
     </row>
@@ -42143,7 +42146,7 @@
         <v>13</v>
       </c>
       <c r="E30" s="14"/>
-      <c r="G30" s="28"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="24"/>
       <c r="I30" s="19"/>
     </row>
@@ -42159,7 +42162,7 @@
         <v>16</v>
       </c>
       <c r="E31" s="14"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="24"/>
       <c r="I31" s="19"/>
     </row>
@@ -42175,7 +42178,7 @@
         <v>13</v>
       </c>
       <c r="E32" s="14"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="24"/>
       <c r="I32" s="19"/>
     </row>
@@ -42191,7 +42194,7 @@
         <v>13</v>
       </c>
       <c r="E33" s="14"/>
-      <c r="G33" s="28"/>
+      <c r="G33" s="29"/>
       <c r="H33" s="24"/>
       <c r="I33" s="19"/>
     </row>
@@ -42207,7 +42210,7 @@
         <v>13</v>
       </c>
       <c r="E34" s="14"/>
-      <c r="G34" s="28"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="24"/>
       <c r="I34" s="19"/>
     </row>
@@ -42223,7 +42226,7 @@
         <v>13</v>
       </c>
       <c r="E35" s="14"/>
-      <c r="G35" s="28"/>
+      <c r="G35" s="29"/>
       <c r="H35" s="24"/>
       <c r="I35" s="19"/>
     </row>
@@ -42241,7 +42244,7 @@
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
-      <c r="G36" s="28" t="s">
+      <c r="G36" s="29" t="s">
         <v>1404</v>
       </c>
       <c r="H36" s="24"/>
@@ -42261,7 +42264,7 @@
         <v>11</v>
       </c>
       <c r="E37" s="14"/>
-      <c r="G37" s="28"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="24"/>
       <c r="I37" s="19"/>
     </row>
@@ -42277,7 +42280,7 @@
         <v>16</v>
       </c>
       <c r="E38" s="14"/>
-      <c r="G38" s="28"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="24"/>
       <c r="I38" s="19"/>
     </row>
@@ -42295,7 +42298,7 @@
       <c r="E39" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="28"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="24"/>
       <c r="I39" s="19"/>
     </row>
@@ -42311,7 +42314,7 @@
         <v>13</v>
       </c>
       <c r="E40" s="14"/>
-      <c r="G40" s="28"/>
+      <c r="G40" s="29"/>
       <c r="H40" s="24"/>
       <c r="I40" s="19"/>
     </row>
@@ -42327,7 +42330,7 @@
         <v>13</v>
       </c>
       <c r="E41" s="14"/>
-      <c r="G41" s="28"/>
+      <c r="G41" s="29"/>
       <c r="H41" s="24"/>
       <c r="I41" s="19"/>
     </row>
@@ -42343,7 +42346,7 @@
         <v>13</v>
       </c>
       <c r="E42" s="14"/>
-      <c r="G42" s="28"/>
+      <c r="G42" s="29"/>
       <c r="H42" s="24"/>
       <c r="I42" s="19"/>
     </row>
@@ -42361,7 +42364,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="14"/>
-      <c r="G43" s="28"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="24"/>
       <c r="I43" s="19"/>
     </row>
@@ -42379,7 +42382,7 @@
         <v>11</v>
       </c>
       <c r="E44" s="14"/>
-      <c r="G44" s="28"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="24"/>
       <c r="I44" s="19"/>
     </row>
@@ -43196,7 +43199,7 @@
       </c>
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A112" s="29">
+      <c r="A112" s="27">
         <v>45133</v>
       </c>
       <c r="B112" s="12">
@@ -43699,8 +43702,8 @@
   <sheetPr/>
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44603,9 +44606,19 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12"/>
+    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A50" s="27">
+        <v>45135</v>
+      </c>
+      <c r="B50" s="12">
+        <v>2740</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A51" s="11"/>
@@ -44819,13 +44832,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44839,13 +44852,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44856,7 +44869,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44870,7 +44883,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -44884,7 +44897,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44898,7 +44911,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -44930,7 +44943,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -44981,7 +44994,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45002,14 +45015,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45025,7 +45038,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45060,7 +45073,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45069,7 +45082,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45106,7 +45119,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45127,7 +45140,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45137,7 +45150,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46611,13 +46624,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46658,7 +46671,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46733,7 +46746,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46746,7 +46759,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46771,7 +46784,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46784,7 +46797,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46797,7 +46810,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46810,7 +46823,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46825,7 +46838,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46840,7 +46853,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46853,7 +46866,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46868,7 +46881,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2582 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="8" activeTab="13"/>
+    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="8" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3357" uniqueCount="1549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3359" uniqueCount="1550">
   <si>
     <t>Date</t>
   </si>
@@ -4621,6 +4621,9 @@
   </si>
   <si>
     <t>Largest Number After Digit Swaps by Parity</t>
+  </si>
+  <si>
+    <t>Pass the Pillow</t>
   </si>
   <si>
     <t>Total Distance Traveled</t>
@@ -13744,7 +13747,7 @@
   <sheetPr/>
   <dimension ref="A1:AV281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+    <sheetView topLeftCell="A246" workbookViewId="0">
       <selection activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
@@ -41599,10 +41602,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -43202,10 +43205,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A111" s="4">
-        <v>45131</v>
+        <v>45137</v>
       </c>
       <c r="B111" s="12">
-        <v>2739</v>
+        <v>2582</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>1473</v>
@@ -43215,11 +43218,11 @@
       </c>
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A112" s="27">
-        <v>45133</v>
+      <c r="A112" s="4">
+        <v>45131</v>
       </c>
       <c r="B112" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1474</v>
@@ -43228,9 +43231,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A113" s="11"/>
-      <c r="B113" s="12"/>
+    <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A113" s="27">
+        <v>45133</v>
+      </c>
+      <c r="B113" s="12">
+        <v>2745</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A114" s="11"/>
@@ -43243,6 +43256,10 @@
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A116" s="11"/>
       <c r="B116" s="12"/>
+    </row>
+    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A117" s="11"/>
+      <c r="B117" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -43340,7 +43357,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F116">
+  <conditionalFormatting sqref="F107:F117">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -43350,94 +43367,94 @@
     <cfRule type="containsText" priority="3" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F107)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G118:XFD1048576 A118:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="53" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="54" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="55" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="56" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F88 F90:F105 F118:F1048576">
+    <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
+      <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="32" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="34" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A117:E1048576 G117:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="54" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="55" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="56" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F117:F1048576">
-    <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="32" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="36" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="38" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="39" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="40" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="41" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="35" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="34" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="38" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="39" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="40" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="41" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:XFD106 A106:E106">
@@ -43462,7 +43479,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD116 A107:E116">
+  <conditionalFormatting sqref="G107:XFD117 A107:E117">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -43549,7 +43566,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43781,7 +43798,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43798,7 +43815,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43817,7 +43834,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43836,7 +43853,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43856,7 +43873,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43876,7 +43893,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -43897,7 +43914,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -43917,7 +43934,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -43927,10 +43944,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -43962,7 +43979,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -43982,7 +43999,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44002,7 +44019,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44025,7 +44042,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44045,7 +44062,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44065,19 +44082,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44091,7 +44108,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44109,7 +44126,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44129,7 +44146,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44138,7 +44155,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44152,7 +44169,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44172,7 +44189,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44190,7 +44207,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44210,7 +44227,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44219,10 +44236,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44234,7 +44251,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44254,7 +44271,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44272,7 +44289,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44355,7 +44372,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44375,7 +44392,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44395,7 +44412,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44405,7 +44422,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44417,7 +44434,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44437,7 +44454,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44571,7 +44588,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44585,7 +44602,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44599,7 +44616,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44613,13 +44630,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44630,7 +44647,7 @@
         <v>2740</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44848,13 +44865,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44868,13 +44885,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44885,7 +44902,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44899,7 +44916,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -44913,7 +44930,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44927,7 +44944,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -44959,7 +44976,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45010,7 +45027,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45031,14 +45048,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45054,7 +45071,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45089,7 +45106,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45098,7 +45115,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45135,7 +45152,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45156,7 +45173,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45166,7 +45183,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46640,13 +46657,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46687,7 +46704,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46702,7 +46719,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46762,7 +46779,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46775,7 +46792,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46800,7 +46817,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46813,7 +46830,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46826,7 +46843,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46839,7 +46856,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46854,7 +46871,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46869,7 +46886,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46882,7 +46899,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46897,7 +46914,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 0108 Category: Recursion Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20297" windowHeight="11545" tabRatio="991" firstSheet="8" activeTab="20"/>
+    <workbookView windowHeight="14544" tabRatio="991" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -6256,17 +6256,17 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.1081081081081" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="12" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="1"/>
-    <col min="5" max="7" width="17.1081081081081" style="1" customWidth="1"/>
-    <col min="8" max="8" width="58.4414414414414" style="1" customWidth="1"/>
-    <col min="9" max="9" width="69.1081081081081" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.5585585585586" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.10810810810811" style="1"/>
+    <col min="1" max="1" width="10.1111111111111" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="12" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="1"/>
+    <col min="5" max="7" width="17.1111111111111" style="1" customWidth="1"/>
+    <col min="8" max="8" width="58.4444444444444" style="1" customWidth="1"/>
+    <col min="9" max="9" width="69.1111111111111" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.5555555555556" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.11111111111111" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -6656,7 +6656,7 @@
       <c r="H21" s="23"/>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" s="8" customFormat="1" ht="14.1" spans="1:11">
+    <row r="22" s="8" customFormat="1" ht="13.8" spans="1:11">
       <c r="A22" s="4">
         <v>44512</v>
       </c>
@@ -7491,19 +7491,19 @@
       <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.1081081081081" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="6" max="6" width="39.8918918918919" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="1" max="1" width="10.1111111111111" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="6" max="6" width="39.8888888888889" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8115,7 +8115,7 @@
       <c r="J29" s="24"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="30" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A30" s="11"/>
       <c r="B30" s="12">
         <v>340</v>
@@ -8130,7 +8130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="31" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A31" s="11"/>
       <c r="B31" s="12">
         <v>356</v>
@@ -8145,7 +8145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="32" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A32" s="4">
         <v>43690</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="33" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A33" s="11"/>
       <c r="B33" s="12">
         <v>388</v>
@@ -8171,7 +8171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="34" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A34" s="4">
         <v>43689</v>
       </c>
@@ -8185,7 +8185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="35" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A35" s="4">
         <v>44463</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="36" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A36" s="11"/>
       <c r="B36" s="12">
         <v>424</v>
@@ -8211,7 +8211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="37" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A37" s="4">
         <v>43922</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="38" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A38" s="4">
         <v>43705</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A39" s="11"/>
       <c r="B39" s="12">
         <v>454</v>
@@ -8254,7 +8254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A40" s="11"/>
       <c r="B40" s="12">
         <v>470</v>
@@ -8266,7 +8266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A41" s="11"/>
       <c r="B41" s="12">
         <v>473</v>
@@ -8278,7 +8278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:6">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:6">
       <c r="A42" s="4">
         <v>44365</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:6">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:6">
       <c r="A43" s="4">
         <v>44371</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A44" s="11"/>
       <c r="B44" s="12">
         <v>523</v>
@@ -8324,7 +8324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A45" s="4">
         <v>43698</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="11"/>
       <c r="B46" s="12">
         <v>554</v>
@@ -8350,7 +8350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="11"/>
       <c r="B47" s="12">
         <v>560</v>
@@ -8362,7 +8362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="4">
         <v>43698</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A49" s="4">
         <v>43698</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A50" s="4">
         <v>43698</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A51" s="4">
         <v>43698</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A52" s="11"/>
       <c r="B52" s="12">
         <v>609</v>
@@ -8430,7 +8430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A53" s="11"/>
       <c r="B53" s="12">
         <v>721</v>
@@ -11059,21 +11059,21 @@
   <sheetPr/>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="$A13:$XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.10810810810811" style="2"/>
+    <col min="1" max="1" width="9.77777777777778" style="2"/>
     <col min="2" max="2" width="11.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5585585585586" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="1"/>
-    <col min="5" max="5" width="14.5585585585586" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5555555555556" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="1"/>
+    <col min="5" max="5" width="14.5555555555556" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5585585585586" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5585585585586" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.10810810810811" style="1"/>
+    <col min="7" max="7" width="46.5555555555556" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50.5555555555556" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.11111111111111" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -11157,7 +11157,9 @@
       <c r="H5" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="11"/>
+      <c r="A8" s="27">
+        <v>45138</v>
+      </c>
       <c r="B8" s="1">
         <v>108</v>
       </c>
@@ -11165,7 +11167,7 @@
         <v>488</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H8" s="30"/>
     </row>
@@ -11509,19 +11511,19 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.10810810810811" style="6"/>
-    <col min="2" max="2" width="14.8918918918919" style="25" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.11111111111111" style="6"/>
+    <col min="2" max="2" width="14.8888888888889" style="25" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -12520,83 +12522,83 @@
       <c r="J58" s="24"/>
       <c r="K58" s="19"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="60" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A60" s="11"/>
       <c r="B60" s="12"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="61" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="62" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="64" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="65" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="66" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="67" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="68" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A68" s="11"/>
       <c r="B68" s="12"/>
     </row>
-    <row r="69" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="69" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="70" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="71" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
     </row>
-    <row r="72" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="72" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A72" s="11"/>
       <c r="B72" s="12"/>
     </row>
-    <row r="73" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="73" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A73" s="11"/>
       <c r="B73" s="12"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="74" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A74" s="11"/>
       <c r="B74" s="12"/>
     </row>
-    <row r="75" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="75" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="76" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A76" s="11"/>
       <c r="B76" s="12"/>
     </row>
-    <row r="77" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="77" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A77" s="11"/>
       <c r="B77" s="12"/>
     </row>
-    <row r="78" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="78" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A78" s="11"/>
       <c r="B78" s="12"/>
     </row>
@@ -12669,15 +12671,15 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.44144144144144" style="59" customWidth="1"/>
-    <col min="2" max="2" width="9.10810810810811" style="60"/>
+    <col min="1" max="1" width="9.44444444444444" style="59" customWidth="1"/>
+    <col min="2" max="2" width="9.11111111111111" style="60"/>
     <col min="3" max="3" width="63" style="60" customWidth="1"/>
     <col min="4" max="5" width="13.6666666666667" style="60" customWidth="1"/>
     <col min="6" max="6" width="69.3333333333333" style="60" customWidth="1"/>
-    <col min="7" max="7" width="59.1081081081081" style="60" customWidth="1"/>
-    <col min="8" max="16384" width="9.10810810810811" style="60"/>
+    <col min="7" max="7" width="59.1111111111111" style="60" customWidth="1"/>
+    <col min="8" max="16384" width="9.11111111111111" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -12802,7 +12804,7 @@
       </c>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" s="58" customFormat="1" ht="25.7" spans="1:7">
+    <row r="7" s="58" customFormat="1" ht="26.4" spans="1:7">
       <c r="A7" s="63">
         <v>43669</v>
       </c>
@@ -12916,7 +12918,7 @@
       </c>
       <c r="G12" s="37"/>
     </row>
-    <row r="13" s="58" customFormat="1" ht="51.45" spans="1:7">
+    <row r="13" s="58" customFormat="1" ht="52.8" spans="1:7">
       <c r="A13" s="63">
         <v>43671</v>
       </c>
@@ -12937,7 +12939,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="14" s="58" customFormat="1" ht="25.3" spans="1:7">
+    <row r="14" s="58" customFormat="1" ht="25.2" spans="1:7">
       <c r="A14" s="66"/>
       <c r="B14" s="16">
         <v>393</v>
@@ -13022,7 +13024,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="19" s="58" customFormat="1" ht="64.3" spans="1:7">
+    <row r="19" s="58" customFormat="1" ht="66" spans="1:7">
       <c r="A19" s="16"/>
       <c r="B19" s="16">
         <v>462</v>
@@ -13079,7 +13081,7 @@
       </c>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" s="58" customFormat="1" spans="1:7">
+    <row r="22" s="58" customFormat="1" ht="25.2" spans="1:7">
       <c r="A22" s="63">
         <v>43672</v>
       </c>
@@ -13121,7 +13123,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="24" s="58" customFormat="1" ht="25.7" spans="1:7">
+    <row r="24" s="58" customFormat="1" ht="26.4" spans="1:7">
       <c r="A24" s="63">
         <v>43672</v>
       </c>
@@ -13751,17 +13753,17 @@
       <selection activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="12.6666666666667" style="42" customWidth="1"/>
     <col min="2" max="2" width="9" style="42"/>
-    <col min="3" max="3" width="61.1081081081081" style="42" customWidth="1"/>
+    <col min="3" max="3" width="61.1111111111111" style="42" customWidth="1"/>
     <col min="4" max="4" width="9" style="42"/>
-    <col min="5" max="5" width="14.8918918918919" style="42" customWidth="1"/>
-    <col min="6" max="6" width="20.4414414414414" style="43" customWidth="1"/>
+    <col min="5" max="5" width="14.8888888888889" style="42" customWidth="1"/>
+    <col min="6" max="6" width="20.4444444444444" style="43" customWidth="1"/>
     <col min="7" max="7" width="67.3333333333333" style="42" customWidth="1"/>
-    <col min="8" max="8" width="91.4414414414414" style="42" customWidth="1"/>
-    <col min="9" max="9" width="33.4414414414414" style="42" customWidth="1"/>
+    <col min="8" max="8" width="91.4444444444444" style="42" customWidth="1"/>
+    <col min="9" max="9" width="33.4444444444444" style="42" customWidth="1"/>
     <col min="10" max="11" width="9" style="42"/>
     <col min="12" max="16384" width="9" style="44"/>
   </cols>
@@ -13868,7 +13870,7 @@
       </c>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" ht="25.7" spans="1:9">
+    <row r="6" ht="26.4" spans="1:9">
       <c r="A6" s="26">
         <v>43675</v>
       </c>
@@ -20264,7 +20266,7 @@
       <c r="G171" s="46"/>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" s="8" customFormat="1" ht="14.1" spans="1:11">
+    <row r="172" s="8" customFormat="1" ht="13.8" spans="1:11">
       <c r="A172" s="4">
         <v>43969</v>
       </c>
@@ -25291,17 +25293,17 @@
       <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="10.3333333333333" style="1"/>
-    <col min="2" max="2" width="9.10810810810811" style="1"/>
-    <col min="3" max="3" width="50.4414414414414" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.11111111111111" style="1"/>
+    <col min="3" max="3" width="50.4444444444444" style="1" customWidth="1"/>
     <col min="4" max="5" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.4414414414414" style="1" customWidth="1"/>
-    <col min="7" max="7" width="76.1081081081081" style="34" customWidth="1"/>
-    <col min="8" max="8" width="62.8918918918919" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.4444444444444" style="1" customWidth="1"/>
+    <col min="7" max="7" width="76.1111111111111" style="34" customWidth="1"/>
+    <col min="8" max="8" width="62.8888888888889" style="1" customWidth="1"/>
     <col min="9" max="9" width="65" style="34" customWidth="1"/>
-    <col min="10" max="16384" width="9.10810810810811" style="1"/>
+    <col min="10" max="16384" width="9.11111111111111" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -28888,19 +28890,19 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.1081081081081" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.1111111111111" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="22.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -29622,7 +29624,7 @@
       <c r="J36" s="24"/>
       <c r="K36" s="19"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="37" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A37" s="4">
         <v>43886</v>
       </c>
@@ -29636,7 +29638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="38" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A38" s="11"/>
       <c r="B38" s="12">
         <v>1367</v>
@@ -29648,7 +29650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A39" s="4">
         <v>44524</v>
       </c>
@@ -29665,7 +29667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A40" s="11"/>
       <c r="B40" s="12">
         <v>1634</v>
@@ -29677,7 +29679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A41" s="4">
         <v>44529</v>
       </c>
@@ -29691,7 +29693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A42" s="4">
         <v>44536</v>
       </c>
@@ -29705,7 +29707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A43" s="11"/>
       <c r="B43" s="12">
         <v>1836</v>
@@ -29717,7 +29719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A44" s="4">
         <v>44529</v>
       </c>
@@ -29731,7 +29733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A45" s="11"/>
       <c r="B45" s="12">
         <v>2058</v>
@@ -29743,7 +29745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="11"/>
       <c r="B46" s="12">
         <v>2074</v>
@@ -29755,7 +29757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="4">
         <v>44570</v>
       </c>
@@ -29769,7 +29771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="4">
         <v>44612</v>
       </c>
@@ -29783,47 +29785,47 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
     </row>
@@ -31022,19 +31024,19 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.10810810810811" style="6"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.11111111111111" style="6"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -31459,87 +31461,87 @@
       <c r="J28" s="24"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="29" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="30" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="31" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="32" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="33" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A33" s="11"/>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="34" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="35" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A35" s="11"/>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="36" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="37" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A37" s="11"/>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="38" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A41" s="11"/>
       <c r="B41" s="12"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
     </row>
@@ -32611,19 +32613,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.89189189189189" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.88888888888889" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -33543,7 +33545,7 @@
       <c r="J49" s="24"/>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" ht="14.55" spans="1:11">
+    <row r="50" ht="14.4" spans="1:11">
       <c r="A50" s="11"/>
       <c r="B50"/>
       <c r="C50" s="14"/>
@@ -33555,87 +33557,87 @@
       <c r="J50" s="24"/>
       <c r="K50" s="19"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="60" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A60" s="11"/>
       <c r="B60" s="12"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="61" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="62" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="64" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="65" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="66" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="67" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A67" s="11"/>
       <c r="B67" s="12"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="68" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A68" s="11"/>
       <c r="B68" s="12"/>
     </row>
-    <row r="69" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="69" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A69" s="11"/>
       <c r="B69" s="12"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="70" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="71" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A71" s="11"/>
       <c r="B71" s="12"/>
     </row>
@@ -34708,22 +34710,22 @@
   <dimension ref="A1:AR126"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="16.8918918918919" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.8888888888889" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
     <col min="3" max="3" width="69.6666666666667" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.1081081081081" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.1111111111111" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -34799,7 +34801,7 @@
       <c r="J3" s="20"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A4" s="4">
         <v>44622</v>
       </c>
@@ -34814,7 +34816,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="5" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A5" s="4">
         <v>44622</v>
       </c>
@@ -34829,7 +34831,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="6" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A6" s="4">
         <v>44621</v>
       </c>
@@ -34868,7 +34870,7 @@
       </c>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="8" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A8" s="4">
         <v>44635</v>
       </c>
@@ -35507,7 +35509,7 @@
       <c r="J40" s="24"/>
       <c r="K40" s="19"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A41" s="11"/>
       <c r="B41" s="12">
         <v>655</v>
@@ -35519,7 +35521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A42" s="11"/>
       <c r="B42" s="12">
         <v>662</v>
@@ -35531,7 +35533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A43" s="11"/>
       <c r="B43" s="12">
         <v>663</v>
@@ -35546,7 +35548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A44" s="11"/>
       <c r="B44" s="12">
         <v>677</v>
@@ -35558,7 +35560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A45" s="11"/>
       <c r="B45" s="12">
         <v>684</v>
@@ -35570,7 +35572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="11"/>
       <c r="B46" s="12">
         <v>685</v>
@@ -35582,7 +35584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="4">
         <v>44635</v>
       </c>
@@ -35596,7 +35598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="11"/>
       <c r="B48" s="12">
         <v>699</v>
@@ -35608,7 +35610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A49" s="4">
         <v>43943</v>
       </c>
@@ -35622,7 +35624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A50" s="4">
         <v>44511</v>
       </c>
@@ -35636,7 +35638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A51" s="11"/>
       <c r="B51" s="12">
         <v>814</v>
@@ -35648,7 +35650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A52" s="11"/>
       <c r="B52" s="12">
         <v>850</v>
@@ -35660,7 +35662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A53" s="11"/>
       <c r="B53" s="12">
         <v>863</v>
@@ -35672,7 +35674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A54" s="11"/>
       <c r="B54" s="12">
         <v>866</v>
@@ -35684,7 +35686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A55" s="11"/>
       <c r="B55" s="12">
         <v>889</v>
@@ -35696,7 +35698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A56" s="11"/>
       <c r="B56" s="12">
         <v>897</v>
@@ -35708,7 +35710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A57" s="11"/>
       <c r="B57" s="12">
         <v>919</v>
@@ -35720,7 +35722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A58" s="4">
         <v>43915</v>
       </c>
@@ -35734,7 +35736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A59" s="11"/>
       <c r="B59" s="12">
         <v>951</v>
@@ -35746,7 +35748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="60" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A60" s="11"/>
       <c r="B60" s="12">
         <v>958</v>
@@ -35758,7 +35760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="61" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A61" s="4">
         <v>43917</v>
       </c>
@@ -35772,7 +35774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="62" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A62" s="11"/>
       <c r="B62" s="12">
         <v>971</v>
@@ -35784,7 +35786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A63" s="11"/>
       <c r="B63" s="12">
         <v>979</v>
@@ -35796,7 +35798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" s="17" customFormat="1" ht="12.85" spans="1:4">
+    <row r="64" s="17" customFormat="1" ht="13.2" spans="1:4">
       <c r="A64" s="5"/>
       <c r="B64" s="32">
         <v>987</v>
@@ -39311,20 +39313,20 @@
       <selection activeCell="A7" sqref="$A7:$XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="18.6666666666667" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="25" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
+    <col min="2" max="2" width="14.8888888888889" style="25" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
     <col min="5" max="5" width="11.6666666666667" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.5585585585586" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5555555555556" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="8" customWidth="1"/>
     <col min="8" max="8" width="10.6666666666667" style="8" customWidth="1"/>
     <col min="9" max="9" width="40.3333333333333" style="9" customWidth="1"/>
-    <col min="10" max="10" width="33.4414414414414" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="10" max="10" width="33.4444444444444" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -39400,7 +39402,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A4" s="4">
         <v>44567</v>
       </c>
@@ -39987,7 +39989,7 @@
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="34" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A34" s="4">
         <v>44384</v>
       </c>
@@ -40001,7 +40003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="35" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A35" s="11"/>
       <c r="B35" s="12">
         <v>802</v>
@@ -40013,7 +40015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="36" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A36" s="11"/>
       <c r="B36" s="12">
         <v>827</v>
@@ -40025,7 +40027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="37" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A37" s="11"/>
       <c r="B37" s="12">
         <v>834</v>
@@ -40037,7 +40039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="38" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A38" s="4">
         <v>44549</v>
       </c>
@@ -40051,7 +40053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A39" s="11"/>
       <c r="B39" s="12">
         <v>851</v>
@@ -40063,7 +40065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A40" s="11"/>
       <c r="B40" s="12">
         <v>913</v>
@@ -40075,7 +40077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A41" s="4">
         <v>43914</v>
       </c>
@@ -40089,7 +40091,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A42" s="11"/>
       <c r="B42" s="12">
         <v>1059</v>
@@ -40104,7 +40106,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A43" s="11"/>
       <c r="B43" s="12">
         <v>1192</v>
@@ -40116,7 +40118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A44" s="11"/>
       <c r="B44" s="12">
         <v>1202</v>
@@ -40128,7 +40130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A45" s="4">
         <v>43914</v>
       </c>
@@ -40145,7 +40147,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="11"/>
       <c r="B46" s="12">
         <v>1273</v>
@@ -40157,7 +40159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="4">
         <v>43942</v>
       </c>
@@ -40171,7 +40173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="11"/>
       <c r="B48" s="12">
         <v>1319</v>
@@ -40236,7 +40238,7 @@
       <c r="AQ49" s="1"/>
       <c r="AR49" s="1"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A50" s="11"/>
       <c r="B50" s="12">
         <v>1367</v>
@@ -40248,7 +40250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A51" s="11"/>
       <c r="B51" s="12">
         <v>1372</v>
@@ -40260,7 +40262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A52" s="11"/>
       <c r="B52" s="12">
         <v>1376</v>
@@ -40272,7 +40274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A53" s="11"/>
       <c r="B53" s="12">
         <v>1377</v>
@@ -40284,7 +40286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A54" s="4">
         <v>43913</v>
       </c>
@@ -40298,7 +40300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A55" s="4">
         <v>43939</v>
       </c>
@@ -40312,7 +40314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A56" s="4">
         <v>44573</v>
       </c>
@@ -40326,7 +40328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A57" s="4">
         <v>44580</v>
       </c>
@@ -40340,7 +40342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A58" s="4">
         <v>44545</v>
       </c>
@@ -40354,7 +40356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A63" s="4">
         <v>44460</v>
       </c>
@@ -40761,13 +40763,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.8918918918919" customWidth="1"/>
-    <col min="3" max="3" width="35.1081081081081" customWidth="1"/>
-    <col min="5" max="5" width="15.8918918918919" customWidth="1"/>
+    <col min="1" max="1" width="11.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="35.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="15.8888888888889" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="9" max="9" width="62" customWidth="1"/>
     <col min="10" max="10" width="64.3333333333333" customWidth="1"/>
   </cols>
@@ -41604,22 +41606,22 @@
   <sheetPr/>
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.4414414414414" style="28"/>
-    <col min="2" max="2" width="14.8918918918919" style="25" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="6" max="6" width="20.4414414414414" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.4414414414414" style="8" customWidth="1"/>
-    <col min="8" max="8" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.10810810810811" style="8"/>
+    <col min="1" max="1" width="11.4444444444444" style="28"/>
+    <col min="2" max="2" width="14.8888888888889" style="25" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="6" max="6" width="20.4444444444444" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.4444444444444" style="8" customWidth="1"/>
+    <col min="8" max="8" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -42015,7 +42017,7 @@
       <c r="H21" s="24"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" ht="25.7" spans="1:9">
+    <row r="22" ht="26.4" spans="1:9">
       <c r="A22" s="2"/>
       <c r="B22" s="12">
         <v>326</v>
@@ -42049,7 +42051,7 @@
       <c r="H23" s="24"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" ht="70.7" spans="1:9">
+    <row r="24" ht="69" spans="1:9">
       <c r="A24" s="4">
         <v>43921</v>
       </c>
@@ -42405,7 +42407,7 @@
       <c r="H44" s="24"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:7">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:7">
       <c r="A45" s="26">
         <v>43697</v>
       </c>
@@ -42422,7 +42424,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="4">
         <v>43950</v>
       </c>
@@ -42436,7 +42438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="4">
         <v>43943</v>
       </c>
@@ -42450,7 +42452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="4">
         <v>44370</v>
       </c>
@@ -42464,7 +42466,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A49" s="4">
         <v>43915</v>
       </c>
@@ -42478,7 +42480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A50" s="11"/>
       <c r="B50" s="12">
         <v>910</v>
@@ -42490,7 +42492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A51" s="4">
         <v>43921</v>
       </c>
@@ -42504,7 +42506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A52" s="4">
         <v>43682</v>
       </c>
@@ -42518,7 +42520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A53" s="4">
         <v>43691</v>
       </c>
@@ -42532,7 +42534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A54" s="4">
         <v>43927</v>
       </c>
@@ -42546,7 +42548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A55" s="4">
         <v>43700</v>
       </c>
@@ -42560,7 +42562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A56" s="5"/>
       <c r="B56" s="12">
         <v>1121</v>
@@ -42575,7 +42577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A57" s="4">
         <v>43700</v>
       </c>
@@ -42589,7 +42591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A58" s="11"/>
       <c r="B58" s="12">
         <v>1131</v>
@@ -42601,7 +42603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A59" s="4">
         <v>43700</v>
       </c>
@@ -42618,7 +42620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" s="1" customFormat="1" ht="12.85" spans="1:5">
+    <row r="60" s="1" customFormat="1" ht="13.2" spans="1:5">
       <c r="A60" s="4">
         <v>43700</v>
       </c>
@@ -42635,7 +42637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" s="1" customFormat="1" ht="12.85" spans="1:7">
+    <row r="61" s="1" customFormat="1" ht="13.2" spans="1:7">
       <c r="A61" s="4">
         <v>43700</v>
       </c>
@@ -42652,7 +42654,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="62" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A62" s="2"/>
       <c r="B62" s="12">
         <v>1157</v>
@@ -42664,7 +42666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A63" s="4">
         <v>43887</v>
       </c>
@@ -42678,11 +42680,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="64" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A64" s="2"/>
       <c r="B64" s="12"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="65" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A65" s="4">
         <v>44509</v>
       </c>
@@ -42696,7 +42698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="66" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A66" s="4">
         <v>43887</v>
       </c>
@@ -42713,7 +42715,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="67" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A67" s="4">
         <v>43915</v>
       </c>
@@ -42727,7 +42729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="68" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A68" s="4">
         <v>43914</v>
       </c>
@@ -42741,7 +42743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="69" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A69" s="4">
         <v>44368</v>
       </c>
@@ -42755,7 +42757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="70" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A70" s="4">
         <v>43882</v>
       </c>
@@ -42769,7 +42771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="71" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A71" s="2"/>
       <c r="B71" s="12">
         <v>1360</v>
@@ -42781,11 +42783,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="72" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A72" s="2"/>
       <c r="B72" s="12"/>
     </row>
-    <row r="73" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="73" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A73" s="4">
         <v>43911</v>
       </c>
@@ -42799,7 +42801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="74" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A74" s="4">
         <v>43953</v>
       </c>
@@ -42816,7 +42818,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="75" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A75" s="4">
         <v>43969</v>
       </c>
@@ -42830,7 +42832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="76" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A76" s="5"/>
       <c r="B76" s="12">
         <v>1447</v>
@@ -42842,7 +42844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" s="1" customFormat="1" ht="12.85" spans="1:6">
+    <row r="77" s="1" customFormat="1" ht="13.2" spans="1:6">
       <c r="A77" s="4">
         <v>44361</v>
       </c>
@@ -42859,7 +42861,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="78" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A78" s="5"/>
       <c r="B78" s="12">
         <v>1492</v>
@@ -42871,7 +42873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="79" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A79" s="5"/>
       <c r="B79" s="12">
         <v>1497</v>
@@ -42883,7 +42885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="80" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A80" s="4">
         <v>44099</v>
       </c>
@@ -42897,7 +42899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="81" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A81" s="11"/>
       <c r="B81" s="12">
         <v>1513</v>
@@ -42909,7 +42911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="82" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A82" s="11"/>
       <c r="B82" s="12">
         <v>1525</v>
@@ -42921,7 +42923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="83" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A83" s="11"/>
       <c r="B83" s="12">
         <v>1537</v>
@@ -42933,7 +42935,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" s="1" customFormat="1" ht="12.85" spans="1:6">
+    <row r="84" s="1" customFormat="1" ht="13.2" spans="1:6">
       <c r="A84" s="4">
         <v>44377</v>
       </c>
@@ -42950,7 +42952,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="85" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A85" s="4">
         <v>44178</v>
       </c>
@@ -42964,7 +42966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="86" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A86" s="4">
         <v>44327</v>
       </c>
@@ -42978,7 +42980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="87" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A87" s="4">
         <v>44329</v>
       </c>
@@ -42992,31 +42994,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="88" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A88" s="11"/>
       <c r="B88" s="12"/>
     </row>
-    <row r="90" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="90" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A90" s="11"/>
       <c r="B90" s="12"/>
     </row>
-    <row r="91" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="91" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A91" s="11"/>
       <c r="B91" s="12"/>
     </row>
-    <row r="92" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="92" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A92" s="11"/>
       <c r="B92" s="12"/>
     </row>
-    <row r="93" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="93" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
     </row>
-    <row r="94" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="94" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A94" s="11"/>
       <c r="B94" s="12"/>
     </row>
-    <row r="95" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="95" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A95" s="4">
         <v>44349</v>
       </c>
@@ -43030,7 +43032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="96" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A96" s="4">
         <v>44327</v>
       </c>
@@ -43044,7 +43046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="97" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A97" s="4">
         <v>44326</v>
       </c>
@@ -43058,23 +43060,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="98" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A98" s="11"/>
       <c r="B98" s="12"/>
     </row>
-    <row r="99" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="99" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A99" s="11"/>
       <c r="B99" s="12"/>
     </row>
-    <row r="100" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="100" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A100" s="11"/>
       <c r="B100" s="12"/>
     </row>
-    <row r="101" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="101" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A101" s="11"/>
       <c r="B101" s="12"/>
     </row>
-    <row r="102" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="102" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A102" s="4">
         <v>44427</v>
       </c>
@@ -43088,7 +43090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="103" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A103" s="4">
         <v>44447</v>
       </c>
@@ -43102,7 +43104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="104" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A104" s="4">
         <v>44556</v>
       </c>
@@ -43116,7 +43118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="105" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A105" s="4">
         <v>44556</v>
       </c>
@@ -43130,7 +43132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="106" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A106" s="4">
         <v>44579</v>
       </c>
@@ -43144,7 +43146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="107" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A107" s="4">
         <v>44605</v>
       </c>
@@ -43158,7 +43160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="108" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A108" s="4">
         <v>44611</v>
       </c>
@@ -43172,7 +43174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" s="1" customFormat="1" ht="12.85" spans="1:7">
+    <row r="109" s="1" customFormat="1" ht="13.2" spans="1:7">
       <c r="A109" s="4">
         <v>44611</v>
       </c>
@@ -43189,7 +43191,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="110" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A110" s="4">
         <v>44699</v>
       </c>
@@ -43203,7 +43205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="111" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A111" s="4">
         <v>45137</v>
       </c>
@@ -43217,7 +43219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="112" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A112" s="4">
         <v>45131</v>
       </c>
@@ -43231,7 +43233,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="113" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A113" s="27">
         <v>45133</v>
       </c>
@@ -43245,19 +43247,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="114" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A114" s="11"/>
       <c r="B114" s="12"/>
     </row>
-    <row r="115" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="115" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A115" s="11"/>
       <c r="B115" s="12"/>
     </row>
-    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="116" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A116" s="11"/>
       <c r="B116" s="12"/>
     </row>
-    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="117" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A117" s="11"/>
       <c r="B117" s="12"/>
     </row>
@@ -43516,13 +43518,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="36.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="9.10810810810811" customWidth="1"/>
+    <col min="5" max="5" width="9.11111111111111" customWidth="1"/>
     <col min="9" max="9" width="29.3333333333333" customWidth="1"/>
     <col min="10" max="10" width="36.6666666666667" customWidth="1"/>
-    <col min="11" max="11" width="54.1081081081081" customWidth="1"/>
+    <col min="11" max="11" width="54.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -43739,20 +43741,20 @@
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.10810810810811" style="6"/>
-    <col min="2" max="2" width="14.8918918918919" style="25" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.11111111111111" style="6"/>
+    <col min="2" max="2" width="14.8888888888889" style="25" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
     <col min="7" max="7" width="24.3333333333333" style="8" customWidth="1"/>
-    <col min="8" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="8" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44576,11 +44578,11 @@
       <c r="J44" s="24"/>
       <c r="K44" s="19"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A46" s="4">
         <v>44341</v>
       </c>
@@ -44594,7 +44596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A47" s="4">
         <v>44376</v>
       </c>
@@ -44608,7 +44610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A48" s="4">
         <v>44375</v>
       </c>
@@ -44622,7 +44624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:10">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:10">
       <c r="A49" s="26">
         <v>44608</v>
       </c>
@@ -44639,7 +44641,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A50" s="27">
         <v>45135</v>
       </c>
@@ -44653,59 +44655,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="60" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A60" s="11"/>
       <c r="B60" s="12"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="61" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A61" s="11"/>
       <c r="B61" s="12"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="62" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A62" s="11"/>
       <c r="B62" s="12"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="63" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A63" s="11"/>
       <c r="B63" s="12"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="64" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
     </row>
@@ -44785,19 +44787,19 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.89189189189189" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.88888888888889" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44857,7 +44859,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="12.85" spans="1:10">
+    <row r="3" s="1" customFormat="1" ht="13.2" spans="1:10">
       <c r="A3" s="13">
         <v>44357</v>
       </c>
@@ -44877,7 +44879,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:6">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:6">
       <c r="A4" s="13">
         <v>44370</v>
       </c>
@@ -44894,7 +44896,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="5" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A5" s="13">
         <v>44532</v>
       </c>
@@ -44908,7 +44910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="6" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A6" s="13">
         <v>44514</v>
       </c>
@@ -44922,7 +44924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="12.85" spans="1:4">
+    <row r="7" s="1" customFormat="1" ht="13.2" spans="1:4">
       <c r="A7" s="13">
         <v>44514</v>
       </c>
@@ -45393,87 +45395,87 @@
       <c r="J38" s="24"/>
       <c r="K38" s="19"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A41" s="11"/>
       <c r="B41" s="12"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="59" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
     </row>
@@ -46566,19 +46568,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="18.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="14.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="56.3333333333333" customWidth="1"/>
     <col min="5" max="5" width="12.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="29.5585585585586" customWidth="1"/>
+    <col min="7" max="7" width="29.5555555555556" customWidth="1"/>
     <col min="8" max="8" width="50" customWidth="1"/>
-    <col min="9" max="9" width="9.10810810810811" customWidth="1"/>
+    <col min="9" max="9" width="9.11111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="1" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -46604,7 +46606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A2" s="4">
         <v>44558</v>
       </c>
@@ -46619,7 +46621,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="3" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A3" s="4">
         <v>44558</v>
       </c>
@@ -46634,7 +46636,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A4" s="4">
         <v>44559</v>
       </c>
@@ -46649,7 +46651,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="5" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A5" s="4">
         <v>44610</v>
       </c>
@@ -46666,7 +46668,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="6" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A6" s="4">
         <v>44557</v>
       </c>
@@ -46681,7 +46683,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="7" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A7" s="4">
         <v>44560</v>
       </c>
@@ -46696,7 +46698,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="8" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A8" s="4">
         <v>44557</v>
       </c>
@@ -46711,7 +46713,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="9" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A9" s="4">
         <v>44579</v>
       </c>
@@ -46726,7 +46728,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="10" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A10" s="4">
         <v>44558</v>
       </c>
@@ -46741,7 +46743,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="11" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A11" s="4">
         <v>44343</v>
       </c>
@@ -46756,7 +46758,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="12" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A12" s="4">
         <v>44560</v>
       </c>
@@ -46771,7 +46773,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="13" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A13" s="4">
         <v>44559</v>
       </c>
@@ -46786,7 +46788,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="14" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A14" s="5"/>
       <c r="B14" s="1">
         <v>1524</v>
@@ -46799,7 +46801,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="15" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A15" s="5"/>
       <c r="B15" s="1">
         <v>1542</v>
@@ -46809,7 +46811,7 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="16" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A16" s="4">
         <v>44559</v>
       </c>
@@ -46824,7 +46826,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="17" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A17" s="5"/>
       <c r="B17" s="1">
         <v>1658</v>
@@ -46837,7 +46839,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="18" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A18" s="5"/>
       <c r="B18" s="1">
         <v>1788</v>
@@ -46850,7 +46852,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="19" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A19" s="5"/>
       <c r="B19" s="1">
         <v>1915</v>
@@ -46863,7 +46865,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="20" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A20" s="4">
         <v>44610</v>
       </c>
@@ -46878,7 +46880,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="21" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A21" s="4">
         <v>44579</v>
       </c>
@@ -46893,7 +46895,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="22" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A22" s="5"/>
       <c r="B22" s="1">
         <v>2025</v>
@@ -46906,7 +46908,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="23" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A23" s="4">
         <v>44609</v>
       </c>
@@ -47264,18 +47266,18 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.1081081081081" customWidth="1"/>
+    <col min="1" max="1" width="10.1111111111111" customWidth="1"/>
     <col min="2" max="2" width="14.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="55.1081081081081" customWidth="1"/>
-    <col min="5" max="5" width="15.1081081081081" customWidth="1"/>
-    <col min="6" max="6" width="22.4414414414414" customWidth="1"/>
-    <col min="7" max="7" width="64.4414414414414" customWidth="1"/>
+    <col min="3" max="3" width="55.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="15.1111111111111" customWidth="1"/>
+    <col min="6" max="6" width="22.4444444444444" customWidth="1"/>
+    <col min="7" max="7" width="64.4444444444444" customWidth="1"/>
     <col min="8" max="8" width="69.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="1" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -47302,7 +47304,7 @@
       </c>
       <c r="I1" s="34"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="2" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A2" s="26">
         <v>44550</v>
       </c>
@@ -47319,7 +47321,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="34"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="3" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A3" s="26">
         <v>44550</v>
       </c>
@@ -47336,7 +47338,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="34"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A4" s="3"/>
       <c r="B4" s="1">
         <v>37</v>
@@ -47351,7 +47353,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="34"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="5" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A5" s="26">
         <v>44356</v>
       </c>
@@ -47368,7 +47370,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="6" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A6" s="26">
         <v>44356</v>
       </c>
@@ -47385,7 +47387,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="7" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A7" s="26">
         <v>43778</v>
       </c>
@@ -47404,7 +47406,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="12.85" spans="1:9">
+    <row r="8" s="1" customFormat="1" ht="13.2" spans="1:9">
       <c r="A8" s="26">
         <v>44355</v>
       </c>
@@ -47421,7 +47423,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" s="43" customFormat="1" ht="12.85" spans="1:9">
+    <row r="9" s="43" customFormat="1" ht="13.2" spans="1:9">
       <c r="A9" s="3"/>
       <c r="B9" s="1">
         <v>51</v>
@@ -47438,7 +47440,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="90"/>
     </row>
-    <row r="10" s="43" customFormat="1" ht="12.85" spans="1:9">
+    <row r="10" s="43" customFormat="1" ht="13.2" spans="1:9">
       <c r="A10" s="3"/>
       <c r="B10" s="1">
         <v>52</v>
@@ -48354,17 +48356,17 @@
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.10810810810811" style="2"/>
+    <col min="1" max="1" width="9.11111111111111" style="2"/>
     <col min="2" max="2" width="11.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5585585585586" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="1"/>
-    <col min="5" max="5" width="14.5585585585586" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.8918918918919" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5585585585586" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5585585585586" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.10810810810811" style="1"/>
+    <col min="3" max="3" width="51.5555555555556" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="1"/>
+    <col min="5" max="5" width="14.5555555555556" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.8888888888889" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46.5555555555556" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50.5555555555556" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.11111111111111" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -49000,16 +49002,16 @@
       <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="10.3333333333333" style="2"/>
     <col min="2" max="2" width="11.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="71.5585585585586" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="1"/>
-    <col min="5" max="7" width="14.5585585585586" style="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5585585585586" style="1" customWidth="1"/>
-    <col min="9" max="9" width="50.5585585585586" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.10810810810811" style="1"/>
+    <col min="3" max="3" width="71.5555555555556" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="1"/>
+    <col min="5" max="7" width="14.5555555555556" style="1" customWidth="1"/>
+    <col min="8" max="8" width="46.5555555555556" style="1" customWidth="1"/>
+    <col min="9" max="9" width="50.5555555555556" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.11111111111111" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -50043,17 +50045,17 @@
       <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="3" max="3" width="44.5585585585586" customWidth="1"/>
-    <col min="4" max="4" width="15.4414414414414" customWidth="1"/>
+    <col min="3" max="3" width="44.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="15.4444444444444" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="30.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="1" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -50079,7 +50081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A2" s="4">
         <v>44544</v>
       </c>
@@ -50149,16 +50151,16 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="3" max="3" width="50.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="16.8918918918919" customWidth="1"/>
-    <col min="5" max="5" width="15.5585585585586" customWidth="1"/>
-    <col min="7" max="7" width="30.4414414414414" customWidth="1"/>
-    <col min="8" max="8" width="29.1081081081081" customWidth="1"/>
+    <col min="4" max="4" width="16.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="15.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="30.4444444444444" customWidth="1"/>
+    <col min="8" max="8" width="29.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="1" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -50184,7 +50186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="12.85" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="13.2" spans="1:8">
       <c r="A2" s="4">
         <v>44544</v>
       </c>
@@ -50254,19 +50256,19 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.89189189189189" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="8"/>
-    <col min="5" max="5" width="17.1081081081081" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.88888888888889" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="8"/>
+    <col min="5" max="5" width="17.1111111111111" style="8" customWidth="1"/>
     <col min="6" max="6" width="18.3333333333333" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="8" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="9" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="8" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="8"/>
+    <col min="7" max="8" width="17.1111111111111" style="8" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="9" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="8" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50346,7 +50348,7 @@
       </c>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="12.85" spans="1:10">
+    <row r="4" s="1" customFormat="1" ht="13.2" spans="1:10">
       <c r="A4" s="13">
         <v>44374</v>
       </c>
@@ -50366,7 +50368,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="12.85" spans="1:10">
+    <row r="5" s="1" customFormat="1" ht="13.2" spans="1:10">
       <c r="A5" s="13">
         <v>44610</v>
       </c>
@@ -50776,87 +50778,87 @@
       <c r="J37" s="24"/>
       <c r="K37" s="19"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="38" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="39" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="40" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="41" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A41" s="11"/>
       <c r="B41" s="12"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="42" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="43" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="44" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="45" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="46" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="47" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="48" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="49" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="50" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="51" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A51" s="11"/>
       <c r="B51" s="12"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="52" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A52" s="11"/>
       <c r="B52" s="12"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="53" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A53" s="11"/>
       <c r="B53" s="12"/>
     </row>
-    <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="54" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="55" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A55" s="11"/>
       <c r="B55" s="12"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="56" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="57" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A57" s="11"/>
       <c r="B57" s="12"/>
     </row>
-    <row r="58" s="1" customFormat="1" ht="12.85" spans="1:2">
+    <row r="58" s="1" customFormat="1" ht="13.2" spans="1:2">
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
     </row>
@@ -51949,19 +51951,19 @@
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.1081081081081" style="83" customWidth="1"/>
-    <col min="2" max="2" width="14.8918918918919" style="84" customWidth="1"/>
-    <col min="3" max="3" width="57.8918918918919" style="85" customWidth="1"/>
-    <col min="4" max="4" width="9.10810810810811" style="85"/>
-    <col min="5" max="5" width="17.1081081081081" style="85" customWidth="1"/>
-    <col min="6" max="6" width="15.5585585585586" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.1081081081081" style="85" customWidth="1"/>
-    <col min="9" max="9" width="58.4414414414414" style="85" customWidth="1"/>
-    <col min="10" max="10" width="69.1081081081081" style="85" customWidth="1"/>
-    <col min="11" max="11" width="43.5585585585586" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.10810810810811" style="85"/>
+    <col min="1" max="1" width="10.1111111111111" style="83" customWidth="1"/>
+    <col min="2" max="2" width="14.8888888888889" style="84" customWidth="1"/>
+    <col min="3" max="3" width="57.8888888888889" style="85" customWidth="1"/>
+    <col min="4" max="4" width="9.11111111111111" style="85"/>
+    <col min="5" max="5" width="17.1111111111111" style="85" customWidth="1"/>
+    <col min="6" max="6" width="15.5555555555556" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.1111111111111" style="85" customWidth="1"/>
+    <col min="9" max="9" width="58.4444444444444" style="85" customWidth="1"/>
+    <col min="10" max="10" width="69.1111111111111" style="85" customWidth="1"/>
+    <col min="11" max="11" width="43.5555555555556" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.11111111111111" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
Solved problem 2469 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="3" activeTab="9"/>
+    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="3" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3363" uniqueCount="1552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="1553">
   <si>
     <t>Date</t>
   </si>
@@ -4627,6 +4627,9 @@
   </si>
   <si>
     <t>Largest Number After Digit Swaps by Parity</t>
+  </si>
+  <si>
+    <t>Convert the Temperature</t>
   </si>
   <si>
     <t>Pass the Pillow</t>
@@ -7493,7 +7496,7 @@
   <sheetPr/>
   <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
@@ -41677,9 +41680,9 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
@@ -43280,10 +43283,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A111" s="4">
-        <v>45137</v>
+        <v>45141</v>
       </c>
       <c r="B111" s="12">
-        <v>2582</v>
+        <v>2469</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>1475</v>
@@ -43294,10 +43297,10 @@
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A112" s="4">
-        <v>45131</v>
+        <v>45137</v>
       </c>
       <c r="B112" s="12">
-        <v>2739</v>
+        <v>2582</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1476</v>
@@ -43307,11 +43310,11 @@
       </c>
     </row>
     <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A113" s="27">
-        <v>45133</v>
+      <c r="A113" s="4">
+        <v>45131</v>
       </c>
       <c r="B113" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1477</v>
@@ -43320,9 +43323,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A114" s="11"/>
-      <c r="B114" s="12"/>
+    <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A114" s="27">
+        <v>45133</v>
+      </c>
+      <c r="B114" s="12">
+        <v>2745</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A115" s="11"/>
@@ -43335,6 +43348,10 @@
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A117" s="11"/>
       <c r="B117" s="12"/>
+    </row>
+    <row r="118" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A118" s="11"/>
+      <c r="B118" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -43432,7 +43449,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F117">
+  <conditionalFormatting sqref="F107:F118">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -43471,7 +43488,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G118:XFD1048576 A118:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A119:E1048576 G119:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -43493,7 +43510,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F118:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F119:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -43554,7 +43571,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD117 A107:E117">
+  <conditionalFormatting sqref="G107:XFD118 A107:E118">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -43641,7 +43658,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43873,7 +43890,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43890,7 +43907,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43909,7 +43926,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43928,7 +43945,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43948,7 +43965,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43968,7 +43985,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -43989,7 +44006,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44009,7 +44026,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44019,10 +44036,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -44054,7 +44071,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -44074,7 +44091,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44094,7 +44111,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44117,7 +44134,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44137,7 +44154,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44157,19 +44174,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44183,7 +44200,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44201,7 +44218,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44221,7 +44238,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44230,7 +44247,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44244,7 +44261,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44264,7 +44281,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44282,7 +44299,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44302,7 +44319,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44311,10 +44328,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44326,7 +44343,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44346,7 +44363,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44364,7 +44381,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44447,7 +44464,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44467,7 +44484,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44487,7 +44504,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44497,7 +44514,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44509,7 +44526,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44529,7 +44546,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44663,7 +44680,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44677,7 +44694,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44691,7 +44708,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44705,13 +44722,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44722,7 +44739,7 @@
         <v>2740</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44940,13 +44957,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44960,13 +44977,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44977,7 +44994,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -44991,7 +45008,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45005,7 +45022,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45019,7 +45036,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45051,7 +45068,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45102,7 +45119,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45123,14 +45140,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45146,7 +45163,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45181,7 +45198,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45190,7 +45207,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45227,7 +45244,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45248,7 +45265,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45258,7 +45275,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46732,13 +46749,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46779,7 +46796,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46794,7 +46811,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46854,7 +46871,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46867,7 +46884,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46892,7 +46909,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46905,7 +46922,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46918,7 +46935,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46931,7 +46948,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46946,7 +46963,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46961,7 +46978,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46974,7 +46991,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -46989,7 +47006,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2475 Category: Array Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="1553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3367" uniqueCount="1554">
   <si>
     <t>Date</t>
   </si>
@@ -4630,6 +4630,9 @@
   </si>
   <si>
     <t>Convert the Temperature</t>
+  </si>
+  <si>
+    <t>Number of Uneual Triplets in Array</t>
   </si>
   <si>
     <t>Pass the Pillow</t>
@@ -41680,10 +41683,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -43297,10 +43300,10 @@
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A112" s="4">
-        <v>45137</v>
+        <v>45141</v>
       </c>
       <c r="B112" s="12">
-        <v>2582</v>
+        <v>2475</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1476</v>
@@ -43311,10 +43314,10 @@
     </row>
     <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A113" s="4">
-        <v>45131</v>
+        <v>45137</v>
       </c>
       <c r="B113" s="12">
-        <v>2739</v>
+        <v>2582</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1477</v>
@@ -43324,11 +43327,11 @@
       </c>
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A114" s="27">
-        <v>45133</v>
+      <c r="A114" s="4">
+        <v>45131</v>
       </c>
       <c r="B114" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1478</v>
@@ -43337,9 +43340,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A115" s="11"/>
-      <c r="B115" s="12"/>
+    <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A115" s="27">
+        <v>45133</v>
+      </c>
+      <c r="B115" s="12">
+        <v>2745</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A116" s="11"/>
@@ -43352,6 +43365,10 @@
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A118" s="11"/>
       <c r="B118" s="12"/>
+    </row>
+    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A119" s="11"/>
+      <c r="B119" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -43449,7 +43466,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F118">
+  <conditionalFormatting sqref="F107:F119">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -43488,7 +43505,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A119:E1048576 G119:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G120:XFD1048576 A120:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -43510,7 +43527,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F119:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F120:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -43571,7 +43588,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD118 A107:E118">
+  <conditionalFormatting sqref="G107:XFD119 A107:E119">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -43658,7 +43675,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43890,7 +43907,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43907,7 +43924,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43926,7 +43943,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43945,7 +43962,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43965,7 +43982,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -43985,7 +44002,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44006,7 +44023,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44026,7 +44043,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44036,10 +44053,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -44071,7 +44088,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -44091,7 +44108,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44111,7 +44128,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44134,7 +44151,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44154,7 +44171,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44174,19 +44191,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44200,7 +44217,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44218,7 +44235,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44238,7 +44255,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44247,7 +44264,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44261,7 +44278,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44281,7 +44298,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44299,7 +44316,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44319,7 +44336,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44328,10 +44345,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44343,7 +44360,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44363,7 +44380,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44381,7 +44398,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44464,7 +44481,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44484,7 +44501,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44504,7 +44521,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44514,7 +44531,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44526,7 +44543,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44546,7 +44563,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44680,7 +44697,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44694,7 +44711,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44708,7 +44725,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44722,13 +44739,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44739,7 +44756,7 @@
         <v>2740</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44957,13 +44974,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44977,13 +44994,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44994,7 +45011,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45008,7 +45025,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45022,7 +45039,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45036,7 +45053,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45068,7 +45085,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45119,7 +45136,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45140,14 +45157,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45163,7 +45180,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45198,7 +45215,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45207,7 +45224,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45244,7 +45261,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45265,7 +45282,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45275,7 +45292,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46749,13 +46766,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46796,7 +46813,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46811,7 +46828,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46871,7 +46888,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46884,7 +46901,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46909,7 +46926,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46922,7 +46939,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46935,7 +46952,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46948,7 +46965,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46963,7 +46980,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46978,7 +46995,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -46991,7 +47008,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47006,7 +47023,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2769 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="3" activeTab="20"/>
+    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3367" uniqueCount="1554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="1555">
   <si>
     <t>Date</t>
   </si>
@@ -4642,6 +4642,9 @@
   </si>
   <si>
     <t>Construct the Longest New String</t>
+  </si>
+  <si>
+    <t>Find the Maximum Achievable Number</t>
   </si>
   <si>
     <t>Print in Order</t>
@@ -41686,7 +41689,7 @@
   <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -43354,9 +43357,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A116" s="11"/>
-      <c r="B116" s="12"/>
+    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A116" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B116" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A117" s="11"/>
@@ -43675,7 +43688,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43907,7 +43920,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43924,7 +43937,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43943,7 +43956,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43962,7 +43975,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43982,7 +43995,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44002,7 +44015,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44023,7 +44036,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44043,7 +44056,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44053,10 +44066,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -44088,7 +44101,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -44108,7 +44121,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44128,7 +44141,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44151,7 +44164,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44171,7 +44184,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44191,19 +44204,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44217,7 +44230,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44235,7 +44248,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44255,7 +44268,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44264,7 +44277,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44278,7 +44291,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44298,7 +44311,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44316,7 +44329,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44336,7 +44349,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44345,10 +44358,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44360,7 +44373,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44380,7 +44393,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44398,7 +44411,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44481,7 +44494,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44501,7 +44514,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44521,7 +44534,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44531,7 +44544,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44543,7 +44556,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44563,7 +44576,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44697,7 +44710,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44711,7 +44724,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44725,7 +44738,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44739,13 +44752,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44756,7 +44769,7 @@
         <v>2740</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44974,13 +44987,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -44994,13 +45007,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45011,7 +45024,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45025,7 +45038,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45039,7 +45052,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45053,7 +45066,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45085,7 +45098,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45136,7 +45149,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45157,14 +45170,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45180,7 +45193,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45215,7 +45228,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45224,7 +45237,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45261,7 +45274,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45282,7 +45295,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45292,7 +45305,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46766,13 +46779,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46813,7 +46826,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46828,7 +46841,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46888,7 +46901,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46901,7 +46914,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46926,7 +46939,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46939,7 +46952,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46952,7 +46965,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46965,7 +46978,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46980,7 +46993,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -46995,7 +47008,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47008,7 +47021,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47023,7 +47036,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2733 Category: Sort Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="20"/>
+    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="1555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="1556">
   <si>
     <t>Date</t>
   </si>
@@ -4771,6 +4771,9 @@
   </si>
   <si>
     <t>to_string</t>
+  </si>
+  <si>
+    <t>Neither Minimum nor Maximum</t>
   </si>
   <si>
     <t>Find the Value of the Partition</t>
@@ -41688,7 +41691,7 @@
   <sheetPr/>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
@@ -43855,9 +43858,9 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -44762,22 +44765,32 @@
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A50" s="27">
-        <v>45135</v>
+      <c r="A50" s="26">
+        <v>45143</v>
       </c>
       <c r="B50" s="12">
-        <v>2740</v>
+        <v>2733</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1523</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A51" s="27">
+        <v>45135</v>
+      </c>
+      <c r="B51" s="12">
+        <v>2740</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A52" s="11"/>
@@ -44831,40 +44844,44 @@
       <c r="A64" s="11"/>
       <c r="B64" s="12"/>
     </row>
+    <row r="65" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A65" s="11"/>
+      <c r="B65" s="12"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="F$1:F$1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60:F62">
+  <conditionalFormatting sqref="F61:F63">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G$1:XFD$1048576 A50:E1048576 B49:E49 A1:E48">
+  <conditionalFormatting sqref="G$1:XFD$1048576 A1:E48 B49:E50 A51:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44987,13 +45004,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45007,13 +45024,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45024,7 +45041,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45038,7 +45055,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45052,7 +45069,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45066,7 +45083,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45098,7 +45115,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45149,7 +45166,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45170,14 +45187,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45193,7 +45210,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45228,7 +45245,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45237,7 +45254,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45274,7 +45291,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45295,7 +45312,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45305,7 +45322,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46779,13 +46796,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46826,7 +46843,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46901,7 +46918,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46914,7 +46931,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46939,7 +46956,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46952,7 +46969,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46965,7 +46982,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46978,7 +46995,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -46993,7 +47010,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47008,7 +47025,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47021,7 +47038,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47036,7 +47053,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2810 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="22"/>
+    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="1557">
   <si>
     <t>Date</t>
   </si>
@@ -3642,6 +3642,9 @@
   </si>
   <si>
     <t>Split Strings by Separator</t>
+  </si>
+  <si>
+    <t>Faulty Keyboard</t>
   </si>
   <si>
     <t>Add Two Numbers</t>
@@ -25360,8 +25363,8 @@
   <sheetPr/>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -28193,8 +28196,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
-      <c r="A213" s="36"/>
+    <row r="213" spans="1:4">
+      <c r="A213" s="39">
+        <v>45144</v>
+      </c>
+      <c r="B213" s="1">
+        <v>2810</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A5:I62">
@@ -29033,7 +29047,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -29056,7 +29070,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -29076,7 +29090,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -29096,7 +29110,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -29116,7 +29130,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -29134,7 +29148,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -29152,7 +29166,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -29170,7 +29184,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -29190,7 +29204,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -29208,7 +29222,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -29226,7 +29240,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -29244,7 +29258,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -29262,7 +29276,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -29336,7 +29350,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -29354,7 +29368,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -29374,7 +29388,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -29386,7 +29400,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -29399,7 +29413,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -29419,7 +29433,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -29442,7 +29456,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -29463,7 +29477,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -29484,7 +29498,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -29504,7 +29518,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -29522,7 +29536,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -29540,7 +29554,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -29558,7 +29572,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -29576,7 +29590,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -29612,7 +29626,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -29632,7 +29646,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -29641,7 +29655,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -29652,7 +29666,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -29670,7 +29684,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -29692,7 +29706,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -29701,7 +29715,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -29717,7 +29731,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -29743,7 +29757,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -29758,7 +29772,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -29772,7 +29786,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -29786,7 +29800,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -29798,7 +29812,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -29812,7 +29826,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -29824,7 +29838,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -29836,7 +29850,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -29850,7 +29864,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -29864,7 +29878,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -31165,7 +31179,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -31183,7 +31197,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -31205,7 +31219,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -31225,7 +31239,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31245,7 +31259,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31263,7 +31277,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -31281,7 +31295,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -31299,7 +31313,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -31315,7 +31329,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32756,7 +32770,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -32777,7 +32791,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -32795,7 +32809,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -32813,7 +32827,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32831,7 +32845,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -32852,7 +32866,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -32863,7 +32877,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -32873,7 +32887,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -32894,7 +32908,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -32912,7 +32926,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32930,7 +32944,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -32948,7 +32962,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -32966,7 +32980,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -32984,7 +32998,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -33004,7 +33018,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -33025,7 +33039,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -33044,7 +33058,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -33065,7 +33079,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -33085,7 +33099,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -33103,7 +33117,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -33123,7 +33137,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -33143,7 +33157,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -33193,7 +33207,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -33213,7 +33227,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -33231,7 +33245,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -33249,7 +33263,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -33267,7 +33281,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -33287,7 +33301,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -33305,7 +33319,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -33323,7 +33337,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -33341,7 +33355,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -33359,7 +33373,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -33377,7 +33391,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -33395,7 +33409,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -33413,7 +33427,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -33433,7 +33447,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -33451,7 +33465,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -33469,7 +33483,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -33487,7 +33501,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -33507,7 +33521,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -33527,7 +33541,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -33548,7 +33562,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -33568,7 +33582,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -33586,7 +33600,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -33606,7 +33620,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -34856,7 +34870,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -34874,7 +34888,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34894,7 +34908,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -34909,7 +34923,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -34924,7 +34938,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -34939,7 +34953,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -34948,10 +34962,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34963,14 +34977,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -34981,7 +34995,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -35001,7 +35015,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -35019,7 +35033,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -35037,7 +35051,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -35057,7 +35071,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -35077,7 +35091,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -35113,7 +35127,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -35131,7 +35145,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -35149,7 +35163,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -35167,7 +35181,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -35207,7 +35221,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35225,7 +35239,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35245,7 +35259,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -35263,7 +35277,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -35286,7 +35300,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35307,7 +35321,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35326,7 +35340,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -35346,7 +35360,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35368,7 +35382,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -35404,7 +35418,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -35424,7 +35438,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -35444,7 +35458,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -35462,7 +35476,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -35480,7 +35494,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35498,7 +35512,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -35518,7 +35532,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -35538,7 +35552,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35558,7 +35572,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -35567,10 +35581,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -35582,7 +35596,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35600,7 +35614,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -35612,7 +35626,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -35624,7 +35638,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -35639,7 +35653,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -35663,7 +35677,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -35677,7 +35691,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -35689,7 +35703,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -35703,7 +35717,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -35717,7 +35731,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -35729,7 +35743,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -35741,7 +35755,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -35753,7 +35767,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -35765,7 +35779,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -35777,7 +35791,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -35789,7 +35803,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -35801,7 +35815,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -35815,7 +35829,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -35827,7 +35841,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -35839,7 +35853,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -35853,7 +35867,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -35865,7 +35879,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -35877,7 +35891,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -35889,7 +35903,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -35901,7 +35915,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -35952,7 +35966,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -36003,7 +36017,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -36056,7 +36070,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -36109,7 +36123,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -36160,7 +36174,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -36211,7 +36225,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -36262,7 +36276,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -36315,7 +36329,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -36366,7 +36380,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -36419,7 +36433,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -36470,7 +36484,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -36521,7 +36535,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -36574,7 +36588,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -36625,7 +36639,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -36678,7 +36692,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -36780,7 +36794,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -36884,7 +36898,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -37042,7 +37056,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -37095,7 +37109,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -37197,7 +37211,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -37250,7 +37264,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -37259,7 +37273,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -37359,7 +37373,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -37410,7 +37424,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -37463,7 +37477,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -37516,7 +37530,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -37620,7 +37634,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -37718,7 +37732,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -40897,7 +40911,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -40914,7 +40928,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -40931,7 +40945,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -40948,7 +40962,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -40967,7 +40981,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -40984,7 +40998,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -41001,7 +41015,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -41018,7 +41032,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -41037,7 +41051,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -41054,7 +41068,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -41071,7 +41085,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -41088,7 +41102,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -41105,7 +41119,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -41124,7 +41138,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -41141,7 +41155,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -41158,7 +41172,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -41743,14 +41757,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -41763,17 +41777,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -41783,7 +41797,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -41801,7 +41815,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -41817,7 +41831,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -41833,7 +41847,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -41849,7 +41863,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -41865,7 +41879,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -41883,17 +41897,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -41903,7 +41917,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -41921,17 +41935,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -41943,17 +41957,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -41965,7 +41979,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -41973,7 +41987,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -41983,7 +41997,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -42000,7 +42014,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -42017,7 +42031,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -42036,7 +42050,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -42054,14 +42068,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -42074,14 +42088,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -42092,7 +42106,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -42108,14 +42122,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -42126,7 +42140,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -42144,7 +42158,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -42153,7 +42167,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -42164,7 +42178,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -42180,7 +42194,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -42196,7 +42210,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -42212,7 +42226,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -42228,7 +42242,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -42246,7 +42260,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -42262,7 +42276,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -42278,7 +42292,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -42294,7 +42308,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -42310,7 +42324,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -42344,14 +42358,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -42364,7 +42378,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -42380,7 +42394,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -42396,7 +42410,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -42430,7 +42444,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -42446,7 +42460,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -42464,7 +42478,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -42482,7 +42496,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -42500,13 +42514,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42517,7 +42531,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -42531,7 +42545,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -42545,7 +42559,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -42559,7 +42573,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -42571,7 +42585,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -42585,7 +42599,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -42599,7 +42613,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -42613,7 +42627,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -42627,7 +42641,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -42641,7 +42655,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -42653,7 +42667,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -42670,7 +42684,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -42682,7 +42696,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -42696,7 +42710,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -42713,7 +42727,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -42730,13 +42744,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42745,7 +42759,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -42759,7 +42773,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -42777,7 +42791,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -42791,13 +42805,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42808,7 +42822,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -42822,7 +42836,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -42836,7 +42850,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -42850,7 +42864,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -42862,7 +42876,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -42880,7 +42894,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -42894,13 +42908,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42911,7 +42925,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -42923,7 +42937,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -42937,13 +42951,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42952,7 +42966,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -42964,7 +42978,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -42978,7 +42992,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -42990,7 +43004,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -43002,7 +43016,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -43014,7 +43028,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -43028,13 +43042,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43045,7 +43059,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -43059,7 +43073,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -43073,7 +43087,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -43111,7 +43125,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -43125,7 +43139,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -43139,7 +43153,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -43169,7 +43183,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -43183,7 +43197,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -43197,7 +43211,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -43211,7 +43225,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -43225,7 +43239,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -43239,7 +43253,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -43253,7 +43267,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -43267,13 +43281,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43284,7 +43298,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -43298,7 +43312,7 @@
         <v>2469</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -43312,7 +43326,7 @@
         <v>2475</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -43326,7 +43340,7 @@
         <v>2582</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -43340,7 +43354,7 @@
         <v>2739</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -43354,7 +43368,7 @@
         <v>2745</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -43368,7 +43382,7 @@
         <v>2769</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -43691,7 +43705,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43860,7 +43874,7 @@
   <sheetPr/>
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -43923,7 +43937,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -43940,7 +43954,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -43959,7 +43973,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -43978,7 +43992,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -43998,7 +44012,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44018,7 +44032,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44039,7 +44053,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44059,7 +44073,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44069,10 +44083,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -44104,7 +44118,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -44124,7 +44138,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44144,7 +44158,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44167,7 +44181,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44187,7 +44201,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44207,19 +44221,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44233,7 +44247,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44251,7 +44265,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44271,7 +44285,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44280,7 +44294,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44294,7 +44308,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44314,7 +44328,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44332,7 +44346,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44352,7 +44366,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44361,10 +44375,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44376,7 +44390,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44396,7 +44410,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44414,7 +44428,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44497,7 +44511,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44517,7 +44531,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44537,7 +44551,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44547,7 +44561,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44559,7 +44573,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44579,7 +44593,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44713,7 +44727,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44727,7 +44741,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44741,7 +44755,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44755,13 +44769,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44772,7 +44786,7 @@
         <v>2733</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -44786,7 +44800,7 @@
         <v>2740</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -44982,7 +44996,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45004,13 +45018,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45024,13 +45038,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45041,7 +45055,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45055,7 +45069,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45069,7 +45083,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45083,7 +45097,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45106,7 +45120,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45115,7 +45129,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45166,7 +45180,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45187,14 +45201,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45210,7 +45224,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45245,7 +45259,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45254,7 +45268,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45291,7 +45305,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45312,7 +45326,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45322,7 +45336,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46781,7 +46795,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46796,13 +46810,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46843,7 +46857,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46858,7 +46872,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46918,7 +46932,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46931,7 +46945,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46956,7 +46970,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -46969,7 +46983,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -46982,7 +46996,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -46995,7 +47009,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47010,7 +47024,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47025,7 +47039,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47038,7 +47052,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47053,7 +47067,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2710 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24128" windowHeight="11091" tabRatio="991" firstSheet="5" activeTab="9"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="1559">
   <si>
     <t>Date</t>
   </si>
@@ -3636,6 +3636,9 @@
   </si>
   <si>
     <t>Lexicographically Smallest Palindrome</t>
+  </si>
+  <si>
+    <t>Remove Trailing Zeros From a String</t>
   </si>
   <si>
     <t>Find Maximum Number of String Pairs</t>
@@ -7511,7 +7514,7 @@
   <sheetPr/>
   <dimension ref="A1:AR105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A105" sqref="$A105:$XFD105"/>
     </sheetView>
   </sheetViews>
@@ -25468,10 +25471,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I213"/>
+  <dimension ref="A1:I214"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A213" sqref="A213"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -28263,10 +28266,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B210" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1152</v>
@@ -28277,43 +28280,57 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B211" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1153</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B212" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C212" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>1154</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
+        <v>45131</v>
+      </c>
+      <c r="B213" s="1">
+        <v>2788</v>
+      </c>
+      <c r="C213" s="16" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="39">
         <v>45144</v>
       </c>
-      <c r="B213" s="1">
+      <c r="B214" s="1">
         <v>2810</v>
       </c>
-      <c r="C213" s="1" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D213" s="1" t="s">
+      <c r="C214" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D214" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -28603,12 +28620,12 @@
       <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F211">
+  <conditionalFormatting sqref="F212">
     <cfRule type="containsText" dxfId="5" priority="27" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="35" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F211)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="43" operator="between">
       <formula>"Amazon"</formula>
@@ -28639,7 +28656,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D212">
+  <conditionalFormatting sqref="D213">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28661,12 +28678,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F212">
+  <conditionalFormatting sqref="F213">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="34" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="42" operator="between">
       <formula>"Amazon"</formula>
@@ -28697,12 +28714,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="F214">
     <cfRule type="containsText" dxfId="5" priority="25" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="33" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="41" operator="between">
       <formula>"Amazon"</formula>
@@ -28733,7 +28750,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A207:A210">
+  <conditionalFormatting sqref="A207:A211">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28767,7 +28784,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207:F210">
+  <conditionalFormatting sqref="F207:F211">
     <cfRule type="containsText" dxfId="5" priority="11" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
@@ -28803,7 +28820,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 A214:E1048576 G214:XFD1048576">
+  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 G215:XFD1048576 A215:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="191" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -28825,7 +28842,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F214:F1048576">
+  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F215:F1048576">
     <cfRule type="containsText" dxfId="5" priority="180" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -28993,7 +29010,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:XFD210 B207:E210">
+  <conditionalFormatting sqref="G207:XFD211 B207:E211">
     <cfRule type="cellIs" dxfId="0" priority="20" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29015,7 +29032,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G211:XFD211 A211:E211">
+  <conditionalFormatting sqref="G212:XFD212 A212:E212">
     <cfRule type="cellIs" dxfId="0" priority="99" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29037,7 +29054,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G212:XFD212 E212 A212:C212">
+  <conditionalFormatting sqref="G213:XFD213 A213:C213 E213">
     <cfRule type="cellIs" dxfId="0" priority="98" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29059,7 +29076,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G213:XFD213 A213:E213">
+  <conditionalFormatting sqref="G214:XFD214 A214:E214">
     <cfRule type="cellIs" dxfId="0" priority="97" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29154,7 +29171,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -29177,7 +29194,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -29197,7 +29214,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -29217,7 +29234,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -29237,7 +29254,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -29255,7 +29272,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -29273,7 +29290,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -29291,7 +29308,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -29311,7 +29328,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -29329,7 +29346,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -29347,7 +29364,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -29365,7 +29382,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -29383,7 +29400,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -29457,7 +29474,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -29475,7 +29492,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -29495,7 +29512,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -29507,7 +29524,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -29520,7 +29537,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -29540,7 +29557,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -29563,7 +29580,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -29584,7 +29601,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -29605,7 +29622,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -29625,7 +29642,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -29643,7 +29660,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -29661,7 +29678,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -29679,7 +29696,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -29697,7 +29714,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -29733,7 +29750,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -29753,7 +29770,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -29762,7 +29779,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -29773,7 +29790,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -29791,7 +29808,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -29813,7 +29830,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -29822,7 +29839,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -29838,7 +29855,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -29864,7 +29881,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -29879,7 +29896,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -29893,7 +29910,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -29907,7 +29924,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -29919,7 +29936,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -29933,7 +29950,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -29945,7 +29962,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -29957,7 +29974,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -29971,7 +29988,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -29985,7 +30002,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -31286,7 +31303,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -31304,7 +31321,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -31326,7 +31343,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -31346,7 +31363,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31366,7 +31383,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31384,7 +31401,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -31402,7 +31419,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -31420,7 +31437,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -31436,7 +31453,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -32877,7 +32894,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -32898,7 +32915,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -32916,7 +32933,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -32934,7 +32951,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32952,7 +32969,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -32973,7 +32990,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -32984,7 +33001,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -32994,7 +33011,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -33015,7 +33032,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -33033,7 +33050,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -33051,7 +33068,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -33069,7 +33086,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -33087,7 +33104,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -33105,7 +33122,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -33125,7 +33142,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -33146,7 +33163,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -33165,7 +33182,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -33186,7 +33203,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -33206,7 +33223,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -33224,7 +33241,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -33244,7 +33261,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -33264,7 +33281,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -33314,7 +33331,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -33334,7 +33351,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -33352,7 +33369,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -33370,7 +33387,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -33388,7 +33405,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -33408,7 +33425,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -33426,7 +33443,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -33444,7 +33461,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -33462,7 +33479,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -33480,7 +33497,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -33498,7 +33515,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -33516,7 +33533,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -33534,7 +33551,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -33554,7 +33571,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -33572,7 +33589,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -33590,7 +33607,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -33608,7 +33625,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -33628,7 +33645,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -33648,7 +33665,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -33669,7 +33686,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -33689,7 +33706,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -33707,7 +33724,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -33727,7 +33744,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -34977,7 +34994,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -34995,7 +35012,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -35015,7 +35032,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -35030,7 +35047,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -35045,7 +35062,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -35060,7 +35077,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -35069,10 +35086,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -35084,14 +35101,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -35102,7 +35119,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -35122,7 +35139,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -35140,7 +35157,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -35158,7 +35175,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -35178,7 +35195,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -35198,7 +35215,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -35234,7 +35251,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -35252,7 +35269,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -35270,7 +35287,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -35288,7 +35305,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -35328,7 +35345,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35346,7 +35363,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35366,7 +35383,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -35384,7 +35401,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -35407,7 +35424,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35428,7 +35445,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35447,7 +35464,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -35467,7 +35484,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35489,7 +35506,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -35525,7 +35542,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -35545,7 +35562,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -35565,7 +35582,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -35583,7 +35600,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -35601,7 +35618,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35619,7 +35636,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -35639,7 +35656,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -35659,7 +35676,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35679,7 +35696,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -35688,10 +35705,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -35703,7 +35720,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35721,7 +35738,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -35733,7 +35750,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -35745,7 +35762,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -35760,7 +35777,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -35784,7 +35801,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -35798,7 +35815,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -35810,7 +35827,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -35824,7 +35841,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -35838,7 +35855,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -35850,7 +35867,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -35862,7 +35879,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -35874,7 +35891,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -35886,7 +35903,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -35898,7 +35915,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -35910,7 +35927,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -35922,7 +35939,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -35936,7 +35953,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -35948,7 +35965,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -35960,7 +35977,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -35974,7 +35991,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -35986,7 +36003,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -35998,7 +36015,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -36010,7 +36027,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -36022,7 +36039,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -36073,7 +36090,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -36124,7 +36141,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -36177,7 +36194,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -36230,7 +36247,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -36281,7 +36298,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -36332,7 +36349,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -36383,7 +36400,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -36436,7 +36453,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -36487,7 +36504,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -36540,7 +36557,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -36591,7 +36608,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -36642,7 +36659,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -36695,7 +36712,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -36746,7 +36763,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -36799,7 +36816,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -36901,7 +36918,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -37005,7 +37022,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -37163,7 +37180,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -37216,7 +37233,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -37318,7 +37335,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -37371,7 +37388,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -37380,7 +37397,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -37480,7 +37497,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -37531,7 +37548,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -37584,7 +37601,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -37637,7 +37654,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -37741,7 +37758,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -37839,7 +37856,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -41018,7 +41035,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -41035,7 +41052,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -41052,7 +41069,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -41069,7 +41086,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -41088,7 +41105,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -41105,7 +41122,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -41122,7 +41139,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -41139,7 +41156,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -41158,7 +41175,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -41175,7 +41192,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -41192,7 +41209,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -41209,7 +41226,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -41226,7 +41243,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -41245,7 +41262,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -41262,7 +41279,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -41279,7 +41296,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -41864,14 +41881,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -41884,17 +41901,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -41904,7 +41921,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -41922,7 +41939,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -41938,7 +41955,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -41954,7 +41971,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -41970,7 +41987,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -41986,7 +42003,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -42004,17 +42021,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -42024,7 +42041,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -42042,17 +42059,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -42064,17 +42081,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -42086,7 +42103,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -42094,7 +42111,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -42104,7 +42121,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -42121,7 +42138,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -42138,7 +42155,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -42157,7 +42174,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -42175,14 +42192,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -42195,14 +42212,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -42213,7 +42230,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -42229,14 +42246,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -42247,7 +42264,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -42265,7 +42282,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -42274,7 +42291,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -42285,7 +42302,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -42301,7 +42318,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -42317,7 +42334,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -42333,7 +42350,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -42349,7 +42366,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -42367,7 +42384,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -42383,7 +42400,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -42399,7 +42416,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -42415,7 +42432,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -42431,7 +42448,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -42465,14 +42482,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -42485,7 +42502,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -42501,7 +42518,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -42517,7 +42534,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -42551,7 +42568,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -42567,7 +42584,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -42585,7 +42602,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -42603,7 +42620,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -42621,13 +42638,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42638,7 +42655,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -42652,7 +42669,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -42666,7 +42683,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -42680,7 +42697,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -42692,7 +42709,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -42706,7 +42723,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -42720,7 +42737,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -42734,7 +42751,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -42748,7 +42765,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -42762,7 +42779,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -42774,7 +42791,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -42791,7 +42808,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -42803,7 +42820,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -42817,7 +42834,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -42834,7 +42851,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -42851,13 +42868,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42866,7 +42883,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -42880,7 +42897,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -42898,7 +42915,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -42912,13 +42929,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -42929,7 +42946,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -42943,7 +42960,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -42957,7 +42974,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -42971,7 +42988,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -42983,7 +43000,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -43001,7 +43018,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -43015,13 +43032,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43032,7 +43049,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -43044,7 +43061,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -43058,13 +43075,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43073,7 +43090,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -43085,7 +43102,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -43099,7 +43116,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -43111,7 +43128,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -43123,7 +43140,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -43135,7 +43152,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -43149,13 +43166,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43166,7 +43183,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -43180,7 +43197,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -43194,7 +43211,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -43232,7 +43249,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -43246,7 +43263,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -43260,7 +43277,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -43290,7 +43307,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -43304,7 +43321,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -43318,7 +43335,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -43332,7 +43349,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -43346,7 +43363,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -43360,7 +43377,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -43374,7 +43391,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -43388,13 +43405,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43405,7 +43422,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -43419,7 +43436,7 @@
         <v>2469</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -43433,7 +43450,7 @@
         <v>2475</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -43447,7 +43464,7 @@
         <v>2582</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -43461,7 +43478,7 @@
         <v>2739</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -43475,7 +43492,7 @@
         <v>2745</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -43489,7 +43506,7 @@
         <v>2769</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -43812,7 +43829,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44044,7 +44061,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44061,7 +44078,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44080,7 +44097,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -44099,7 +44116,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -44119,7 +44136,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44139,7 +44156,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44160,7 +44177,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44180,7 +44197,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44190,10 +44207,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -44225,7 +44242,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -44245,7 +44262,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -44265,7 +44282,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -44288,7 +44305,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -44308,7 +44325,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -44328,19 +44345,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -44354,7 +44371,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -44372,7 +44389,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -44392,7 +44409,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -44401,7 +44418,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -44415,7 +44432,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -44435,7 +44452,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -44453,7 +44470,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -44473,7 +44490,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -44482,10 +44499,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -44497,7 +44514,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -44517,7 +44534,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44535,7 +44552,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44618,7 +44635,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -44638,7 +44655,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44658,7 +44675,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -44668,7 +44685,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -44680,7 +44697,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -44700,7 +44717,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -44834,7 +44851,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -44848,7 +44865,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -44862,7 +44879,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44876,13 +44893,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44893,7 +44910,7 @@
         <v>2733</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -44907,7 +44924,7 @@
         <v>2740</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -45103,7 +45120,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45125,13 +45142,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45145,13 +45162,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45162,7 +45179,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45176,7 +45193,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45190,7 +45207,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45204,7 +45221,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -45227,7 +45244,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45236,7 +45253,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -45287,7 +45304,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45308,14 +45325,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -45331,7 +45348,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -45366,7 +45383,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -45375,7 +45392,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -45412,7 +45429,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45433,7 +45450,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -45443,7 +45460,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -46902,7 +46919,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46917,13 +46934,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -46964,7 +46981,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46979,7 +46996,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47039,7 +47056,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47052,7 +47069,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47077,7 +47094,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47090,7 +47107,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -47103,7 +47120,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -47116,7 +47133,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47131,7 +47148,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47146,7 +47163,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47159,7 +47176,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47174,7 +47191,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2652 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="4" activeTab="9"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="7" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3379" uniqueCount="1560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1561">
   <si>
     <t>Date</t>
   </si>
@@ -4648,6 +4648,9 @@
   </si>
   <si>
     <t>Pass the Pillow</t>
+  </si>
+  <si>
+    <t>Sum Multipels</t>
   </si>
   <si>
     <t>Total Distance Traveled</t>
@@ -7517,7 +7520,7 @@
   <sheetPr/>
   <dimension ref="A1:AR113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
@@ -42606,10 +42609,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44251,10 +44254,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B114" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1482</v>
@@ -44264,11 +44267,11 @@
       </c>
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A115" s="27">
-        <v>45133</v>
+      <c r="A115" s="4">
+        <v>45131</v>
       </c>
       <c r="B115" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1483</v>
@@ -44279,10 +44282,10 @@
     </row>
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A116" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B116" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>1484</v>
@@ -44291,9 +44294,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A117" s="11"/>
-      <c r="B117" s="12"/>
+    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A117" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B117" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A118" s="11"/>
@@ -44302,6 +44315,10 @@
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A119" s="11"/>
       <c r="B119" s="12"/>
+    </row>
+    <row r="120" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A120" s="11"/>
+      <c r="B120" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -44399,7 +44416,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F119">
+  <conditionalFormatting sqref="F107:F120">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -44438,7 +44455,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G120:XFD1048576 A120:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A121:E1048576 G121:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44460,7 +44477,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F120:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F121:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -44521,7 +44538,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD119 A107:E119">
+  <conditionalFormatting sqref="G107:XFD120 A107:E120">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44608,7 +44625,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44840,7 +44857,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44857,7 +44874,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44876,7 +44893,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -44895,7 +44912,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -44915,7 +44932,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44935,7 +44952,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44956,7 +44973,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44976,7 +44993,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -44986,10 +45003,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45021,7 +45038,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45041,7 +45058,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45061,7 +45078,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45084,7 +45101,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45104,7 +45121,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45124,19 +45141,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45150,7 +45167,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45168,7 +45185,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45188,7 +45205,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45197,7 +45214,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45211,7 +45228,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45231,7 +45248,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45249,7 +45266,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45269,7 +45286,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45278,10 +45295,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45293,7 +45310,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45313,7 +45330,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45331,7 +45348,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45414,7 +45431,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45434,7 +45451,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45454,7 +45471,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45464,7 +45481,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45476,7 +45493,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45496,7 +45513,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45630,7 +45647,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45644,7 +45661,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45658,7 +45675,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45672,13 +45689,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45689,7 +45706,7 @@
         <v>2733</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45703,7 +45720,7 @@
         <v>2740</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -45921,13 +45938,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45941,13 +45958,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45958,7 +45975,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45972,7 +45989,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -45986,7 +46003,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46000,7 +46017,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46032,7 +46049,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46083,7 +46100,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46104,14 +46121,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46127,7 +46144,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46162,7 +46179,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46171,7 +46188,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46208,7 +46225,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46229,7 +46246,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46239,7 +46256,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47713,13 +47730,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47760,7 +47777,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47775,7 +47792,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47835,7 +47852,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47848,7 +47865,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47873,7 +47890,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47886,7 +47903,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -47899,7 +47916,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -47912,7 +47929,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47927,7 +47944,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47942,7 +47959,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47955,7 +47972,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47970,7 +47987,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2413 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1562">
   <si>
     <t>Date</t>
   </si>
@@ -4639,6 +4639,9 @@
   </si>
   <si>
     <t>Largest Number After Digit Swaps by Parity</t>
+  </si>
+  <si>
+    <t>Smallest Even Multiple</t>
   </si>
   <si>
     <t>Convert the Temperature</t>
@@ -42609,10 +42612,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44212,10 +44215,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A111" s="4">
-        <v>45141</v>
+        <v>45146</v>
       </c>
       <c r="B111" s="12">
-        <v>2469</v>
+        <v>2413</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>1479</v>
@@ -44229,7 +44232,7 @@
         <v>45141</v>
       </c>
       <c r="B112" s="12">
-        <v>2475</v>
+        <v>2469</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1480</v>
@@ -44240,10 +44243,10 @@
     </row>
     <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A113" s="4">
-        <v>45137</v>
+        <v>45141</v>
       </c>
       <c r="B113" s="12">
-        <v>2582</v>
+        <v>2475</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1481</v>
@@ -44254,10 +44257,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45145</v>
+        <v>45137</v>
       </c>
       <c r="B114" s="12">
-        <v>2652</v>
+        <v>2582</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1482</v>
@@ -44268,10 +44271,10 @@
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A115" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B115" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1483</v>
@@ -44281,11 +44284,11 @@
       </c>
     </row>
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A116" s="27">
-        <v>45133</v>
+      <c r="A116" s="4">
+        <v>45131</v>
       </c>
       <c r="B116" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>1484</v>
@@ -44296,10 +44299,10 @@
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B117" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1485</v>
@@ -44308,9 +44311,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A118" s="11"/>
-      <c r="B118" s="12"/>
+    <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A118" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B118" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A119" s="11"/>
@@ -44319,6 +44332,10 @@
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A120" s="11"/>
       <c r="B120" s="12"/>
+    </row>
+    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A121" s="11"/>
+      <c r="B121" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -44416,7 +44433,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F120">
+  <conditionalFormatting sqref="F107:F121">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -44455,7 +44472,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A121:E1048576 G121:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G122:XFD1048576 A122:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44477,7 +44494,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F121:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F122:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -44538,7 +44555,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD120 A107:E120">
+  <conditionalFormatting sqref="G107:XFD121 A107:E121">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44625,7 +44642,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44857,7 +44874,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44874,7 +44891,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44893,7 +44910,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -44912,7 +44929,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -44932,7 +44949,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44952,7 +44969,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44973,7 +44990,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -44993,7 +45010,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45003,10 +45020,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45038,7 +45055,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45058,7 +45075,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45078,7 +45095,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45101,7 +45118,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45121,7 +45138,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45141,19 +45158,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45167,7 +45184,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45185,7 +45202,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45205,7 +45222,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45214,7 +45231,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45228,7 +45245,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45248,7 +45265,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45266,7 +45283,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45286,7 +45303,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45295,10 +45312,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45310,7 +45327,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45330,7 +45347,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45348,7 +45365,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45431,7 +45448,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45451,7 +45468,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45471,7 +45488,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45481,7 +45498,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45493,7 +45510,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45513,7 +45530,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45647,7 +45664,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45661,7 +45678,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45675,7 +45692,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45689,13 +45706,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45706,7 +45723,7 @@
         <v>2733</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45720,7 +45737,7 @@
         <v>2740</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -45938,13 +45955,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45958,13 +45975,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45975,7 +45992,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -45989,7 +46006,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46003,7 +46020,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46017,7 +46034,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46049,7 +46066,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46100,7 +46117,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46121,14 +46138,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46144,7 +46161,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46179,7 +46196,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46188,7 +46205,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46225,7 +46242,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46246,7 +46263,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46256,7 +46273,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47730,13 +47747,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47777,7 +47794,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47792,7 +47809,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47852,7 +47869,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47865,7 +47882,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47890,7 +47907,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47903,7 +47920,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -47916,7 +47933,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -47929,7 +47946,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47944,7 +47961,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47959,7 +47976,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47972,7 +47989,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -47987,7 +48004,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2418 Category: Sort Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="7" activeTab="20"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="1563">
   <si>
     <t>Date</t>
   </si>
@@ -4789,6 +4789,9 @@
   </si>
   <si>
     <t>to_string</t>
+  </si>
+  <si>
+    <t>Sort the People</t>
   </si>
   <si>
     <t>Neither Minimum nor Maximum</t>
@@ -42614,7 +42617,7 @@
   <sheetPr/>
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
@@ -44809,9 +44812,9 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -45717,10 +45720,10 @@
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A50" s="26">
-        <v>45143</v>
+        <v>45146</v>
       </c>
       <c r="B50" s="12">
-        <v>2733</v>
+        <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1529</v>
@@ -45730,22 +45733,32 @@
       </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A51" s="27">
-        <v>45135</v>
+      <c r="A51" s="26">
+        <v>45143</v>
       </c>
       <c r="B51" s="12">
-        <v>2740</v>
+        <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>1530</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A52" s="27">
+        <v>45135</v>
+      </c>
+      <c r="B52" s="12">
+        <v>2740</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A53" s="11"/>
@@ -45798,6 +45811,10 @@
     <row r="65" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A65" s="11"/>
       <c r="B65" s="12"/>
+    </row>
+    <row r="66" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A66" s="11"/>
+      <c r="B66" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F$1:F$1048576">
@@ -45826,13 +45843,13 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:F63">
+  <conditionalFormatting sqref="F62:F64">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G$1:XFD$1048576 A1:E48 B49:E50 A51:E1048576">
+  <conditionalFormatting sqref="G$1:XFD$1048576 B49:E51 A1:E48 A52:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45955,13 +45972,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45975,13 +45992,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45992,7 +46009,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46006,7 +46023,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46020,7 +46037,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46034,7 +46051,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46066,7 +46083,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46117,7 +46134,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46138,14 +46155,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46161,7 +46178,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46196,7 +46213,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46205,7 +46222,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46242,7 +46259,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46263,7 +46280,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46273,7 +46290,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47747,13 +47764,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47794,7 +47811,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47869,7 +47886,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47882,7 +47899,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47907,7 +47924,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47920,7 +47937,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -47933,7 +47950,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -47946,7 +47963,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47961,7 +47978,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47976,7 +47993,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -47989,7 +48006,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48004,7 +48021,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2651 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="22"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="1563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3387" uniqueCount="1564">
   <si>
     <t>Date</t>
   </si>
@@ -4651,6 +4651,9 @@
   </si>
   <si>
     <t>Pass the Pillow</t>
+  </si>
+  <si>
+    <t>Calculate Delayed Arrival Time</t>
   </si>
   <si>
     <t>Sum Multipels</t>
@@ -42615,10 +42618,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44274,10 +44277,10 @@
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A115" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B115" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1483</v>
@@ -44288,10 +44291,10 @@
     </row>
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A116" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B116" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>1484</v>
@@ -44301,11 +44304,11 @@
       </c>
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A117" s="27">
-        <v>45133</v>
+      <c r="A117" s="4">
+        <v>45131</v>
       </c>
       <c r="B117" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1485</v>
@@ -44316,10 +44319,10 @@
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B118" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1486</v>
@@ -44328,9 +44331,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A119" s="11"/>
-      <c r="B119" s="12"/>
+    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A119" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B119" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A120" s="11"/>
@@ -44339,6 +44352,10 @@
     <row r="121" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A121" s="11"/>
       <c r="B121" s="12"/>
+    </row>
+    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A122" s="11"/>
+      <c r="B122" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -44436,7 +44453,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F121">
+  <conditionalFormatting sqref="F107:F122">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -44475,7 +44492,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G122:XFD1048576 A122:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A123:E1048576 G123:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44497,7 +44514,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F122:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F123:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -44558,7 +44575,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD121 A107:E121">
+  <conditionalFormatting sqref="G107:XFD122 A107:E122">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44645,7 +44662,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44814,7 +44831,7 @@
   <sheetPr/>
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -44877,7 +44894,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44894,7 +44911,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44913,7 +44930,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -44932,7 +44949,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -44952,7 +44969,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -44972,7 +44989,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -44993,7 +45010,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45013,7 +45030,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45023,10 +45040,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45058,7 +45075,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45078,7 +45095,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45098,7 +45115,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45121,7 +45138,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45141,7 +45158,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45161,19 +45178,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45187,7 +45204,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45205,7 +45222,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45225,7 +45242,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45234,7 +45251,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45248,7 +45265,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45268,7 +45285,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45286,7 +45303,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45306,7 +45323,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45315,10 +45332,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45330,7 +45347,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45350,7 +45367,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45368,7 +45385,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45451,7 +45468,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45471,7 +45488,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45491,7 +45508,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45501,7 +45518,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45513,7 +45530,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45533,7 +45550,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45667,7 +45684,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45681,7 +45698,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45695,7 +45712,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45709,13 +45726,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45726,7 +45743,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45740,7 +45757,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45754,7 +45771,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -45972,13 +45989,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -45992,13 +46009,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46009,7 +46026,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46023,7 +46040,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46037,7 +46054,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46051,7 +46068,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46083,7 +46100,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46134,7 +46151,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46155,14 +46172,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46178,7 +46195,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46213,7 +46230,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46222,7 +46239,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46259,7 +46276,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46280,7 +46297,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46290,7 +46307,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47764,13 +47781,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47811,7 +47828,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47826,7 +47843,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47886,7 +47903,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47899,7 +47916,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47924,7 +47941,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47937,7 +47954,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -47950,7 +47967,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -47963,7 +47980,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -47978,7 +47995,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -47993,7 +48010,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48006,7 +48023,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48021,7 +48038,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2485 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="13"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="1566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="1567">
   <si>
     <t>Date</t>
   </si>
@@ -4654,6 +4654,9 @@
   </si>
   <si>
     <t>Number of Uneual Triplets in Array</t>
+  </si>
+  <si>
+    <t>Find the Pivot Integer</t>
   </si>
   <si>
     <t>Pass the Pillow</t>
@@ -14741,7 +14744,7 @@
   <sheetPr/>
   <dimension ref="A1:AV282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+    <sheetView topLeftCell="A246" workbookViewId="0">
       <selection activeCell="A273" sqref="A273"/>
     </sheetView>
   </sheetViews>
@@ -42649,10 +42652,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A115" sqref="$A115:$XFD115"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44294,10 +44297,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45137</v>
+        <v>45148</v>
       </c>
       <c r="B114" s="12">
-        <v>2582</v>
+        <v>2485</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1484</v>
@@ -44306,30 +44309,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A115" s="4"/>
-      <c r="B115" s="12"/>
-    </row>
-    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A116" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B116" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C116" s="1" t="s">
+    <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A115" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B115" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>1485</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A116" s="4"/>
+      <c r="B116" s="12"/>
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B117" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1486</v>
@@ -44340,10 +44343,10 @@
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B118" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1487</v>
@@ -44353,11 +44356,11 @@
       </c>
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A119" s="27">
-        <v>45133</v>
+      <c r="A119" s="4">
+        <v>45131</v>
       </c>
       <c r="B119" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>1488</v>
@@ -44368,10 +44371,10 @@
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A120" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B120" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1489</v>
@@ -44380,9 +44383,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A121" s="11"/>
-      <c r="B121" s="12"/>
+    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A121" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B121" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="122" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A122" s="11"/>
@@ -44391,6 +44404,10 @@
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A123" s="11"/>
       <c r="B123" s="12"/>
+    </row>
+    <row r="124" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A124" s="11"/>
+      <c r="B124" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -44488,7 +44505,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F123">
+  <conditionalFormatting sqref="F107:F124">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -44527,7 +44544,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G124:XFD1048576 A124:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A125:E1048576 G125:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44549,7 +44566,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F124:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F125:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -44610,7 +44627,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD123 A107:E123">
+  <conditionalFormatting sqref="G107:XFD124 A107:E124">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44697,7 +44714,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44929,7 +44946,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44946,7 +44963,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44965,7 +44982,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -44984,7 +45001,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45004,7 +45021,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45024,7 +45041,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45045,7 +45062,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45065,7 +45082,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45075,10 +45092,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45110,7 +45127,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45130,7 +45147,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45150,7 +45167,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45173,7 +45190,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45193,7 +45210,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45213,19 +45230,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45239,7 +45256,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45257,7 +45274,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45277,7 +45294,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45286,7 +45303,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45300,7 +45317,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45320,7 +45337,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45338,7 +45355,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45358,7 +45375,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45367,10 +45384,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45382,7 +45399,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45402,7 +45419,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45420,7 +45437,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45503,7 +45520,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45523,7 +45540,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45543,7 +45560,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45553,7 +45570,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45565,7 +45582,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45585,7 +45602,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45719,7 +45736,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45733,7 +45750,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45747,7 +45764,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45761,13 +45778,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45778,7 +45795,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45792,7 +45809,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45806,7 +45823,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46024,13 +46041,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46044,13 +46061,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46061,7 +46078,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46075,7 +46092,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46089,7 +46106,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46103,7 +46120,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46135,7 +46152,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46186,7 +46203,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46207,14 +46224,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46230,7 +46247,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46265,7 +46282,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46274,7 +46291,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46311,7 +46328,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46332,7 +46349,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46342,7 +46359,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47816,13 +47833,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47863,7 +47880,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47878,7 +47895,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47938,7 +47955,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47951,7 +47968,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47976,7 +47993,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -47989,7 +48006,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48002,7 +48019,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48015,7 +48032,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48030,7 +48047,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48045,7 +48062,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48058,7 +48075,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48073,7 +48090,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2315 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="1567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3395" uniqueCount="1568">
   <si>
     <t>Date</t>
   </si>
@@ -4645,6 +4645,9 @@
   </si>
   <si>
     <t>Largest Number After Digit Swaps by Parity</t>
+  </si>
+  <si>
+    <t>Count Asterisks</t>
   </si>
   <si>
     <t>Smallest Even Multiple</t>
@@ -42652,10 +42655,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44255,10 +44258,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A111" s="4">
-        <v>45146</v>
+        <v>45149</v>
       </c>
       <c r="B111" s="12">
-        <v>2413</v>
+        <v>2315</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>1481</v>
@@ -44269,10 +44272,10 @@
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A112" s="4">
-        <v>45141</v>
+        <v>45146</v>
       </c>
       <c r="B112" s="12">
-        <v>2469</v>
+        <v>2413</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1482</v>
@@ -44286,7 +44289,7 @@
         <v>45141</v>
       </c>
       <c r="B113" s="12">
-        <v>2475</v>
+        <v>2469</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1483</v>
@@ -44297,10 +44300,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45148</v>
+        <v>45141</v>
       </c>
       <c r="B114" s="12">
-        <v>2485</v>
+        <v>2475</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1484</v>
@@ -44311,10 +44314,10 @@
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A115" s="4">
-        <v>45137</v>
+        <v>45148</v>
       </c>
       <c r="B115" s="12">
-        <v>2582</v>
+        <v>2485</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1485</v>
@@ -44323,30 +44326,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="12"/>
-    </row>
-    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A117" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B117" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C117" s="1" t="s">
+    <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A116" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B116" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>1486</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="117" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="12"/>
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B118" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1487</v>
@@ -44357,10 +44360,10 @@
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A119" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B119" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>1488</v>
@@ -44370,11 +44373,11 @@
       </c>
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A120" s="27">
-        <v>45133</v>
+      <c r="A120" s="4">
+        <v>45131</v>
       </c>
       <c r="B120" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1489</v>
@@ -44385,10 +44388,10 @@
     </row>
     <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A121" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B121" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>1490</v>
@@ -44397,9 +44400,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A122" s="11"/>
-      <c r="B122" s="12"/>
+    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A122" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B122" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A123" s="11"/>
@@ -44408,6 +44421,10 @@
     <row r="124" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A124" s="11"/>
       <c r="B124" s="12"/>
+    </row>
+    <row r="125" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A125" s="11"/>
+      <c r="B125" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -44505,7 +44522,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F124">
+  <conditionalFormatting sqref="F107:F125">
     <cfRule type="containsText" dxfId="10" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -44544,7 +44561,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A125:E1048576 G125:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G126:XFD1048576 A126:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44566,7 +44583,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F125:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F126:F1048576">
     <cfRule type="containsText" dxfId="10" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -44627,7 +44644,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD124 A107:E124">
+  <conditionalFormatting sqref="G107:XFD125 A107:E125">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -44714,7 +44731,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -44946,7 +44963,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -44963,7 +44980,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -44982,7 +44999,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45001,7 +45018,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45021,7 +45038,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45041,7 +45058,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45062,7 +45079,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45082,7 +45099,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45092,10 +45109,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45127,7 +45144,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45147,7 +45164,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45167,7 +45184,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45190,7 +45207,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45210,7 +45227,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45230,19 +45247,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45256,7 +45273,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45274,7 +45291,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45294,7 +45311,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45303,7 +45320,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45317,7 +45334,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45337,7 +45354,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45355,7 +45372,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45375,7 +45392,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45384,10 +45401,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45399,7 +45416,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45419,7 +45436,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45437,7 +45454,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45520,7 +45537,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45540,7 +45557,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45560,7 +45577,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45570,7 +45587,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45582,7 +45599,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45602,7 +45619,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45736,7 +45753,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45750,7 +45767,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45764,7 +45781,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45778,13 +45795,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45795,7 +45812,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45809,7 +45826,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45823,7 +45840,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46041,13 +46058,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46061,13 +46078,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46078,7 +46095,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46092,7 +46109,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46106,7 +46123,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46120,7 +46137,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46152,7 +46169,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46203,7 +46220,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46224,14 +46241,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46247,7 +46264,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46282,7 +46299,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46291,7 +46308,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46328,7 +46345,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46349,7 +46366,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46359,7 +46376,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47833,13 +47850,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47880,7 +47897,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47895,7 +47912,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47955,7 +47972,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47968,7 +47985,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -47993,7 +48010,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48006,7 +48023,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48019,7 +48036,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48032,7 +48049,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48047,7 +48064,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48062,7 +48079,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48075,7 +48092,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48090,7 +48107,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2496 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="9"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3399" uniqueCount="1570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="1571">
   <si>
     <t>Date</t>
   </si>
@@ -3645,6 +3645,9 @@
   </si>
   <si>
     <t>Remove Letter To Equalize Frequency</t>
+  </si>
+  <si>
+    <t>Maximum Value of a String in an Array</t>
   </si>
   <si>
     <t>Number of Senior Citizens</t>
@@ -7550,7 +7553,7 @@
   <sheetPr/>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
@@ -26358,10 +26361,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I214"/>
+  <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A204" sqref="$A204:$XFD204"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29136,10 +29139,10 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="39">
-        <v>45135</v>
+        <v>45150</v>
       </c>
       <c r="B208" s="1">
-        <v>2678</v>
+        <v>2496</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>1155</v>
@@ -29150,10 +29153,10 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="39">
-        <v>45140</v>
+        <v>45135</v>
       </c>
       <c r="B209" s="1">
-        <v>2697</v>
+        <v>2678</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>1156</v>
@@ -29164,10 +29167,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B210" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1157</v>
@@ -29178,10 +29181,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B211" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1158</v>
@@ -29192,43 +29195,57 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B212" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>1159</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B213" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C213" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>1160</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="39">
+        <v>45131</v>
+      </c>
+      <c r="B214" s="1">
+        <v>2788</v>
+      </c>
+      <c r="C214" s="16" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="39">
         <v>45144</v>
       </c>
-      <c r="B214" s="1">
+      <c r="B215" s="1">
         <v>2810</v>
       </c>
-      <c r="C214" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D214" s="1" t="s">
+      <c r="C215" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -29521,12 +29538,12 @@
       <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F212">
+  <conditionalFormatting sqref="F213">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F212)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -29557,7 +29574,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D213">
+  <conditionalFormatting sqref="D214">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29579,12 +29596,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="F214">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -29615,12 +29632,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F214">
+  <conditionalFormatting sqref="F215">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -29651,7 +29668,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A207:A211">
+  <conditionalFormatting sqref="A207:A212">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29685,7 +29702,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207:F211">
+  <conditionalFormatting sqref="F207:F212">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
@@ -29721,7 +29738,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 G215:XFD1048576 A215:E1048576">
+  <conditionalFormatting sqref="G1:XFD186 A1:E170 D171:E171 A171:B171 A172:E178 D179:E179 A179:B179 A180:E186 G188:XFD192 A188:E192 A194:E195 G194:XFD202 A197:E202 D196:E196 A196:B196 A216:E1048576 G216:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29743,7 +29760,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F215:F1048576">
+  <conditionalFormatting sqref="F1:F186 F188:F192 F194:F202 F216:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -29911,7 +29928,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G207:XFD211 B207:E211">
+  <conditionalFormatting sqref="G207:XFD212 B207:E212">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29933,7 +29950,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G212:XFD212 A212:E212">
+  <conditionalFormatting sqref="G213:XFD213 A213:E213">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29955,7 +29972,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G213:XFD213 A213:C213 E213">
+  <conditionalFormatting sqref="G214:XFD214 E214 A214:C214">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29977,7 +29994,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G214:XFD214 A214:E214">
+  <conditionalFormatting sqref="G215:XFD215 A215:E215">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30072,7 +30089,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30095,7 +30112,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30115,7 +30132,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30135,7 +30152,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30155,7 +30172,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30173,7 +30190,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30191,7 +30208,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30209,7 +30226,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30229,7 +30246,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30247,7 +30264,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30265,7 +30282,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30283,7 +30300,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30301,7 +30318,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -30375,7 +30392,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -30393,7 +30410,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -30413,7 +30430,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -30425,7 +30442,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -30438,7 +30455,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -30458,7 +30475,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -30481,7 +30498,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -30502,7 +30519,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -30523,7 +30540,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -30543,7 +30560,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -30561,7 +30578,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -30579,7 +30596,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -30597,7 +30614,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -30615,7 +30632,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -30651,7 +30668,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -30671,7 +30688,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -30680,7 +30697,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -30691,7 +30708,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -30709,7 +30726,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -30731,7 +30748,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -30740,7 +30757,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -30756,7 +30773,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -30782,7 +30799,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -30797,7 +30814,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -30811,7 +30828,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -30825,7 +30842,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -30837,7 +30854,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -30851,7 +30868,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -30863,7 +30880,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -30875,7 +30892,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -30889,7 +30906,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -30903,7 +30920,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32204,7 +32221,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32222,7 +32239,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32244,7 +32261,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32264,7 +32281,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32284,7 +32301,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32302,7 +32319,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32320,7 +32337,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32338,7 +32355,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -32354,7 +32371,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -33795,7 +33812,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -33816,7 +33833,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -33834,7 +33851,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -33852,7 +33869,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33870,7 +33887,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -33891,7 +33908,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -33902,7 +33919,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -33912,7 +33929,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -33933,7 +33950,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -33951,7 +33968,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -33969,7 +33986,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -33987,7 +34004,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34005,7 +34022,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34023,7 +34040,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34043,7 +34060,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34064,7 +34081,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34083,7 +34100,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34104,7 +34121,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34124,7 +34141,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34142,7 +34159,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34162,7 +34179,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34182,7 +34199,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34232,7 +34249,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34252,7 +34269,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34270,7 +34287,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34288,7 +34305,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34306,7 +34323,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34326,7 +34343,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34344,7 +34361,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -34362,7 +34379,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -34380,7 +34397,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -34398,7 +34415,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -34416,7 +34433,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -34434,7 +34451,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -34452,7 +34469,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -34472,7 +34489,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -34490,7 +34507,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -34508,7 +34525,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -34526,7 +34543,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -34546,7 +34563,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -34566,7 +34583,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -34587,7 +34604,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -34607,7 +34624,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -34625,7 +34642,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -34645,7 +34662,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -35895,7 +35912,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -35913,7 +35930,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -35933,7 +35950,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -35948,7 +35965,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -35963,7 +35980,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -35978,7 +35995,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -35987,10 +36004,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36002,14 +36019,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36020,7 +36037,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36040,7 +36057,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36058,7 +36075,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36076,7 +36093,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36096,7 +36113,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36116,7 +36133,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36152,7 +36169,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36170,7 +36187,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36188,7 +36205,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36206,7 +36223,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36246,7 +36263,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36264,7 +36281,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36284,7 +36301,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36302,7 +36319,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36325,7 +36342,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36346,7 +36363,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -36365,7 +36382,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -36385,7 +36402,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -36407,7 +36424,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -36443,7 +36460,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -36463,7 +36480,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -36483,7 +36500,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -36501,7 +36518,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -36519,7 +36536,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -36537,7 +36554,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -36557,7 +36574,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -36577,7 +36594,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -36597,7 +36614,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -36606,10 +36623,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -36621,7 +36638,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -36639,7 +36656,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -36651,7 +36668,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -36663,7 +36680,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -36678,7 +36695,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -36702,7 +36719,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -36716,7 +36733,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -36728,7 +36745,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -36742,7 +36759,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -36756,7 +36773,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -36768,7 +36785,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -36780,7 +36797,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -36792,7 +36809,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -36804,7 +36821,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -36816,7 +36833,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -36828,7 +36845,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -36840,7 +36857,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -36854,7 +36871,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -36866,7 +36883,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -36878,7 +36895,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -36892,7 +36909,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -36904,7 +36921,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -36916,7 +36933,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -36928,7 +36945,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -36940,7 +36957,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -36991,7 +37008,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37042,7 +37059,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37095,7 +37112,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37148,7 +37165,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37199,7 +37216,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37250,7 +37267,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37301,7 +37318,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -37354,7 +37371,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -37405,7 +37422,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -37458,7 +37475,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -37509,7 +37526,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -37560,7 +37577,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -37613,7 +37630,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -37664,7 +37681,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -37717,7 +37734,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -37819,7 +37836,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -37923,7 +37940,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38081,7 +38098,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38134,7 +38151,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38236,7 +38253,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38289,7 +38306,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38298,7 +38315,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -38398,7 +38415,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -38449,7 +38466,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -38502,7 +38519,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -38555,7 +38572,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -38659,7 +38676,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -38757,7 +38774,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -41936,7 +41953,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -41953,7 +41970,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -41970,7 +41987,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -41987,7 +42004,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42006,7 +42023,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42023,7 +42040,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42040,7 +42057,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42057,7 +42074,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42076,7 +42093,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42093,7 +42110,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42110,7 +42127,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42127,7 +42144,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42144,7 +42161,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42163,7 +42180,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42180,7 +42197,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42197,7 +42214,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -42782,14 +42799,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -42802,17 +42819,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -42822,7 +42839,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -42840,7 +42857,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -42856,7 +42873,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -42872,7 +42889,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -42888,7 +42905,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -42904,7 +42921,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -42922,17 +42939,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -42942,7 +42959,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -42960,17 +42977,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -42982,17 +42999,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43004,7 +43021,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43012,7 +43029,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43022,7 +43039,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43039,7 +43056,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43056,7 +43073,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43075,7 +43092,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43093,14 +43110,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43113,14 +43130,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43131,7 +43148,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43147,14 +43164,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43165,7 +43182,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43183,7 +43200,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43192,7 +43209,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43203,7 +43220,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43219,7 +43236,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43235,7 +43252,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43251,7 +43268,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43267,7 +43284,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43285,7 +43302,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43301,7 +43318,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43317,7 +43334,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43333,7 +43350,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43349,7 +43366,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43383,14 +43400,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43403,7 +43420,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43419,7 +43436,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43435,7 +43452,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43469,7 +43486,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -43485,7 +43502,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -43503,7 +43520,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -43521,7 +43538,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -43539,13 +43556,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43556,7 +43573,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -43570,7 +43587,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -43584,7 +43601,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -43598,7 +43615,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -43610,7 +43627,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -43624,7 +43641,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -43638,7 +43655,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -43652,7 +43669,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -43666,7 +43683,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -43680,7 +43697,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -43692,7 +43709,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -43709,7 +43726,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -43721,7 +43738,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -43735,7 +43752,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -43752,7 +43769,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -43769,13 +43786,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43784,7 +43801,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -43798,7 +43815,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -43816,7 +43833,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -43830,13 +43847,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43847,7 +43864,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -43861,7 +43878,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -43875,7 +43892,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -43889,7 +43906,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -43901,7 +43918,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -43919,7 +43936,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -43933,13 +43950,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43950,7 +43967,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -43962,7 +43979,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -43976,13 +43993,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43991,7 +44008,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44003,7 +44020,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44017,7 +44034,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44029,7 +44046,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44041,7 +44058,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44053,7 +44070,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44067,13 +44084,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44084,7 +44101,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44098,7 +44115,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44112,7 +44129,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44150,7 +44167,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44164,7 +44181,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44178,7 +44195,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44208,7 +44225,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44222,7 +44239,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44236,7 +44253,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44250,7 +44267,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44264,7 +44281,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44278,7 +44295,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44292,7 +44309,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44306,13 +44323,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44323,7 +44340,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44337,7 +44354,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44352,7 +44369,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44366,7 +44383,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44380,7 +44397,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44394,7 +44411,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44408,7 +44425,7 @@
         <v>2582</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44426,7 +44443,7 @@
         <v>2651</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -44440,7 +44457,7 @@
         <v>2652</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -44454,7 +44471,7 @@
         <v>2739</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44468,7 +44485,7 @@
         <v>2745</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -44482,7 +44499,7 @@
         <v>2769</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -44805,7 +44822,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45037,7 +45054,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45054,7 +45071,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45073,7 +45090,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45092,7 +45109,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45112,7 +45129,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45132,7 +45149,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45153,7 +45170,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45173,7 +45190,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45183,10 +45200,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45218,7 +45235,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45238,7 +45255,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45258,7 +45275,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45281,7 +45298,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45301,7 +45318,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45321,19 +45338,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45347,7 +45364,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45365,7 +45382,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45385,7 +45402,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45394,7 +45411,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45408,7 +45425,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45428,7 +45445,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45446,7 +45463,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45466,7 +45483,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45475,10 +45492,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45490,7 +45507,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45510,7 +45527,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45528,7 +45545,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45611,7 +45628,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45631,7 +45648,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45651,7 +45668,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45661,7 +45678,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45673,7 +45690,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45693,7 +45710,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45827,7 +45844,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45841,7 +45858,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45855,7 +45872,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45869,13 +45886,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45886,7 +45903,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45900,7 +45917,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45914,7 +45931,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46110,7 +46127,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46132,13 +46149,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46152,13 +46169,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46169,7 +46186,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46183,7 +46200,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46197,7 +46214,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46211,7 +46228,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46234,7 +46251,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46243,7 +46260,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46294,7 +46311,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46315,14 +46332,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46338,7 +46355,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46373,7 +46390,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46382,7 +46399,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46419,7 +46436,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46440,7 +46457,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46450,7 +46467,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47909,7 +47926,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -47924,13 +47941,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47971,7 +47988,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -47986,7 +48003,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48046,7 +48063,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48059,7 +48076,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48084,7 +48101,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48097,7 +48114,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48110,7 +48127,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48123,7 +48140,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48138,7 +48155,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48153,7 +48170,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48166,7 +48183,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48181,7 +48198,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2236 Category: Tree Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="14"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="1571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1572">
   <si>
     <t>Date</t>
   </si>
@@ -4239,6 +4239,9 @@
   </si>
   <si>
     <t>Lowest Common Ancestor of a Binary Tree IV</t>
+  </si>
+  <si>
+    <t>Root Equals Sum of Children</t>
   </si>
   <si>
     <t>Ugly Number II</t>
@@ -26363,7 +26366,7 @@
   <sheetPr/>
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+    <sheetView topLeftCell="A197" workbookViewId="0">
       <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
@@ -35850,8 +35853,8 @@
   <sheetPr/>
   <dimension ref="A1:AR126"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -38955,10 +38958,18 @@
       <c r="AR103" s="1"/>
     </row>
     <row r="104" spans="1:44">
-      <c r="A104" s="11"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
+      <c r="A104" s="27">
+        <v>45150</v>
+      </c>
+      <c r="B104" s="12">
+        <v>2236</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
@@ -41953,7 +41964,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -41970,7 +41981,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -41987,7 +41998,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42004,7 +42015,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42023,7 +42034,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42040,7 +42051,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42057,7 +42068,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42074,7 +42085,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42093,7 +42104,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42110,7 +42121,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42127,7 +42138,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42144,7 +42155,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42161,7 +42172,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42180,7 +42191,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42197,7 +42208,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42214,7 +42225,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -42799,14 +42810,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -42819,17 +42830,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -42839,7 +42850,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -42857,7 +42868,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -42873,7 +42884,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -42889,7 +42900,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -42905,7 +42916,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -42921,7 +42932,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -42939,17 +42950,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -42959,7 +42970,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -42977,17 +42988,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -42999,17 +43010,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43021,7 +43032,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43029,7 +43040,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43039,7 +43050,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43056,7 +43067,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43073,7 +43084,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43092,7 +43103,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43110,14 +43121,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43130,14 +43141,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43148,7 +43159,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43164,14 +43175,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43182,7 +43193,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43200,7 +43211,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43209,7 +43220,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43220,7 +43231,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43236,7 +43247,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43252,7 +43263,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43284,7 +43295,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43302,7 +43313,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43318,7 +43329,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43334,7 +43345,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43350,7 +43361,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43366,7 +43377,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43400,14 +43411,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43420,7 +43431,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43436,7 +43447,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43452,7 +43463,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43486,7 +43497,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -43502,7 +43513,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -43520,7 +43531,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -43538,7 +43549,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -43556,13 +43567,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43573,7 +43584,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -43587,7 +43598,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -43601,7 +43612,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -43615,7 +43626,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -43627,7 +43638,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -43641,7 +43652,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -43655,7 +43666,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -43669,7 +43680,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -43683,7 +43694,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -43697,7 +43708,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -43709,7 +43720,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -43726,7 +43737,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -43738,7 +43749,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -43752,7 +43763,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -43769,7 +43780,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -43786,13 +43797,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43801,7 +43812,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -43815,7 +43826,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -43833,7 +43844,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -43847,13 +43858,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43864,7 +43875,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -43878,7 +43889,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -43892,7 +43903,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -43906,7 +43917,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -43918,7 +43929,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -43936,7 +43947,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -43950,13 +43961,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43967,7 +43978,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -43979,7 +43990,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -43993,13 +44004,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44008,7 +44019,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44020,7 +44031,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44034,7 +44045,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44046,7 +44057,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44058,7 +44069,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44070,7 +44081,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44084,13 +44095,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44101,7 +44112,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44115,7 +44126,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44129,7 +44140,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44167,7 +44178,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44181,7 +44192,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44195,7 +44206,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44225,7 +44236,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44239,7 +44250,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44253,7 +44264,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44267,7 +44278,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44281,7 +44292,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44295,7 +44306,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44309,7 +44320,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44323,13 +44334,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44340,7 +44351,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44354,7 +44365,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44369,7 +44380,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44383,7 +44394,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44397,7 +44408,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44411,7 +44422,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44425,7 +44436,7 @@
         <v>2582</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44443,7 +44454,7 @@
         <v>2651</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -44457,7 +44468,7 @@
         <v>2652</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -44471,7 +44482,7 @@
         <v>2739</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44485,7 +44496,7 @@
         <v>2745</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -44499,7 +44510,7 @@
         <v>2769</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -44822,7 +44833,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45054,7 +45065,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45071,7 +45082,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45090,7 +45101,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45109,7 +45120,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45129,7 +45140,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45149,7 +45160,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45170,7 +45181,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45190,7 +45201,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45200,10 +45211,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45235,7 +45246,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45255,7 +45266,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45275,7 +45286,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45298,7 +45309,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45318,7 +45329,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45338,19 +45349,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45364,7 +45375,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45382,7 +45393,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45402,7 +45413,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45411,7 +45422,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45425,7 +45436,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45445,7 +45456,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45463,7 +45474,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45483,7 +45494,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45492,10 +45503,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45507,7 +45518,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45527,7 +45538,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45545,7 +45556,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45628,7 +45639,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45648,7 +45659,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45668,7 +45679,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45678,7 +45689,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45690,7 +45701,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45710,7 +45721,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45844,7 +45855,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45858,7 +45869,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45872,7 +45883,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45886,13 +45897,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45903,7 +45914,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45917,7 +45928,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45931,7 +45942,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46149,13 +46160,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46169,13 +46180,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46186,7 +46197,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46200,7 +46211,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46214,7 +46225,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46228,7 +46239,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46260,7 +46271,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46311,7 +46322,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46332,14 +46343,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46355,7 +46366,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46390,7 +46401,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46399,7 +46410,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46436,7 +46447,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46457,7 +46468,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46467,7 +46478,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47941,13 +47952,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47988,7 +47999,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48003,7 +48014,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48063,7 +48074,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48076,7 +48087,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48101,7 +48112,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48114,7 +48125,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48127,7 +48138,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48140,7 +48151,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48155,7 +48166,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48170,7 +48181,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48183,7 +48194,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48198,7 +48209,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2309 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="18"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3405" uniqueCount="1573">
   <si>
     <t>Date</t>
   </si>
@@ -3639,6 +3639,9 @@
   </si>
   <si>
     <t>Percentage of Letter in String</t>
+  </si>
+  <si>
+    <t>Greatest English Letter in Upper and Lower Case</t>
   </si>
   <si>
     <t>Count Asterisks</t>
@@ -26366,8 +26369,8 @@
   <sheetPr/>
   <dimension ref="A1:I215"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="E211" sqref="E211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29103,8 +29106,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
-      <c r="A203" s="36"/>
+    <row r="203" spans="1:4">
+      <c r="A203" s="39">
+        <v>45151</v>
+      </c>
+      <c r="B203" s="1">
+        <v>2309</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="204" s="1" customFormat="1" spans="1:4">
       <c r="A204" s="4">
@@ -29114,7 +29128,7 @@
         <v>2315</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>11</v>
@@ -29134,7 +29148,7 @@
         <v>2423</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>11</v>
@@ -29148,7 +29162,7 @@
         <v>2496</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>11</v>
@@ -29162,7 +29176,7 @@
         <v>2678</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>11</v>
@@ -29176,7 +29190,7 @@
         <v>2697</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>11</v>
@@ -29190,7 +29204,7 @@
         <v>2710</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>11</v>
@@ -29204,7 +29218,7 @@
         <v>2744</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>11</v>
@@ -29218,7 +29232,7 @@
         <v>2785</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>13</v>
@@ -29232,7 +29246,7 @@
         <v>2788</v>
       </c>
       <c r="C214" s="16" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>11</v>
@@ -29246,7 +29260,7 @@
         <v>2810</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>11</v>
@@ -30092,7 +30106,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30115,7 +30129,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30135,7 +30149,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30155,7 +30169,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30175,7 +30189,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30193,7 +30207,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30211,7 +30225,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30229,7 +30243,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30249,7 +30263,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30267,7 +30281,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30285,7 +30299,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30303,7 +30317,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30321,7 +30335,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -30395,7 +30409,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -30413,7 +30427,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -30433,7 +30447,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -30445,7 +30459,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -30458,7 +30472,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -30478,7 +30492,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -30501,7 +30515,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -30522,7 +30536,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -30543,7 +30557,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -30563,7 +30577,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -30581,7 +30595,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -30599,7 +30613,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -30617,7 +30631,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -30635,7 +30649,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -30671,7 +30685,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -30691,7 +30705,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -30700,7 +30714,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -30711,7 +30725,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -30729,7 +30743,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -30751,7 +30765,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -30760,7 +30774,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -30776,7 +30790,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -30802,7 +30816,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -30817,7 +30831,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -30831,7 +30845,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -30845,7 +30859,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -30857,7 +30871,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -30871,7 +30885,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -30883,7 +30897,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -30895,7 +30909,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -30909,7 +30923,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -30923,7 +30937,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32224,7 +32238,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32242,7 +32256,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32264,7 +32278,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32284,7 +32298,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32304,7 +32318,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32322,7 +32336,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32340,7 +32354,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32358,7 +32372,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -32374,7 +32388,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -33815,7 +33829,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -33836,7 +33850,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -33854,7 +33868,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -33872,7 +33886,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33890,7 +33904,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -33911,7 +33925,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -33922,7 +33936,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -33932,7 +33946,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -33953,7 +33967,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -33971,7 +33985,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -33989,7 +34003,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34007,7 +34021,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34025,7 +34039,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34043,7 +34057,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34063,7 +34077,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34084,7 +34098,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34103,7 +34117,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34124,7 +34138,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34144,7 +34158,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34162,7 +34176,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34182,7 +34196,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34202,7 +34216,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34252,7 +34266,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34272,7 +34286,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34290,7 +34304,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34308,7 +34322,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34326,7 +34340,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34346,7 +34360,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34364,7 +34378,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -34382,7 +34396,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -34400,7 +34414,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -34418,7 +34432,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -34436,7 +34450,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -34454,7 +34468,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -34472,7 +34486,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -34492,7 +34506,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -34510,7 +34524,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -34528,7 +34542,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -34546,7 +34560,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -34566,7 +34580,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -34586,7 +34600,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -34607,7 +34621,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -34627,7 +34641,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -34645,7 +34659,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -34665,7 +34679,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -35853,7 +35867,7 @@
   <sheetPr/>
   <dimension ref="A1:AR126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A77" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
@@ -35915,7 +35929,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -35933,7 +35947,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -35953,7 +35967,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -35968,7 +35982,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -35983,7 +35997,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -35998,7 +36012,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36007,10 +36021,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36022,14 +36036,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36040,7 +36054,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36060,7 +36074,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36078,7 +36092,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36096,7 +36110,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36116,7 +36130,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36136,7 +36150,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36172,7 +36186,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36190,7 +36204,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36208,7 +36222,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36226,7 +36240,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36266,7 +36280,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36284,7 +36298,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36304,7 +36318,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36322,7 +36336,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36345,7 +36359,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36366,7 +36380,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -36385,7 +36399,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -36405,7 +36419,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -36427,7 +36441,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -36463,7 +36477,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -36483,7 +36497,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -36503,7 +36517,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -36521,7 +36535,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -36539,7 +36553,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -36557,7 +36571,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -36577,7 +36591,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -36597,7 +36611,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -36617,7 +36631,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -36626,10 +36640,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -36641,7 +36655,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -36659,7 +36673,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -36671,7 +36685,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -36683,7 +36697,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -36698,7 +36712,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -36722,7 +36736,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -36736,7 +36750,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -36748,7 +36762,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -36762,7 +36776,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -36776,7 +36790,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -36788,7 +36802,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -36800,7 +36814,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -36812,7 +36826,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -36824,7 +36838,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -36836,7 +36850,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -36848,7 +36862,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -36860,7 +36874,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -36874,7 +36888,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -36886,7 +36900,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -36898,7 +36912,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -36912,7 +36926,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -36924,7 +36938,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -36936,7 +36950,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -36948,7 +36962,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -36960,7 +36974,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37011,7 +37025,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37062,7 +37076,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37115,7 +37129,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37168,7 +37182,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37219,7 +37233,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37270,7 +37284,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37321,7 +37335,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -37374,7 +37388,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -37425,7 +37439,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -37478,7 +37492,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -37529,7 +37543,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -37580,7 +37594,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -37633,7 +37647,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -37684,7 +37698,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -37737,7 +37751,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -37839,7 +37853,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -37943,7 +37957,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38101,7 +38115,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38154,7 +38168,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38256,7 +38270,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38309,7 +38323,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38318,7 +38332,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -38418,7 +38432,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -38469,7 +38483,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -38522,7 +38536,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -38575,7 +38589,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -38679,7 +38693,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -38777,7 +38791,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -38965,7 +38979,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -41964,7 +41978,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -41981,7 +41995,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -41998,7 +42012,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42015,7 +42029,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42034,7 +42048,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42051,7 +42065,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42068,7 +42082,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42085,7 +42099,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42104,7 +42118,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42121,7 +42135,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42138,7 +42152,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42155,7 +42169,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42172,7 +42186,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42191,7 +42205,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42208,7 +42222,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42225,7 +42239,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -42810,14 +42824,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -42830,17 +42844,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -42850,7 +42864,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -42868,7 +42882,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -42884,7 +42898,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -42900,7 +42914,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -42916,7 +42930,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -42932,7 +42946,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -42950,17 +42964,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -42970,7 +42984,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -42988,17 +43002,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43010,17 +43024,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43032,7 +43046,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43040,7 +43054,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43050,7 +43064,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43067,7 +43081,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43084,7 +43098,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43103,7 +43117,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43121,14 +43135,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43141,14 +43155,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43159,7 +43173,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43175,14 +43189,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43193,7 +43207,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43211,7 +43225,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43220,7 +43234,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43231,7 +43245,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43247,7 +43261,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43263,7 +43277,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43279,7 +43293,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43295,7 +43309,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43313,7 +43327,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43329,7 +43343,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43345,7 +43359,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43361,7 +43375,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43377,7 +43391,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43411,14 +43425,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43431,7 +43445,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43447,7 +43461,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43463,7 +43477,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43497,7 +43511,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -43513,7 +43527,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -43531,7 +43545,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -43549,7 +43563,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -43567,13 +43581,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43584,7 +43598,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -43598,7 +43612,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -43612,7 +43626,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -43626,7 +43640,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -43638,7 +43652,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -43652,7 +43666,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -43666,7 +43680,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -43680,7 +43694,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -43694,7 +43708,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -43708,7 +43722,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -43720,7 +43734,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -43737,7 +43751,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -43749,7 +43763,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -43763,7 +43777,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -43780,7 +43794,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -43797,13 +43811,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43812,7 +43826,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -43826,7 +43840,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -43844,7 +43858,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -43858,13 +43872,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43875,7 +43889,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -43889,7 +43903,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -43903,7 +43917,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -43917,7 +43931,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -43929,7 +43943,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -43947,7 +43961,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -43961,13 +43975,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43978,7 +43992,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -43990,7 +44004,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44004,13 +44018,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44019,7 +44033,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44031,7 +44045,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44045,7 +44059,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44057,7 +44071,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44069,7 +44083,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44081,7 +44095,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44095,13 +44109,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44112,7 +44126,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44126,7 +44140,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44140,7 +44154,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44178,7 +44192,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44192,7 +44206,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44206,7 +44220,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44236,7 +44250,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44250,7 +44264,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44264,7 +44278,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44278,7 +44292,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44292,7 +44306,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44306,7 +44320,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44320,7 +44334,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44334,13 +44348,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44351,7 +44365,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44365,7 +44379,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44380,7 +44394,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44394,7 +44408,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44408,7 +44422,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44422,7 +44436,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44436,7 +44450,7 @@
         <v>2582</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44454,7 +44468,7 @@
         <v>2651</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -44468,7 +44482,7 @@
         <v>2652</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -44482,7 +44496,7 @@
         <v>2739</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44496,7 +44510,7 @@
         <v>2745</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -44510,7 +44524,7 @@
         <v>2769</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -44833,7 +44847,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45065,7 +45079,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45082,7 +45096,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45101,7 +45115,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45120,7 +45134,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45140,7 +45154,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45160,7 +45174,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45181,7 +45195,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45201,7 +45215,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45211,10 +45225,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45246,7 +45260,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45266,7 +45280,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45286,7 +45300,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45309,7 +45323,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45329,7 +45343,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45349,19 +45363,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45375,7 +45389,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45393,7 +45407,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45413,7 +45427,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45422,7 +45436,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45436,7 +45450,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45456,7 +45470,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45474,7 +45488,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45494,7 +45508,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45503,10 +45517,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45518,7 +45532,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45538,7 +45552,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45556,7 +45570,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45639,7 +45653,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45659,7 +45673,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45679,7 +45693,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45689,7 +45703,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45701,7 +45715,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45721,7 +45735,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -45855,7 +45869,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -45869,7 +45883,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -45883,7 +45897,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -45897,13 +45911,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45914,7 +45928,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -45928,7 +45942,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -45942,7 +45956,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46138,7 +46152,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46160,13 +46174,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46180,13 +46194,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46197,7 +46211,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46211,7 +46225,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46225,7 +46239,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46239,7 +46253,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46262,7 +46276,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46271,7 +46285,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46322,7 +46336,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46343,14 +46357,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46366,7 +46380,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46401,7 +46415,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46410,7 +46424,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46447,7 +46461,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46468,7 +46482,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46478,7 +46492,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -47937,7 +47951,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -47952,13 +47966,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -47999,7 +48013,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48014,7 +48028,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48074,7 +48088,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48087,7 +48101,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48112,7 +48126,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48125,7 +48139,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48138,7 +48152,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48151,7 +48165,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48166,7 +48180,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48181,7 +48195,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48194,7 +48208,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48209,7 +48223,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2264 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3409" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="1576">
   <si>
     <t>Date</t>
   </si>
@@ -3642,6 +3642,9 @@
   </si>
   <si>
     <t>Remove Digit From Number to Maximize Result</t>
+  </si>
+  <si>
+    <t>Largest 3-Same-Digit Number in String</t>
   </si>
   <si>
     <t>Percentage of Letter in String</t>
@@ -26573,10 +26576,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I216"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29313,11 +29316,11 @@
       </c>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="39">
-        <v>44726</v>
+      <c r="A203" s="26">
+        <v>45153</v>
       </c>
       <c r="B203" s="1">
-        <v>2278</v>
+        <v>2264</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>1154</v>
@@ -29328,10 +29331,10 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="39">
-        <v>45151</v>
+        <v>44726</v>
       </c>
       <c r="B204" s="1">
-        <v>2309</v>
+        <v>2278</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>1155</v>
@@ -29340,12 +29343,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" s="1" customFormat="1" spans="1:4">
-      <c r="A205" s="4">
-        <v>45149</v>
-      </c>
-      <c r="B205" s="12">
-        <v>2315</v>
+    <row r="205" spans="1:4">
+      <c r="A205" s="39">
+        <v>45151</v>
+      </c>
+      <c r="B205" s="1">
+        <v>2309</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>1156</v>
@@ -29354,32 +29357,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
-      <c r="A206" s="36"/>
+    <row r="206" s="1" customFormat="1" spans="1:4">
+      <c r="A206" s="4">
+        <v>45149</v>
+      </c>
+      <c r="B206" s="12">
+        <v>2315</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="36"/>
     </row>
-    <row r="208" spans="1:4">
-      <c r="A208" s="39">
-        <v>44838</v>
-      </c>
-      <c r="B208" s="1">
-        <v>2423</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="208" spans="1:1">
+      <c r="A208" s="36"/>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="39">
-        <v>45150</v>
+        <v>44838</v>
       </c>
       <c r="B209" s="1">
-        <v>2496</v>
+        <v>2423</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>1158</v>
@@ -29390,10 +29393,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
-        <v>45135</v>
+        <v>45150</v>
       </c>
       <c r="B210" s="1">
-        <v>2678</v>
+        <v>2496</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1159</v>
@@ -29404,10 +29407,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45140</v>
+        <v>45135</v>
       </c>
       <c r="B211" s="1">
-        <v>2697</v>
+        <v>2678</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1160</v>
@@ -29418,10 +29421,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B212" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>1161</v>
@@ -29432,10 +29435,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B213" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>1162</v>
@@ -29446,43 +29449,57 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B214" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>1163</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B215" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C215" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>1164</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="39">
+        <v>45131</v>
+      </c>
+      <c r="B216" s="1">
+        <v>2788</v>
+      </c>
+      <c r="C216" s="16" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="39">
         <v>45144</v>
       </c>
-      <c r="B216" s="1">
+      <c r="B217" s="1">
         <v>2810</v>
       </c>
-      <c r="C216" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="D216" s="1" t="s">
+      <c r="C217" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D217" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -29628,12 +29645,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F204">
+  <conditionalFormatting sqref="F205">
     <cfRule type="containsText" dxfId="5" priority="47" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F204)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="55" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F204)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="63" operator="between">
       <formula>"Amazon"</formula>
@@ -29664,15 +29681,15 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F205">
+  <conditionalFormatting sqref="F206">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Apple",F206)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="3" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
       <formula>"Amazon"</formula>
@@ -29703,12 +29720,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
+  <conditionalFormatting sqref="F207">
     <cfRule type="containsText" dxfId="5" priority="45" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="53" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="61" operator="between">
       <formula>"Amazon"</formula>
@@ -29739,12 +29756,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
+  <conditionalFormatting sqref="F208">
     <cfRule type="containsText" dxfId="5" priority="44" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="52" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="60" operator="between">
       <formula>"Amazon"</formula>
@@ -29775,12 +29792,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F214">
+  <conditionalFormatting sqref="F215">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -29811,7 +29828,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D215">
+  <conditionalFormatting sqref="D216">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29833,12 +29850,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F215">
+  <conditionalFormatting sqref="F216">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -29869,12 +29886,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F216">
+  <conditionalFormatting sqref="F217">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -29905,7 +29922,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A208:A213">
+  <conditionalFormatting sqref="A209:A214">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29939,12 +29956,12 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208:F213">
+  <conditionalFormatting sqref="F209:F214">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="27" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="28" operator="between">
       <formula>"Amazon"</formula>
@@ -29975,7 +29992,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 G217:XFD1048576 A217:E1048576 A197:B197 D197:E197 A198:E203 G195:XFD203 A195:E196 A189:E193 G189:XFD193 A181:E187 A180:B180 D180:E180">
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 G218:XFD1048576 A218:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -29997,7 +30014,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F217:F1048576 F195:F203 F189:F193">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F218:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30077,7 +30094,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G204:XFD204 A204:E204">
+  <conditionalFormatting sqref="G205:XFD205 A205:E205">
     <cfRule type="cellIs" dxfId="0" priority="119" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30095,55 +30112,55 @@
       <formula>"Medium"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="151" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G205:XFD205 A205:E205">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G206:XFD206 A206:E206">
-    <cfRule type="cellIs" dxfId="0" priority="117" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="125" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="133" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="141" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="149" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:XFD207 A207:E207">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="133" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="141" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="149" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G208:XFD208 A208:E208">
     <cfRule type="cellIs" dxfId="0" priority="116" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30165,7 +30182,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G208:XFD213 B208:E213">
+  <conditionalFormatting sqref="G209:XFD214 B209:E214">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30187,7 +30204,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G214:XFD214 A214:E214">
+  <conditionalFormatting sqref="G215:XFD215 A215:E215">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30209,7 +30226,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G215:XFD215 A215:C215 E215">
+  <conditionalFormatting sqref="G216:XFD216 E216 A216:C216">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30231,7 +30248,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G216:XFD216 A216:E216">
+  <conditionalFormatting sqref="G217:XFD217 A217:E217">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30326,7 +30343,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30349,7 +30366,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30369,7 +30386,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30389,7 +30406,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30409,7 +30426,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30427,7 +30444,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30445,7 +30462,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30463,7 +30480,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30483,7 +30500,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30501,7 +30518,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30519,7 +30536,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30537,7 +30554,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30555,7 +30572,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -30629,7 +30646,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -30647,7 +30664,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -30667,7 +30684,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -30679,7 +30696,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -30692,7 +30709,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -30712,7 +30729,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -30735,7 +30752,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -30756,7 +30773,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -30777,7 +30794,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -30797,7 +30814,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -30815,7 +30832,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -30833,7 +30850,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -30851,7 +30868,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -30869,7 +30886,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -30905,7 +30922,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -30925,7 +30942,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -30934,7 +30951,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -30945,7 +30962,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -30963,7 +30980,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -30985,7 +31002,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -30994,7 +31011,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31010,7 +31027,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31036,7 +31053,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31051,7 +31068,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31065,7 +31082,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31079,7 +31096,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31091,7 +31108,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31105,7 +31122,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31117,7 +31134,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31129,7 +31146,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31143,7 +31160,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31157,7 +31174,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32458,7 +32475,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32476,7 +32493,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32498,7 +32515,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32518,7 +32535,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32538,7 +32555,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32556,7 +32573,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32574,7 +32591,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32592,7 +32609,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -32608,7 +32625,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34049,7 +34066,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34070,7 +34087,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34088,7 +34105,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34106,7 +34123,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34124,7 +34141,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34145,7 +34162,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34156,7 +34173,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34166,7 +34183,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34187,7 +34204,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34205,7 +34222,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34223,7 +34240,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34241,7 +34258,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34259,7 +34276,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34277,7 +34294,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34297,7 +34314,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34318,7 +34335,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34337,7 +34354,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34358,7 +34375,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34378,7 +34395,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34396,7 +34413,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34416,7 +34433,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34436,7 +34453,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34486,7 +34503,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34506,7 +34523,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34524,7 +34541,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34542,7 +34559,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34560,7 +34577,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34580,7 +34597,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34598,7 +34615,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -34616,7 +34633,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -34634,7 +34651,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -34652,7 +34669,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -34670,7 +34687,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -34688,7 +34705,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -34706,7 +34723,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -34726,7 +34743,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -34744,7 +34761,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -34762,7 +34779,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -34780,7 +34797,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -34800,7 +34817,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -34820,7 +34837,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -34841,7 +34858,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -34861,7 +34878,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -34879,7 +34896,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -34899,7 +34916,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36149,7 +36166,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36167,7 +36184,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36187,7 +36204,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36202,7 +36219,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36217,7 +36234,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36232,7 +36249,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36241,10 +36258,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36256,14 +36273,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36274,7 +36291,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36294,7 +36311,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36312,7 +36329,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36330,7 +36347,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36350,7 +36367,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36370,7 +36387,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36406,7 +36423,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36424,7 +36441,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36442,7 +36459,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36460,7 +36477,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36500,7 +36517,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36518,7 +36535,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36538,7 +36555,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36556,7 +36573,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36579,7 +36596,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36600,7 +36617,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -36619,7 +36636,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -36639,7 +36656,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -36661,7 +36678,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -36697,7 +36714,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -36717,7 +36734,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -36737,7 +36754,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -36755,7 +36772,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -36773,7 +36790,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -36791,7 +36808,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -36811,7 +36828,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -36831,7 +36848,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -36851,7 +36868,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -36860,10 +36877,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -36875,7 +36892,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -36893,7 +36910,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -36905,7 +36922,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -36917,7 +36934,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -36932,7 +36949,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -36956,7 +36973,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -36970,7 +36987,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -36982,7 +36999,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -36996,7 +37013,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37010,7 +37027,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37022,7 +37039,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37034,7 +37051,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37046,7 +37063,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37058,7 +37075,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37070,7 +37087,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37082,7 +37099,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37094,7 +37111,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37108,7 +37125,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37120,7 +37137,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37132,7 +37149,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37146,7 +37163,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37158,7 +37175,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37170,7 +37187,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37182,7 +37199,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37194,7 +37211,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37245,7 +37262,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37296,7 +37313,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37349,7 +37366,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37402,7 +37419,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37453,7 +37470,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37504,7 +37521,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37555,7 +37572,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -37608,7 +37625,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -37659,7 +37676,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -37712,7 +37729,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -37763,7 +37780,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -37814,7 +37831,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -37867,7 +37884,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -37918,7 +37935,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -37971,7 +37988,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38073,7 +38090,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38177,7 +38194,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38335,7 +38352,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38388,7 +38405,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38490,7 +38507,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38543,7 +38560,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38552,7 +38569,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -38652,7 +38669,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -38703,7 +38720,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -38756,7 +38773,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -38809,7 +38826,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -38913,7 +38930,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39011,7 +39028,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39199,7 +39216,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42198,7 +42215,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42215,7 +42232,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42232,7 +42249,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42249,7 +42266,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42268,7 +42285,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42285,7 +42302,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42302,7 +42319,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42319,7 +42336,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42338,7 +42355,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42355,7 +42372,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42372,7 +42389,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42389,7 +42406,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42406,7 +42423,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42425,7 +42442,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42442,7 +42459,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42459,7 +42476,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43044,14 +43061,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43064,17 +43081,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43084,7 +43101,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43102,7 +43119,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43118,7 +43135,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43134,7 +43151,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43150,7 +43167,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43166,7 +43183,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43184,17 +43201,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43204,7 +43221,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43222,17 +43239,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43244,17 +43261,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43266,7 +43283,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43274,7 +43291,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43284,7 +43301,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43301,7 +43318,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43318,7 +43335,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43337,7 +43354,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43355,14 +43372,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43375,14 +43392,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43393,7 +43410,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43409,14 +43426,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43427,7 +43444,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43445,7 +43462,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43454,7 +43471,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43465,7 +43482,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43481,7 +43498,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43497,7 +43514,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43513,7 +43530,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43529,7 +43546,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43547,7 +43564,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43563,7 +43580,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43579,7 +43596,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43595,7 +43612,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43611,7 +43628,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43645,14 +43662,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43665,7 +43682,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43681,7 +43698,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43697,7 +43714,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43731,7 +43748,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -43747,7 +43764,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -43765,7 +43782,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -43783,7 +43800,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -43801,13 +43818,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -43818,7 +43835,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -43832,7 +43849,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -43846,7 +43863,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -43860,7 +43877,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -43872,7 +43889,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -43886,7 +43903,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -43900,7 +43917,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -43914,7 +43931,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -43928,7 +43945,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -43942,7 +43959,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -43954,7 +43971,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -43971,7 +43988,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -43983,7 +44000,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -43997,7 +44014,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44014,7 +44031,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44031,13 +44048,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44046,7 +44063,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44060,7 +44077,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44078,7 +44095,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44092,13 +44109,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44109,7 +44126,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44123,7 +44140,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44137,7 +44154,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44151,7 +44168,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44163,7 +44180,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44181,7 +44198,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44195,13 +44212,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44212,7 +44229,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44224,7 +44241,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44238,13 +44255,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44253,7 +44270,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44265,7 +44282,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44279,7 +44296,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44291,7 +44308,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44303,7 +44320,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44315,7 +44332,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44329,13 +44346,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44346,7 +44363,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44360,7 +44377,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44374,7 +44391,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44412,7 +44429,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44426,7 +44443,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44440,7 +44457,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44470,7 +44487,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44484,7 +44501,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44498,7 +44515,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44512,7 +44529,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44526,7 +44543,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44540,7 +44557,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44554,7 +44571,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44568,13 +44585,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44585,7 +44602,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44599,7 +44616,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44614,7 +44631,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44628,7 +44645,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44642,7 +44659,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44656,7 +44673,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44670,7 +44687,7 @@
         <v>2582</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44688,7 +44705,7 @@
         <v>2651</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -44702,7 +44719,7 @@
         <v>2652</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -44716,7 +44733,7 @@
         <v>2739</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44730,7 +44747,7 @@
         <v>2745</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -44744,7 +44761,7 @@
         <v>2769</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45067,7 +45084,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45299,7 +45316,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45316,7 +45333,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45335,7 +45352,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45354,7 +45371,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45374,7 +45391,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45394,7 +45411,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45415,7 +45432,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45435,7 +45452,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45445,10 +45462,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45480,7 +45497,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45500,7 +45517,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45520,7 +45537,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45543,7 +45560,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45563,7 +45580,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45583,19 +45600,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45609,7 +45626,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45627,7 +45644,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45647,7 +45664,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45656,7 +45673,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45670,7 +45687,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45690,7 +45707,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45708,7 +45725,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45728,7 +45745,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45737,10 +45754,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45752,7 +45769,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45772,7 +45789,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45790,7 +45807,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -45873,7 +45890,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -45893,7 +45910,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -45913,7 +45930,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -45923,7 +45940,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -45935,7 +45952,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -45955,7 +45972,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46089,7 +46106,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46103,7 +46120,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46117,7 +46134,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46131,13 +46148,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46148,7 +46165,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46162,7 +46179,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46176,7 +46193,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46372,7 +46389,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46394,13 +46411,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46414,13 +46431,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46431,7 +46448,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46445,7 +46462,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46459,7 +46476,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46473,7 +46490,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46496,7 +46513,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46505,7 +46522,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46556,7 +46573,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46577,14 +46594,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46600,7 +46617,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46635,7 +46652,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46644,7 +46661,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46681,7 +46698,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46702,7 +46719,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46712,7 +46729,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48171,7 +48188,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48186,13 +48203,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48233,7 +48250,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48248,7 +48265,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48308,7 +48325,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48321,7 +48338,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48346,7 +48363,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48359,7 +48376,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48372,7 +48389,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48385,7 +48402,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48400,7 +48417,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48415,7 +48432,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48428,7 +48445,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48443,7 +48460,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2535 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="9"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3419" uniqueCount="1580">
   <si>
     <t>Date</t>
   </si>
@@ -4693,6 +4693,9 @@
   </si>
   <si>
     <t>Find the Pivot Integer</t>
+  </si>
+  <si>
+    <t>Difference Between Element Sum and Digit Sum of an Array</t>
   </si>
   <si>
     <t>Pass the Pillow</t>
@@ -7577,7 +7580,7 @@
   <sheetPr/>
   <dimension ref="A1:AR116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
@@ -43136,10 +43139,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A112" sqref="$A112:$XFD112"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44810,10 +44813,10 @@
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="4">
-        <v>45137</v>
+        <v>45156</v>
       </c>
       <c r="B117" s="12">
-        <v>2582</v>
+        <v>2535</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1497</v>
@@ -44822,30 +44825,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A118" s="4"/>
-      <c r="B118" s="12"/>
-    </row>
-    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A119" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B119" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C119" s="1" t="s">
+    <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A118" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B118" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>1498</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A119" s="4"/>
+      <c r="B119" s="12"/>
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A120" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B120" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1499</v>
@@ -44856,10 +44859,10 @@
     </row>
     <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A121" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B121" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>1500</v>
@@ -44869,11 +44872,11 @@
       </c>
     </row>
     <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A122" s="27">
-        <v>45133</v>
+      <c r="A122" s="4">
+        <v>45131</v>
       </c>
       <c r="B122" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>1501</v>
@@ -44884,10 +44887,10 @@
     </row>
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A123" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B123" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>1502</v>
@@ -44896,9 +44899,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A124" s="11"/>
-      <c r="B124" s="12"/>
+    <row r="124" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A124" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B124" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="125" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A125" s="11"/>
@@ -44907,6 +44920,10 @@
     <row r="126" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A126" s="11"/>
       <c r="B126" s="12"/>
+    </row>
+    <row r="127" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A127" s="11"/>
+      <c r="B127" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -45004,7 +45021,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A127:E1048576 G127:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G128:XFD1048576 A128:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45026,7 +45043,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F127:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F128:F1048576">
     <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -45087,7 +45104,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD126 A113:E126 A107:E111">
+  <conditionalFormatting sqref="G107:XFD111 G113:XFD127 A107:E111 A113:E127">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45109,7 +45126,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F126">
+  <conditionalFormatting sqref="F107:F111 F113:F127">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -45213,7 +45230,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45445,7 +45462,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45462,7 +45479,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45481,7 +45498,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45500,7 +45517,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45520,7 +45537,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45540,7 +45557,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45561,7 +45578,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45581,7 +45598,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45591,10 +45608,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45626,7 +45643,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45646,7 +45663,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45666,7 +45683,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45689,7 +45706,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45709,7 +45726,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45729,19 +45746,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45755,7 +45772,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45773,7 +45790,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45793,7 +45810,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45802,7 +45819,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45816,7 +45833,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45836,7 +45853,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45854,7 +45871,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45874,7 +45891,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45883,10 +45900,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45898,7 +45915,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45918,7 +45935,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -45936,7 +45953,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46019,7 +46036,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46039,7 +46056,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46059,7 +46076,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46069,7 +46086,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46081,7 +46098,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46101,7 +46118,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46235,7 +46252,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46249,7 +46266,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46263,7 +46280,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46277,13 +46294,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46294,7 +46311,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46308,7 +46325,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46322,7 +46339,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46540,13 +46557,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46560,13 +46577,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46577,7 +46594,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46591,7 +46608,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46605,7 +46622,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46619,7 +46636,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46651,7 +46668,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46702,7 +46719,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46723,14 +46740,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46746,7 +46763,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46781,7 +46798,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46790,7 +46807,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46827,7 +46844,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46848,7 +46865,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46858,7 +46875,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48332,13 +48349,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48379,7 +48396,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48394,7 +48411,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48454,7 +48471,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48467,7 +48484,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48492,7 +48509,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48505,7 +48522,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48518,7 +48535,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48531,7 +48548,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48546,7 +48563,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48561,7 +48578,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48574,7 +48591,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48589,7 +48606,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2828 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="9"/>
+    <workbookView windowWidth="17845" windowHeight="10148" tabRatio="991" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3424" uniqueCount="1583">
   <si>
     <t>Date</t>
   </si>
@@ -3696,6 +3696,9 @@
   </si>
   <si>
     <t>Faulty Keyboard</t>
+  </si>
+  <si>
+    <t>Check if a String Is an Acronym of Words</t>
   </si>
   <si>
     <t>Add Two Numbers</t>
@@ -7586,8 +7589,8 @@
   <sheetPr/>
   <dimension ref="A1:AR117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -26769,10 +26772,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I217"/>
+  <dimension ref="A1:I218"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29693,6 +29696,20 @@
         <v>1171</v>
       </c>
       <c r="D217" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="39">
+        <v>45159</v>
+      </c>
+      <c r="B218" s="1">
+        <v>2828</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30536,7 +30553,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30559,7 +30576,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30579,7 +30596,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30599,7 +30616,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30619,7 +30636,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30637,7 +30654,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30655,7 +30672,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30673,7 +30690,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30693,7 +30710,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30711,7 +30728,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30729,7 +30746,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30747,7 +30764,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30765,7 +30782,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -30839,7 +30856,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -30857,7 +30874,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -30877,7 +30894,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -30889,7 +30906,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -30902,7 +30919,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -30922,7 +30939,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -30945,7 +30962,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -30966,7 +30983,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -30987,7 +31004,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31007,7 +31024,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31025,7 +31042,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31043,7 +31060,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31061,7 +31078,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31079,7 +31096,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31115,7 +31132,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31135,7 +31152,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31144,7 +31161,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31155,7 +31172,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31173,7 +31190,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31195,7 +31212,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31204,7 +31221,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31220,7 +31237,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31246,7 +31263,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31261,7 +31278,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31275,7 +31292,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31289,7 +31306,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31301,7 +31318,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31315,7 +31332,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31327,7 +31344,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31339,7 +31356,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31353,7 +31370,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31367,7 +31384,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32668,7 +32685,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32686,7 +32703,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32708,7 +32725,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32728,7 +32745,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32748,7 +32765,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32766,7 +32783,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32784,7 +32801,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32802,7 +32819,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -32818,7 +32835,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34259,7 +34276,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34280,7 +34297,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34298,7 +34315,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34316,7 +34333,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34334,7 +34351,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34355,7 +34372,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34366,7 +34383,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34376,7 +34393,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34397,7 +34414,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34415,7 +34432,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34433,7 +34450,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34451,7 +34468,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34469,7 +34486,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34487,7 +34504,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34507,7 +34524,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34528,7 +34545,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34547,7 +34564,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34568,7 +34585,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34588,7 +34605,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34606,7 +34623,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34626,7 +34643,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34646,7 +34663,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34696,7 +34713,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34716,7 +34733,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34734,7 +34751,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34752,7 +34769,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34770,7 +34787,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34790,7 +34807,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34808,7 +34825,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -34826,7 +34843,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -34844,7 +34861,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -34862,7 +34879,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -34880,7 +34897,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -34898,7 +34915,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -34916,7 +34933,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -34936,7 +34953,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -34954,7 +34971,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -34972,7 +34989,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -34990,7 +35007,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35010,7 +35027,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35030,7 +35047,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35051,7 +35068,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35071,7 +35088,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35089,7 +35106,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35109,7 +35126,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36359,7 +36376,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36377,7 +36394,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36397,7 +36414,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36412,7 +36429,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36427,7 +36444,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36442,7 +36459,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36451,10 +36468,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36466,14 +36483,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36484,7 +36501,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36504,7 +36521,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36522,7 +36539,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36540,7 +36557,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36560,7 +36577,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36580,7 +36597,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36616,7 +36633,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36634,7 +36651,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36652,7 +36669,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36670,7 +36687,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36710,7 +36727,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36728,7 +36745,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36748,7 +36765,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36766,7 +36783,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36789,7 +36806,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36810,7 +36827,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -36829,7 +36846,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -36849,7 +36866,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -36871,7 +36888,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -36907,7 +36924,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -36927,7 +36944,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -36947,7 +36964,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -36965,7 +36982,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -36983,7 +37000,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37001,7 +37018,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37021,7 +37038,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37041,7 +37058,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37061,7 +37078,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37070,10 +37087,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37085,7 +37102,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37103,7 +37120,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37115,7 +37132,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37127,7 +37144,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37142,7 +37159,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37166,7 +37183,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37180,7 +37197,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37192,7 +37209,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37206,7 +37223,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37220,7 +37237,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37232,7 +37249,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37244,7 +37261,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37256,7 +37273,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37268,7 +37285,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37280,7 +37297,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37292,7 +37309,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37304,7 +37321,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37318,7 +37335,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37330,7 +37347,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37342,7 +37359,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37356,7 +37373,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37368,7 +37385,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37380,7 +37397,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37392,7 +37409,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37404,7 +37421,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37455,7 +37472,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37506,7 +37523,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37559,7 +37576,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37612,7 +37629,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37663,7 +37680,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37714,7 +37731,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37765,7 +37782,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -37818,7 +37835,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -37869,7 +37886,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -37922,7 +37939,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -37973,7 +37990,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38024,7 +38041,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38077,7 +38094,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38128,7 +38145,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38181,7 +38198,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38283,7 +38300,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38387,7 +38404,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38545,7 +38562,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38598,7 +38615,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38700,7 +38717,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38753,7 +38770,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38762,7 +38779,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -38862,7 +38879,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -38913,7 +38930,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -38966,7 +38983,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39019,7 +39036,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39123,7 +39140,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39221,7 +39238,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39409,7 +39426,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42408,7 +42425,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42425,7 +42442,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42442,7 +42459,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42459,7 +42476,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42478,7 +42495,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42495,7 +42512,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42512,7 +42529,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42529,7 +42546,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42548,7 +42565,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42565,7 +42582,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42582,7 +42599,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42599,7 +42616,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42616,7 +42633,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42635,7 +42652,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42652,7 +42669,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42669,7 +42686,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43254,14 +43271,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43274,17 +43291,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43294,7 +43311,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43312,7 +43329,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43328,7 +43345,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43344,7 +43361,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43360,7 +43377,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43376,7 +43393,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43394,17 +43411,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43414,7 +43431,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43432,17 +43449,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43454,17 +43471,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43476,7 +43493,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43484,7 +43501,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43494,7 +43511,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43511,7 +43528,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43528,7 +43545,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43547,7 +43564,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43565,14 +43582,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43585,14 +43602,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43603,7 +43620,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43619,14 +43636,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43637,7 +43654,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43655,7 +43672,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43664,7 +43681,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43675,7 +43692,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43691,7 +43708,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43707,7 +43724,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43723,7 +43740,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43739,7 +43756,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43757,7 +43774,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43773,7 +43790,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43789,7 +43806,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43805,7 +43822,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43821,7 +43838,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43855,14 +43872,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43875,7 +43892,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43891,7 +43908,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43907,7 +43924,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43941,7 +43958,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -43957,7 +43974,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -43975,7 +43992,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -43993,7 +44010,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44011,13 +44028,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44028,7 +44045,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44042,7 +44059,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44056,7 +44073,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44070,7 +44087,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44082,7 +44099,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44096,7 +44113,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44110,7 +44127,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44124,7 +44141,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44138,7 +44155,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44152,7 +44169,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44164,7 +44181,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44181,7 +44198,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44193,7 +44210,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44207,7 +44224,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44224,7 +44241,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44241,13 +44258,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44256,7 +44273,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44270,7 +44287,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44288,7 +44305,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44302,13 +44319,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44319,7 +44336,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44333,7 +44350,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44347,7 +44364,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44361,7 +44378,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44373,7 +44390,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44391,7 +44408,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44405,13 +44422,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44422,7 +44439,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44434,7 +44451,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44448,13 +44465,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44463,7 +44480,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44475,7 +44492,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44489,7 +44506,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44501,7 +44518,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44513,7 +44530,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44525,7 +44542,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44539,13 +44556,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44556,7 +44573,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44570,7 +44587,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44584,7 +44601,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44622,7 +44639,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44636,7 +44653,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44650,7 +44667,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44680,7 +44697,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44694,7 +44711,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44708,7 +44725,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44722,7 +44739,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44736,7 +44753,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44750,7 +44767,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44764,7 +44781,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44778,13 +44795,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44795,7 +44812,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44809,7 +44826,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44824,7 +44841,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44838,7 +44855,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44852,7 +44869,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44866,7 +44883,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44880,7 +44897,7 @@
         <v>2535</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44894,7 +44911,7 @@
         <v>2582</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -44912,7 +44929,7 @@
         <v>2651</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -44926,7 +44943,7 @@
         <v>2652</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44940,7 +44957,7 @@
         <v>2739</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -44954,7 +44971,7 @@
         <v>2745</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -44968,7 +44985,7 @@
         <v>2769</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45291,7 +45308,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45523,7 +45540,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45540,7 +45557,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45559,7 +45576,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45578,7 +45595,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45598,7 +45615,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45618,7 +45635,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45639,7 +45656,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45659,7 +45676,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45669,10 +45686,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45704,7 +45721,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45724,7 +45741,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45744,7 +45761,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45767,7 +45784,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45787,7 +45804,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45807,19 +45824,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45833,7 +45850,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45851,7 +45868,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45871,7 +45888,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45880,7 +45897,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45894,7 +45911,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45914,7 +45931,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45932,7 +45949,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -45952,7 +45969,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -45961,10 +45978,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -45976,7 +45993,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -45996,7 +46013,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46014,7 +46031,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46097,7 +46114,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46117,7 +46134,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46137,7 +46154,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46147,7 +46164,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46159,7 +46176,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46179,7 +46196,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46313,7 +46330,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46327,7 +46344,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46341,7 +46358,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46355,13 +46372,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46372,7 +46389,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46386,7 +46403,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46400,7 +46417,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46596,7 +46613,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46618,13 +46635,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46638,13 +46655,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46655,7 +46672,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46669,7 +46686,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46683,7 +46700,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46697,7 +46714,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46720,7 +46737,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46729,7 +46746,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46780,7 +46797,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46801,14 +46818,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46824,7 +46841,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46859,7 +46876,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46868,7 +46885,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46905,7 +46922,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46926,7 +46943,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46936,7 +46953,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48395,7 +48412,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48410,13 +48427,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48457,7 +48474,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48472,7 +48489,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48532,7 +48549,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48545,7 +48562,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48570,7 +48587,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48583,7 +48600,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48596,7 +48613,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48609,7 +48626,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48624,7 +48641,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48639,7 +48656,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48652,7 +48669,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48667,7 +48684,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2520 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="8" activeTab="13"/>
+    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3428" uniqueCount="1585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1586">
   <si>
     <t>Date</t>
   </si>
@@ -4708,6 +4708,9 @@
   </si>
   <si>
     <t>Find the Pivot Integer</t>
+  </si>
+  <si>
+    <t>Count the Digits That Divide a Number</t>
   </si>
   <si>
     <t>Difference Between Element Sum and Digit Sum of an Array</t>
@@ -15212,7 +15215,7 @@
   <sheetPr/>
   <dimension ref="A1:AV284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+    <sheetView topLeftCell="A267" workbookViewId="0">
       <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
@@ -43250,9 +43253,9 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
       <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
@@ -44924,10 +44927,10 @@
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="4">
-        <v>45156</v>
+        <v>45160</v>
       </c>
       <c r="B117" s="12">
-        <v>2535</v>
+        <v>2520</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1502</v>
@@ -44938,10 +44941,10 @@
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="4">
-        <v>45137</v>
+        <v>45156</v>
       </c>
       <c r="B118" s="12">
-        <v>2582</v>
+        <v>2535</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1503</v>
@@ -44950,30 +44953,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A119" s="4"/>
-      <c r="B119" s="12"/>
-    </row>
-    <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A120" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B120" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C120" s="1" t="s">
+    <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A119" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B119" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>1504</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="120" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="12"/>
     </row>
     <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A121" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B121" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>1505</v>
@@ -44984,10 +44987,10 @@
     </row>
     <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A122" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B122" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>1506</v>
@@ -44997,11 +45000,11 @@
       </c>
     </row>
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A123" s="27">
-        <v>45133</v>
+      <c r="A123" s="4">
+        <v>45131</v>
       </c>
       <c r="B123" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>1507</v>
@@ -45012,10 +45015,10 @@
     </row>
     <row r="124" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A124" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B124" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>1508</v>
@@ -45024,9 +45027,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A125" s="11"/>
-      <c r="B125" s="12"/>
+    <row r="125" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A125" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B125" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="126" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A126" s="11"/>
@@ -45035,6 +45048,10 @@
     <row r="127" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A127" s="11"/>
       <c r="B127" s="12"/>
+    </row>
+    <row r="128" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A128" s="11"/>
+      <c r="B128" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -45132,7 +45149,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G128:XFD1048576 A128:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A129:E1048576 G129:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45154,7 +45171,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F128:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F129:F1048576">
     <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -45215,7 +45232,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD127 A107:E111 A113:E127">
+  <conditionalFormatting sqref="G107:XFD111 G113:XFD128 A113:E128 A107:E111">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45237,7 +45254,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F127">
+  <conditionalFormatting sqref="F107:F111 F113:F128">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -45341,7 +45358,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45573,7 +45590,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45590,7 +45607,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45609,7 +45626,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45628,7 +45645,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45648,7 +45665,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45668,7 +45685,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45689,7 +45706,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45709,7 +45726,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45719,10 +45736,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45754,7 +45771,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45774,7 +45791,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45794,7 +45811,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45817,7 +45834,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45837,7 +45854,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45857,19 +45874,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45883,7 +45900,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45901,7 +45918,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45921,7 +45938,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45930,7 +45947,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45944,7 +45961,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45964,7 +45981,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45982,7 +45999,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46002,7 +46019,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46011,10 +46028,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46026,7 +46043,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46046,7 +46063,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46064,7 +46081,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46147,7 +46164,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46167,7 +46184,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46187,7 +46204,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46197,7 +46214,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46209,7 +46226,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46229,7 +46246,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46363,7 +46380,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46377,7 +46394,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46391,7 +46408,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46405,13 +46422,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46422,7 +46439,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46436,7 +46453,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46450,7 +46467,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46668,13 +46685,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46688,13 +46705,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46705,7 +46722,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46719,7 +46736,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46733,7 +46750,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46747,7 +46764,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46779,7 +46796,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46830,7 +46847,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46851,14 +46868,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46874,7 +46891,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46909,7 +46926,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46918,7 +46935,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46955,7 +46972,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46976,7 +46993,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -46986,7 +47003,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48460,13 +48477,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48507,7 +48524,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48522,7 +48539,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48582,7 +48599,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48595,7 +48612,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48620,7 +48637,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48633,7 +48650,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48646,7 +48663,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48659,7 +48676,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48674,7 +48691,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48689,7 +48706,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48702,7 +48719,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48717,7 +48734,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2586 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="20"/>
+    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="1586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="1587">
   <si>
     <t>Date</t>
   </si>
@@ -3681,6 +3681,9 @@
   </si>
   <si>
     <t>Maximum Value of a String in an Array</t>
+  </si>
+  <si>
+    <t>Count the Number of Vowel Strings in Range</t>
   </si>
   <si>
     <t>Number of Senior Citizens</t>
@@ -26808,10 +26811,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I218"/>
+  <dimension ref="A1:I219"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A211" sqref="A211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29639,10 +29642,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45135</v>
+        <v>45160</v>
       </c>
       <c r="B211" s="1">
-        <v>2678</v>
+        <v>2586</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1167</v>
@@ -29653,10 +29656,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45140</v>
+        <v>45135</v>
       </c>
       <c r="B212" s="1">
-        <v>2697</v>
+        <v>2678</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>1168</v>
@@ -29667,10 +29670,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B213" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>1169</v>
@@ -29681,10 +29684,10 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B214" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>1170</v>
@@ -29695,40 +29698,40 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B215" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>1171</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B216" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C216" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>1172</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="39">
-        <v>45144</v>
+        <v>45131</v>
       </c>
       <c r="B217" s="1">
-        <v>2810</v>
-      </c>
-      <c r="C217" s="1" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C217" s="16" t="s">
         <v>1173</v>
       </c>
       <c r="D217" s="1" t="s">
@@ -29737,15 +29740,29 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="39">
-        <v>45159</v>
+        <v>45144</v>
       </c>
       <c r="B218" s="1">
-        <v>2828</v>
+        <v>2810</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>1174</v>
       </c>
       <c r="D218" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="39">
+        <v>45159</v>
+      </c>
+      <c r="B219" s="1">
+        <v>2828</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30038,12 +30055,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F215">
+  <conditionalFormatting sqref="F216">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F215)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -30074,7 +30091,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D216">
+  <conditionalFormatting sqref="D217">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30096,12 +30113,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F216">
+  <conditionalFormatting sqref="F217">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -30132,12 +30149,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F217">
+  <conditionalFormatting sqref="F218">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -30168,7 +30185,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A214">
+  <conditionalFormatting sqref="A209:A215">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30202,7 +30219,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209:F214">
+  <conditionalFormatting sqref="F209:F215">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
@@ -30238,7 +30255,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 G218:XFD1048576 A218:E1048576">
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 A219:E1048576 G219:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30260,7 +30277,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F218:F1048576">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F219:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30428,7 +30445,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:XFD214 B209:E214">
+  <conditionalFormatting sqref="G209:XFD215 B209:E215">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30450,7 +30467,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G215:XFD215 A215:E215">
+  <conditionalFormatting sqref="G216:XFD216 A216:E216">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30472,7 +30489,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G216:XFD216 E216 A216:C216">
+  <conditionalFormatting sqref="G217:XFD217 A217:C217 E217">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30494,7 +30511,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G217:XFD217 A217:E217">
+  <conditionalFormatting sqref="G218:XFD218 A218:E218">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30589,7 +30606,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30612,7 +30629,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30632,7 +30649,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30652,7 +30669,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30672,7 +30689,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30690,7 +30707,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30708,7 +30725,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30726,7 +30743,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30746,7 +30763,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30764,7 +30781,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30782,7 +30799,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30800,7 +30817,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30818,7 +30835,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -30892,7 +30909,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -30910,7 +30927,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -30930,7 +30947,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -30942,7 +30959,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -30955,7 +30972,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -30975,7 +30992,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -30998,7 +31015,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31019,7 +31036,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31040,7 +31057,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31060,7 +31077,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31078,7 +31095,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31096,7 +31113,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31114,7 +31131,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31132,7 +31149,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31168,7 +31185,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31188,7 +31205,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31197,7 +31214,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31208,7 +31225,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31226,7 +31243,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31248,7 +31265,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31257,7 +31274,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31273,7 +31290,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31299,7 +31316,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31314,7 +31331,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31328,7 +31345,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31342,7 +31359,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31354,7 +31371,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31368,7 +31385,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31380,7 +31397,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31392,7 +31409,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31406,7 +31423,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31420,7 +31437,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32721,7 +32738,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32739,7 +32756,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32761,7 +32778,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32781,7 +32798,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32801,7 +32818,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32819,7 +32836,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32837,7 +32854,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32855,7 +32872,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -32871,7 +32888,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34312,7 +34329,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34333,7 +34350,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34351,7 +34368,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34369,7 +34386,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34387,7 +34404,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34408,7 +34425,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34419,7 +34436,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34429,7 +34446,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34450,7 +34467,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34468,7 +34485,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34486,7 +34503,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34504,7 +34521,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34522,7 +34539,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34540,7 +34557,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34560,7 +34577,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34581,7 +34598,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34600,7 +34617,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34621,7 +34638,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34641,7 +34658,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34659,7 +34676,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34679,7 +34696,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34699,7 +34716,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34749,7 +34766,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34769,7 +34786,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34787,7 +34804,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34805,7 +34822,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34823,7 +34840,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34843,7 +34860,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34861,7 +34878,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -34879,7 +34896,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -34897,7 +34914,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -34915,7 +34932,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -34933,7 +34950,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -34951,7 +34968,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -34969,7 +34986,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -34989,7 +35006,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35007,7 +35024,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35025,7 +35042,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35043,7 +35060,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35063,7 +35080,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35083,7 +35100,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35104,7 +35121,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35124,7 +35141,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35142,7 +35159,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35162,7 +35179,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36412,7 +36429,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36430,7 +36447,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36450,7 +36467,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36465,7 +36482,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36480,7 +36497,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36495,7 +36512,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36504,10 +36521,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36519,14 +36536,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36537,7 +36554,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36557,7 +36574,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36575,7 +36592,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36593,7 +36610,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36613,7 +36630,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36633,7 +36650,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36669,7 +36686,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36687,7 +36704,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36705,7 +36722,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36723,7 +36740,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36763,7 +36780,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36781,7 +36798,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36801,7 +36818,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36819,7 +36836,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36842,7 +36859,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36863,7 +36880,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -36882,7 +36899,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -36902,7 +36919,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -36924,7 +36941,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -36960,7 +36977,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -36980,7 +36997,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37000,7 +37017,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37018,7 +37035,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37036,7 +37053,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37054,7 +37071,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37074,7 +37091,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37094,7 +37111,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37114,7 +37131,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37123,10 +37140,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37138,7 +37155,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37156,7 +37173,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37168,7 +37185,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37180,7 +37197,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37195,7 +37212,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37219,7 +37236,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37233,7 +37250,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37245,7 +37262,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37259,7 +37276,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37273,7 +37290,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37285,7 +37302,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37297,7 +37314,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37309,7 +37326,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37321,7 +37338,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37333,7 +37350,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37345,7 +37362,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37357,7 +37374,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37371,7 +37388,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37383,7 +37400,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37395,7 +37412,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37409,7 +37426,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37421,7 +37438,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37433,7 +37450,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37445,7 +37462,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37457,7 +37474,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37508,7 +37525,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37559,7 +37576,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37612,7 +37629,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37665,7 +37682,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37716,7 +37733,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37767,7 +37784,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37818,7 +37835,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -37871,7 +37888,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -37922,7 +37939,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -37975,7 +37992,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38026,7 +38043,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38077,7 +38094,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38130,7 +38147,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38181,7 +38198,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38234,7 +38251,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38336,7 +38353,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38440,7 +38457,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38598,7 +38615,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38651,7 +38668,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38753,7 +38770,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38806,7 +38823,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38815,7 +38832,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -38915,7 +38932,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -38966,7 +38983,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39019,7 +39036,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39072,7 +39089,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39176,7 +39193,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39274,7 +39291,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39462,7 +39479,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42461,7 +42478,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42478,7 +42495,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42495,7 +42512,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42512,7 +42529,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42531,7 +42548,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42548,7 +42565,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42565,7 +42582,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42582,7 +42599,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42601,7 +42618,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42618,7 +42635,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42635,7 +42652,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42652,7 +42669,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42669,7 +42686,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42688,7 +42705,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42705,7 +42722,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42722,7 +42739,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43255,7 +43272,7 @@
   <sheetPr/>
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
@@ -43307,14 +43324,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43327,17 +43344,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43347,7 +43364,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43365,7 +43382,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43381,7 +43398,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43397,7 +43414,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43413,7 +43430,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43429,7 +43446,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43447,17 +43464,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43467,7 +43484,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43485,17 +43502,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43507,17 +43524,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43529,7 +43546,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43537,7 +43554,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43547,7 +43564,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43564,7 +43581,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43581,7 +43598,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43600,7 +43617,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43618,14 +43635,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43638,14 +43655,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43656,7 +43673,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43672,14 +43689,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43690,7 +43707,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43708,7 +43725,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43717,7 +43734,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43728,7 +43745,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43744,7 +43761,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43760,7 +43777,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43776,7 +43793,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43792,7 +43809,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43810,7 +43827,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43826,7 +43843,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43842,7 +43859,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43858,7 +43875,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -43874,7 +43891,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -43908,14 +43925,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -43928,7 +43945,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -43944,7 +43961,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -43960,7 +43977,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -43994,7 +44011,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44010,7 +44027,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44028,7 +44045,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44046,7 +44063,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44064,13 +44081,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44081,7 +44098,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44095,7 +44112,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44109,7 +44126,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44123,7 +44140,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44135,7 +44152,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44149,7 +44166,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44163,7 +44180,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44177,7 +44194,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44191,7 +44208,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44205,7 +44222,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44217,7 +44234,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44234,7 +44251,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44246,7 +44263,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44260,7 +44277,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44277,7 +44294,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44294,13 +44311,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44309,7 +44326,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44323,7 +44340,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44341,7 +44358,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44355,13 +44372,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44372,7 +44389,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44386,7 +44403,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44400,7 +44417,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44414,7 +44431,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44426,7 +44443,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44444,7 +44461,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44458,13 +44475,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44475,7 +44492,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44487,7 +44504,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44501,13 +44518,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44516,7 +44533,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44528,7 +44545,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44542,7 +44559,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44554,7 +44571,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44566,7 +44583,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44578,7 +44595,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44592,13 +44609,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44609,7 +44626,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44623,7 +44640,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44637,7 +44654,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44675,7 +44692,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44689,7 +44706,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44703,7 +44720,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44733,7 +44750,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44747,7 +44764,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44761,7 +44778,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44775,7 +44792,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44789,7 +44806,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44803,7 +44820,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44817,7 +44834,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44831,13 +44848,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44848,7 +44865,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44862,7 +44879,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -44877,7 +44894,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -44891,7 +44908,7 @@
         <v>2469</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -44905,7 +44922,7 @@
         <v>2475</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -44919,7 +44936,7 @@
         <v>2485</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -44933,7 +44950,7 @@
         <v>2520</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -44947,7 +44964,7 @@
         <v>2535</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -44961,7 +44978,7 @@
         <v>2582</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -44979,7 +44996,7 @@
         <v>2651</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -44993,7 +45010,7 @@
         <v>2652</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -45007,7 +45024,7 @@
         <v>2739</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45021,7 +45038,7 @@
         <v>2745</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45035,7 +45052,7 @@
         <v>2769</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45358,7 +45375,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45590,7 +45607,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45607,7 +45624,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45626,7 +45643,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45645,7 +45662,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45665,7 +45682,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45685,7 +45702,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45706,7 +45723,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45726,7 +45743,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45736,10 +45753,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45771,7 +45788,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45791,7 +45808,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45811,7 +45828,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45834,7 +45851,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45854,7 +45871,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45874,19 +45891,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45900,7 +45917,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45918,7 +45935,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -45938,7 +45955,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -45947,7 +45964,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -45961,7 +45978,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -45981,7 +45998,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -45999,7 +46016,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46019,7 +46036,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46028,10 +46045,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46043,7 +46060,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46063,7 +46080,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46081,7 +46098,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46164,7 +46181,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46184,7 +46201,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46204,7 +46221,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46214,7 +46231,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46226,7 +46243,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46246,7 +46263,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46380,7 +46397,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46394,7 +46411,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46408,7 +46425,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46422,13 +46439,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46439,7 +46456,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46453,7 +46470,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46467,7 +46484,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46663,7 +46680,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46685,13 +46702,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46705,13 +46722,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46722,7 +46739,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46736,7 +46753,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46750,7 +46767,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46764,7 +46781,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46787,7 +46804,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46796,7 +46813,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46847,7 +46864,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46868,14 +46885,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46891,7 +46908,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46926,7 +46943,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -46935,7 +46952,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -46972,7 +46989,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46993,7 +47010,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47003,7 +47020,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48462,7 +48479,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48477,13 +48494,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48524,7 +48541,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48539,7 +48556,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48599,7 +48616,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48612,7 +48629,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48637,7 +48654,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48650,7 +48667,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48663,7 +48680,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48676,7 +48693,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48691,7 +48708,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48706,7 +48723,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48719,7 +48736,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48734,7 +48751,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2544 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="11"/>
+    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="1588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3436" uniqueCount="1589">
   <si>
     <t>Date</t>
   </si>
@@ -4720,6 +4720,9 @@
   </si>
   <si>
     <t>Difference Between Element Sum and Digit Sum of an Array</t>
+  </si>
+  <si>
+    <t>Alternating Digit Sum</t>
   </si>
   <si>
     <t>Pass the Pillow</t>
@@ -12965,7 +12968,7 @@
   <sheetPr/>
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A38" sqref="$A38:$XFD38"/>
     </sheetView>
   </sheetViews>
@@ -43323,10 +43326,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -45025,10 +45028,10 @@
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A119" s="4">
-        <v>45137</v>
+        <v>45163</v>
       </c>
       <c r="B119" s="12">
-        <v>2582</v>
+        <v>2544</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>1506</v>
@@ -45037,30 +45040,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A120" s="4"/>
-      <c r="B120" s="12"/>
-    </row>
-    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A121" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B121" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C121" s="1" t="s">
+    <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A120" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B120" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>1507</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A121" s="4"/>
+      <c r="B121" s="12"/>
     </row>
     <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A122" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B122" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>1508</v>
@@ -45071,10 +45074,10 @@
     </row>
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A123" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B123" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>1509</v>
@@ -45084,11 +45087,11 @@
       </c>
     </row>
     <row r="124" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A124" s="27">
-        <v>45133</v>
+      <c r="A124" s="4">
+        <v>45131</v>
       </c>
       <c r="B124" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>1510</v>
@@ -45099,10 +45102,10 @@
     </row>
     <row r="125" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A125" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B125" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>1511</v>
@@ -45111,9 +45114,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A126" s="11"/>
-      <c r="B126" s="12"/>
+    <row r="126" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A126" s="27">
+        <v>45143</v>
+      </c>
+      <c r="B126" s="12">
+        <v>2769</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="127" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A127" s="11"/>
@@ -45122,6 +45135,10 @@
     <row r="128" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A128" s="11"/>
       <c r="B128" s="12"/>
+    </row>
+    <row r="129" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A129" s="11"/>
+      <c r="B129" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -45219,7 +45236,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A129:E1048576 G129:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G130:XFD1048576 A130:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45241,7 +45258,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F129:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F130:F1048576">
     <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -45302,7 +45319,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD128 A113:E128 A107:E111">
+  <conditionalFormatting sqref="G107:XFD111 G113:XFD129 A107:E111 A113:E129">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45324,7 +45341,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F128">
+  <conditionalFormatting sqref="F107:F111 F113:F129">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -45428,7 +45445,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45660,7 +45677,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45677,7 +45694,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45696,7 +45713,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45715,7 +45732,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45735,7 +45752,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45755,7 +45772,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45776,7 +45793,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45796,7 +45813,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45806,10 +45823,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45841,7 +45858,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45861,7 +45878,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45881,7 +45898,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45904,7 +45921,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45924,7 +45941,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45944,19 +45961,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45970,7 +45987,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -45988,7 +46005,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46008,7 +46025,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46017,7 +46034,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46031,7 +46048,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46051,7 +46068,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46069,7 +46086,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46089,7 +46106,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46098,10 +46115,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46113,7 +46130,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46133,7 +46150,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46151,7 +46168,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46234,7 +46251,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46254,7 +46271,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46274,7 +46291,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46284,7 +46301,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46296,7 +46313,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46316,7 +46333,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46450,7 +46467,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46464,7 +46481,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46478,7 +46495,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46492,13 +46509,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46509,7 +46526,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46523,7 +46540,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46537,7 +46554,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46755,13 +46772,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46775,13 +46792,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46792,7 +46809,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46806,7 +46823,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46820,7 +46837,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46834,7 +46851,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46866,7 +46883,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46917,7 +46934,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46938,14 +46955,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46961,7 +46978,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -46996,7 +47013,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47005,7 +47022,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47042,7 +47059,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47063,7 +47080,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47073,7 +47090,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48547,13 +48564,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48594,7 +48611,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48609,7 +48626,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48669,7 +48686,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48682,7 +48699,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48707,7 +48724,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48720,7 +48737,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48733,7 +48750,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48746,7 +48763,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48761,7 +48778,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48776,7 +48793,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48789,7 +48806,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48804,7 +48821,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2806 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5048" tabRatio="991" firstSheet="9" activeTab="20"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="9" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3436" uniqueCount="1589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3438" uniqueCount="1590">
   <si>
     <t>Date</t>
   </si>
@@ -4743,6 +4743,9 @@
     <t>Find the Maximum Achievable Number</t>
   </si>
   <si>
+    <t>Account Balance After Rounded Purchase</t>
+  </si>
+  <si>
     <t>Print in Order</t>
   </si>
   <si>
@@ -4974,7 +4977,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -43328,8 +43331,8 @@
   <sheetPr/>
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -45128,9 +45131,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A127" s="11"/>
-      <c r="B127" s="12"/>
+    <row r="127" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A127" s="27">
+        <v>45167</v>
+      </c>
+      <c r="B127" s="12">
+        <v>2806</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="128" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A128" s="11"/>
@@ -45445,7 +45458,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45677,7 +45690,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45694,7 +45707,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45713,7 +45726,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45732,7 +45745,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45752,7 +45765,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45772,7 +45785,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45793,7 +45806,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45813,7 +45826,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45823,10 +45836,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45858,7 +45871,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45878,7 +45891,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45898,7 +45911,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45921,7 +45934,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45941,7 +45954,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45961,19 +45974,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -45987,7 +46000,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46005,7 +46018,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46025,7 +46038,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46034,7 +46047,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46048,7 +46061,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46068,7 +46081,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46086,7 +46099,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46106,7 +46119,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46115,10 +46128,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46130,7 +46143,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46150,7 +46163,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46168,7 +46181,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46251,7 +46264,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46271,7 +46284,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46291,7 +46304,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46301,7 +46314,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46313,7 +46326,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46333,7 +46346,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46467,7 +46480,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46481,7 +46494,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46495,7 +46508,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46509,13 +46522,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46526,7 +46539,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46540,7 +46553,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46554,7 +46567,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46772,13 +46785,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46792,13 +46805,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46809,7 +46822,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46823,7 +46836,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46837,7 +46850,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46851,7 +46864,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46883,7 +46896,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46934,7 +46947,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46955,14 +46968,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -46978,7 +46991,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47013,7 +47026,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47022,7 +47035,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47059,7 +47072,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47080,7 +47093,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47090,7 +47103,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48564,13 +48577,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48611,7 +48624,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48626,7 +48639,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48686,7 +48699,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48699,7 +48712,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48724,7 +48737,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48737,7 +48750,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48750,7 +48763,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48763,7 +48776,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48778,7 +48791,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48793,7 +48806,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48806,7 +48819,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48821,7 +48834,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2455 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="9" activeTab="11"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="1591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3442" uniqueCount="1592">
   <si>
     <t>Date</t>
   </si>
@@ -4708,6 +4708,9 @@
   </si>
   <si>
     <t>Smallest Even Multiple</t>
+  </si>
+  <si>
+    <t>Average Value of Even Numbers That Are Divisible by Three</t>
   </si>
   <si>
     <t>Convert the Temperature</t>
@@ -12974,7 +12977,7 @@
   <sheetPr/>
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -43352,10 +43355,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -44984,10 +44987,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45141</v>
+        <v>45167</v>
       </c>
       <c r="B114" s="12">
-        <v>2469</v>
+        <v>2455</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1502</v>
@@ -45001,7 +45004,7 @@
         <v>45141</v>
       </c>
       <c r="B115" s="12">
-        <v>2475</v>
+        <v>2469</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1503</v>
@@ -45012,10 +45015,10 @@
     </row>
     <row r="116" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A116" s="4">
-        <v>45148</v>
+        <v>45141</v>
       </c>
       <c r="B116" s="12">
-        <v>2485</v>
+        <v>2475</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>1504</v>
@@ -45026,10 +45029,10 @@
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="4">
-        <v>45160</v>
+        <v>45148</v>
       </c>
       <c r="B117" s="12">
-        <v>2520</v>
+        <v>2485</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1505</v>
@@ -45040,10 +45043,10 @@
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="4">
-        <v>45156</v>
+        <v>45160</v>
       </c>
       <c r="B118" s="12">
-        <v>2535</v>
+        <v>2520</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1506</v>
@@ -45054,10 +45057,10 @@
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A119" s="4">
-        <v>45163</v>
+        <v>45156</v>
       </c>
       <c r="B119" s="12">
-        <v>2544</v>
+        <v>2535</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>1507</v>
@@ -45068,10 +45071,10 @@
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A120" s="4">
-        <v>45137</v>
+        <v>45163</v>
       </c>
       <c r="B120" s="12">
-        <v>2582</v>
+        <v>2544</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1508</v>
@@ -45080,30 +45083,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="12"/>
-    </row>
-    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A122" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B122" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C122" s="1" t="s">
+    <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A121" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B121" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>1509</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="12"/>
     </row>
     <row r="123" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A123" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B123" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>1510</v>
@@ -45114,10 +45117,10 @@
     </row>
     <row r="124" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A124" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B124" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>1511</v>
@@ -45127,11 +45130,11 @@
       </c>
     </row>
     <row r="125" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A125" s="27">
-        <v>45133</v>
+      <c r="A125" s="4">
+        <v>45131</v>
       </c>
       <c r="B125" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>1512</v>
@@ -45142,10 +45145,10 @@
     </row>
     <row r="126" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A126" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B126" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>1513</v>
@@ -45156,10 +45159,10 @@
     </row>
     <row r="127" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A127" s="27">
-        <v>45167</v>
+        <v>45143</v>
       </c>
       <c r="B127" s="12">
-        <v>2806</v>
+        <v>2769</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>1514</v>
@@ -45168,13 +45171,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A128" s="11"/>
-      <c r="B128" s="12"/>
+    <row r="128" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A128" s="27">
+        <v>45167</v>
+      </c>
+      <c r="B128" s="12">
+        <v>2806</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="129" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A129" s="11"/>
       <c r="B129" s="12"/>
+    </row>
+    <row r="130" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A130" s="11"/>
+      <c r="B130" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -45272,7 +45289,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G130:XFD1048576 A130:E1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A131:E1048576 G131:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45294,7 +45311,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F130:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F131:F1048576">
     <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -45355,7 +45372,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD129 A107:E111 A113:E129">
+  <conditionalFormatting sqref="G107:XFD111 G113:XFD130 A113:E130 A107:E111">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45377,7 +45394,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F129">
+  <conditionalFormatting sqref="F107:F111 F113:F130">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -45481,7 +45498,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45713,7 +45730,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45730,7 +45747,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45749,7 +45766,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45768,7 +45785,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45788,7 +45805,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45808,7 +45825,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45829,7 +45846,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45849,7 +45866,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45859,10 +45876,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45894,7 +45911,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45914,7 +45931,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45934,7 +45951,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -45957,7 +45974,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -45977,7 +45994,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -45997,19 +46014,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46023,7 +46040,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46041,7 +46058,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46061,7 +46078,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46070,7 +46087,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46084,7 +46101,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46104,7 +46121,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46122,7 +46139,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46142,7 +46159,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46151,10 +46168,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46166,7 +46183,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46186,7 +46203,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46204,7 +46221,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46287,7 +46304,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46307,7 +46324,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46327,7 +46344,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46337,7 +46354,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46349,7 +46366,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46369,7 +46386,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46503,7 +46520,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46517,7 +46534,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46531,7 +46548,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46545,13 +46562,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46562,7 +46579,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46576,7 +46593,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46590,7 +46607,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46808,13 +46825,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46828,13 +46845,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46845,7 +46862,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46859,7 +46876,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46873,7 +46890,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46887,7 +46904,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46919,7 +46936,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -46970,7 +46987,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46991,14 +47008,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47014,7 +47031,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47049,7 +47066,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47058,7 +47075,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47095,7 +47112,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47116,7 +47133,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47126,7 +47143,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48600,13 +48617,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48647,7 +48664,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48662,7 +48679,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48722,7 +48739,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48735,7 +48752,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48760,7 +48777,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48773,7 +48790,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48786,7 +48803,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48799,7 +48816,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48814,7 +48831,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48829,7 +48846,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48842,7 +48859,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48857,7 +48874,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2490 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="13"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="1594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="1595">
   <si>
     <t>Date</t>
   </si>
@@ -3690,6 +3690,9 @@
   </si>
   <si>
     <t>Remove Letter To Equalize Frequency</t>
+  </si>
+  <si>
+    <t>Circular Sentence</t>
   </si>
   <si>
     <t>Maximum Value of a String in an Array</t>
@@ -15309,7 +15312,7 @@
   <sheetPr/>
   <dimension ref="A1:AV286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+    <sheetView topLeftCell="A273" workbookViewId="0">
       <selection activeCell="B285" sqref="B285"/>
     </sheetView>
   </sheetViews>
@@ -26930,10 +26933,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I219"/>
+  <dimension ref="A1:I220"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="B220" sqref="B220"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29747,10 +29750,10 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
-        <v>45150</v>
+        <v>45169</v>
       </c>
       <c r="B210" s="1">
-        <v>2496</v>
+        <v>2490</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1170</v>
@@ -29761,10 +29764,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45160</v>
+        <v>45150</v>
       </c>
       <c r="B211" s="1">
-        <v>2586</v>
+        <v>2496</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1171</v>
@@ -29775,10 +29778,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45135</v>
+        <v>45160</v>
       </c>
       <c r="B212" s="1">
-        <v>2678</v>
+        <v>2586</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>1172</v>
@@ -29789,10 +29792,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
-        <v>45140</v>
+        <v>45135</v>
       </c>
       <c r="B213" s="1">
-        <v>2697</v>
+        <v>2678</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>1173</v>
@@ -29803,10 +29806,10 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B214" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>1174</v>
@@ -29817,10 +29820,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B215" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>1175</v>
@@ -29831,40 +29834,40 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B216" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>1176</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B217" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C217" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C217" s="1" t="s">
         <v>1177</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="39">
-        <v>45144</v>
+        <v>45131</v>
       </c>
       <c r="B218" s="1">
-        <v>2810</v>
-      </c>
-      <c r="C218" s="1" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C218" s="16" t="s">
         <v>1178</v>
       </c>
       <c r="D218" s="1" t="s">
@@ -29873,15 +29876,29 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="39">
-        <v>45159</v>
+        <v>45144</v>
       </c>
       <c r="B219" s="1">
-        <v>2828</v>
+        <v>2810</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>1179</v>
       </c>
       <c r="D219" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="39">
+        <v>45159</v>
+      </c>
+      <c r="B220" s="1">
+        <v>2828</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30174,12 +30191,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F216">
+  <conditionalFormatting sqref="F217">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F216)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -30210,7 +30227,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D217">
+  <conditionalFormatting sqref="D218">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30232,12 +30249,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F217">
+  <conditionalFormatting sqref="F218">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -30268,12 +30285,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F218">
+  <conditionalFormatting sqref="F219">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -30304,7 +30321,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A215">
+  <conditionalFormatting sqref="A209:A216">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30338,7 +30355,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209:F215">
+  <conditionalFormatting sqref="F209:F216">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
@@ -30374,7 +30391,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 A219:E1048576 G219:XFD1048576">
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 G220:XFD1048576 A220:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30396,7 +30413,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F219:F1048576">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F220:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30564,7 +30581,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:XFD215 B209:E215">
+  <conditionalFormatting sqref="G209:XFD216 B209:E216">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30586,7 +30603,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G216:XFD216 A216:E216">
+  <conditionalFormatting sqref="G217:XFD217 A217:E217">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30608,7 +30625,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G217:XFD217 A217:C217 E217">
+  <conditionalFormatting sqref="G218:XFD218 E218 A218:C218">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30630,7 +30647,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G218:XFD218 A218:E218">
+  <conditionalFormatting sqref="G219:XFD219 A219:E219">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30725,7 +30742,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30748,7 +30765,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30768,7 +30785,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30788,7 +30805,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30808,7 +30825,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30826,7 +30843,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30844,7 +30861,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30862,7 +30879,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30882,7 +30899,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30900,7 +30917,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30918,7 +30935,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30936,7 +30953,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30954,7 +30971,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31028,7 +31045,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31046,7 +31063,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31066,7 +31083,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31078,7 +31095,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31091,7 +31108,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31111,7 +31128,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31134,7 +31151,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31155,7 +31172,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31176,7 +31193,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31196,7 +31213,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31214,7 +31231,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31232,7 +31249,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31250,7 +31267,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31268,7 +31285,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31304,7 +31321,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31324,7 +31341,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31333,7 +31350,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31344,7 +31361,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31362,7 +31379,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31384,7 +31401,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31393,7 +31410,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31409,7 +31426,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31435,7 +31452,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31450,7 +31467,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31464,7 +31481,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31478,7 +31495,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31490,7 +31507,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31504,7 +31521,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31516,7 +31533,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31528,7 +31545,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31542,7 +31559,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31556,7 +31573,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32857,7 +32874,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32875,7 +32892,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32897,7 +32914,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32917,7 +32934,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32937,7 +32954,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32955,7 +32972,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32973,7 +32990,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -32991,7 +33008,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33007,7 +33024,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34448,7 +34465,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34469,7 +34486,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34487,7 +34504,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34505,7 +34522,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34523,7 +34540,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34544,7 +34561,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34555,7 +34572,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34565,7 +34582,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34586,7 +34603,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34604,7 +34621,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34622,7 +34639,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34640,7 +34657,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34658,7 +34675,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34676,7 +34693,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34696,7 +34713,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34717,7 +34734,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34736,7 +34753,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34757,7 +34774,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34777,7 +34794,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34795,7 +34812,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34815,7 +34832,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34835,7 +34852,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34885,7 +34902,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34905,7 +34922,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34923,7 +34940,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34941,7 +34958,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34959,7 +34976,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34979,7 +34996,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -34997,7 +35014,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35015,7 +35032,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35033,7 +35050,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35051,7 +35068,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35069,7 +35086,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35087,7 +35104,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35105,7 +35122,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35125,7 +35142,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35143,7 +35160,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35161,7 +35178,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35179,7 +35196,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35199,7 +35216,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35219,7 +35236,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35240,7 +35257,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35260,7 +35277,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35278,7 +35295,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35298,7 +35315,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36548,7 +36565,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36566,7 +36583,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36586,7 +36603,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36601,7 +36618,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36616,7 +36633,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36631,7 +36648,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36640,10 +36657,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36655,14 +36672,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36673,7 +36690,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36693,7 +36710,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36711,7 +36728,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36729,7 +36746,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36749,7 +36766,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36769,7 +36786,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36805,7 +36822,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36823,7 +36840,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36841,7 +36858,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36859,7 +36876,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36899,7 +36916,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36917,7 +36934,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36937,7 +36954,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36955,7 +36972,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36978,7 +36995,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -36999,7 +37016,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37018,7 +37035,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37038,7 +37055,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37060,7 +37077,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37096,7 +37113,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37116,7 +37133,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37136,7 +37153,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37154,7 +37171,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37172,7 +37189,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37190,7 +37207,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37210,7 +37227,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37230,7 +37247,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37250,7 +37267,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37259,10 +37276,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37274,7 +37291,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37292,7 +37309,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37304,7 +37321,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37316,7 +37333,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37331,7 +37348,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37355,7 +37372,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37369,7 +37386,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37381,7 +37398,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37395,7 +37412,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37409,7 +37426,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37421,7 +37438,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37433,7 +37450,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37445,7 +37462,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37457,7 +37474,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37469,7 +37486,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37481,7 +37498,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37493,7 +37510,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37507,7 +37524,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37519,7 +37536,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37531,7 +37548,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37545,7 +37562,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37557,7 +37574,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37569,7 +37586,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37581,7 +37598,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37593,7 +37610,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37644,7 +37661,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37695,7 +37712,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37748,7 +37765,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37801,7 +37818,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37852,7 +37869,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37903,7 +37920,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37954,7 +37971,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38007,7 +38024,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38058,7 +38075,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38111,7 +38128,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38162,7 +38179,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38213,7 +38230,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38266,7 +38283,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38317,7 +38334,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38370,7 +38387,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38472,7 +38489,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38576,7 +38593,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38734,7 +38751,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38787,7 +38804,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38889,7 +38906,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38942,7 +38959,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38951,7 +38968,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39051,7 +39068,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39102,7 +39119,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39155,7 +39172,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39208,7 +39225,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39312,7 +39329,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39410,7 +39427,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39598,7 +39615,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42597,7 +42614,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42614,7 +42631,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42631,7 +42648,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42648,7 +42665,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42667,7 +42684,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42684,7 +42701,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42701,7 +42718,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42718,7 +42735,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42737,7 +42754,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42754,7 +42771,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42771,7 +42788,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42788,7 +42805,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42805,7 +42822,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42824,7 +42841,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42841,7 +42858,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42858,7 +42875,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43443,14 +43460,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43463,17 +43480,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43483,7 +43500,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43501,7 +43518,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43517,7 +43534,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43533,7 +43550,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43549,7 +43566,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43565,7 +43582,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43583,17 +43600,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43603,7 +43620,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43621,17 +43638,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43643,17 +43660,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43665,7 +43682,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43673,7 +43690,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43683,7 +43700,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43700,7 +43717,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43717,7 +43734,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43736,7 +43753,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43754,14 +43771,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43774,14 +43791,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43792,7 +43809,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43808,14 +43825,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43826,7 +43843,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43844,7 +43861,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43853,7 +43870,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43864,7 +43881,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43880,7 +43897,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43896,7 +43913,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43912,7 +43929,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43928,7 +43945,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43946,7 +43963,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43962,7 +43979,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43978,7 +43995,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -43994,7 +44011,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44010,7 +44027,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44044,14 +44061,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44064,7 +44081,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44080,7 +44097,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44096,7 +44113,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44130,7 +44147,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44146,7 +44163,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44164,7 +44181,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44182,7 +44199,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44200,13 +44217,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44217,7 +44234,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44231,7 +44248,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44245,7 +44262,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44259,7 +44276,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44271,7 +44288,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44285,7 +44302,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44299,7 +44316,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44313,7 +44330,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44327,7 +44344,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44341,7 +44358,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44353,7 +44370,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44370,7 +44387,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44382,7 +44399,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44396,7 +44413,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44413,7 +44430,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44430,13 +44447,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44445,7 +44462,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44459,7 +44476,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44477,7 +44494,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44491,13 +44508,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44508,7 +44525,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44522,7 +44539,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44536,7 +44553,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44550,7 +44567,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44562,7 +44579,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44580,7 +44597,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44594,13 +44611,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44611,7 +44628,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44623,7 +44640,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44637,13 +44654,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44652,7 +44669,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44664,7 +44681,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44678,7 +44695,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44690,7 +44707,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44702,7 +44719,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44714,7 +44731,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44728,13 +44745,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44745,7 +44762,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44759,7 +44776,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44773,7 +44790,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44811,7 +44828,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44825,7 +44842,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44839,7 +44856,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44869,7 +44886,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44883,7 +44900,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44897,7 +44914,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44911,7 +44928,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44925,7 +44942,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44939,7 +44956,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44953,7 +44970,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44967,13 +44984,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44984,7 +45001,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -44998,7 +45015,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45013,7 +45030,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45027,7 +45044,7 @@
         <v>2455</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45041,7 +45058,7 @@
         <v>2469</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45055,7 +45072,7 @@
         <v>2475</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45069,7 +45086,7 @@
         <v>2485</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45083,7 +45100,7 @@
         <v>2520</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45097,7 +45114,7 @@
         <v>2535</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45111,7 +45128,7 @@
         <v>2544</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45125,7 +45142,7 @@
         <v>2582</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45143,7 +45160,7 @@
         <v>2651</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45157,7 +45174,7 @@
         <v>2652</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45171,7 +45188,7 @@
         <v>2739</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45185,7 +45202,7 @@
         <v>2745</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45199,7 +45216,7 @@
         <v>2769</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45213,7 +45230,7 @@
         <v>2806</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45532,7 +45549,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45764,7 +45781,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45781,7 +45798,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45800,7 +45817,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45819,7 +45836,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45839,7 +45856,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45859,7 +45876,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45880,7 +45897,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45900,7 +45917,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45910,10 +45927,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45945,7 +45962,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45965,7 +45982,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -45985,7 +46002,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46008,7 +46025,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46028,7 +46045,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46048,19 +46065,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46074,7 +46091,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46092,7 +46109,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46112,7 +46129,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46121,7 +46138,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46135,7 +46152,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46155,7 +46172,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46173,7 +46190,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46193,7 +46210,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46202,10 +46219,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46217,7 +46234,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46237,7 +46254,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46255,7 +46272,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46338,7 +46355,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46358,7 +46375,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46378,7 +46395,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46388,7 +46405,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46400,7 +46417,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46420,7 +46437,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46554,7 +46571,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46568,7 +46585,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46582,7 +46599,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46596,13 +46613,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46613,7 +46630,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46627,7 +46644,7 @@
         <v>2733</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46641,7 +46658,7 @@
         <v>2740</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -46837,7 +46854,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46859,13 +46876,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46879,13 +46896,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46896,7 +46913,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46910,7 +46927,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46924,7 +46941,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46938,7 +46955,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46961,7 +46978,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46970,7 +46987,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47021,7 +47038,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47042,14 +47059,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47065,7 +47082,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47100,7 +47117,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47109,7 +47126,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47146,7 +47163,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47167,7 +47184,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47177,7 +47194,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48636,7 +48653,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48651,13 +48668,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48698,7 +48715,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48713,7 +48730,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48773,7 +48790,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48786,7 +48803,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48811,7 +48828,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48824,7 +48841,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48837,7 +48854,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48850,7 +48867,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48865,7 +48882,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48880,7 +48897,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48893,7 +48910,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48908,7 +48925,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2500 Category: Sort Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="14"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="1595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3450" uniqueCount="1596">
   <si>
     <t>Date</t>
   </si>
@@ -4888,6 +4888,9 @@
   </si>
   <si>
     <t>Sort the People</t>
+  </si>
+  <si>
+    <t>Delete Greatest Value in Each Row</t>
   </si>
   <si>
     <t>Neither Minimum nor Maximum</t>
@@ -26935,7 +26938,7 @@
   <sheetPr/>
   <dimension ref="A1:I220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+    <sheetView topLeftCell="A206" workbookViewId="0">
       <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
@@ -45716,10 +45719,10 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -46638,10 +46641,10 @@
     </row>
     <row r="51" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A51" s="26">
-        <v>45143</v>
+        <v>44441</v>
       </c>
       <c r="B51" s="12">
-        <v>2733</v>
+        <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>1562</v>
@@ -46651,22 +46654,32 @@
       </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A52" s="27">
-        <v>45135</v>
+      <c r="A52" s="26">
+        <v>45143</v>
       </c>
       <c r="B52" s="12">
-        <v>2740</v>
+        <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>1563</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A53" s="11"/>
-      <c r="B53" s="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A53" s="27">
+        <v>45135</v>
+      </c>
+      <c r="B53" s="12">
+        <v>2740</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="54" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A54" s="11"/>
@@ -46719,6 +46732,10 @@
     <row r="66" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A66" s="11"/>
       <c r="B66" s="12"/>
+    </row>
+    <row r="67" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A67" s="11"/>
+      <c r="B67" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F$1:F$1048576">
@@ -46747,13 +46764,13 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62:F64">
+  <conditionalFormatting sqref="F63:F65">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G$1:XFD$1048576 B49:E51 A1:E48 A52:E1048576">
+  <conditionalFormatting sqref="G$1:XFD$1048576 A1:E48 B49:E52 A53:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -46876,13 +46893,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46896,13 +46913,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46913,7 +46930,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46927,7 +46944,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46941,7 +46958,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46955,7 +46972,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46987,7 +47004,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47038,7 +47055,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47059,14 +47076,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47082,7 +47099,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47117,7 +47134,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47126,7 +47143,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47163,7 +47180,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47184,7 +47201,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47194,7 +47211,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48668,13 +48685,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48715,7 +48732,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48790,7 +48807,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48803,7 +48820,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48828,7 +48845,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48841,7 +48858,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48854,7 +48871,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48867,7 +48884,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48882,7 +48899,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48897,7 +48914,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48910,7 +48927,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48925,7 +48942,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2833 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="22"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3450" uniqueCount="1596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="1597">
   <si>
     <t>Date</t>
   </si>
@@ -3723,6 +3723,9 @@
   </si>
   <si>
     <t>Check if a String Is an Acronym of Words</t>
+  </si>
+  <si>
+    <t>Furthest Point From Origin</t>
   </si>
   <si>
     <t>Add Two Numbers</t>
@@ -26936,10 +26939,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I220"/>
+  <dimension ref="A1:I221"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29902,6 +29905,20 @@
         <v>1180</v>
       </c>
       <c r="D220" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="39">
+        <v>45171</v>
+      </c>
+      <c r="B221" s="1">
+        <v>2833</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D221" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30745,7 +30762,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30768,7 +30785,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30788,7 +30805,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30808,7 +30825,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30828,7 +30845,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30846,7 +30863,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30864,7 +30881,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30882,7 +30899,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -30902,7 +30919,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -30920,7 +30937,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -30938,7 +30955,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -30956,7 +30973,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -30974,7 +30991,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31048,7 +31065,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31066,7 +31083,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31086,7 +31103,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31098,7 +31115,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31111,7 +31128,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31131,7 +31148,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31154,7 +31171,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31175,7 +31192,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31196,7 +31213,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31216,7 +31233,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31234,7 +31251,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31252,7 +31269,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31270,7 +31287,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31288,7 +31305,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31324,7 +31341,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31344,7 +31361,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31353,7 +31370,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31364,7 +31381,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31382,7 +31399,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31404,7 +31421,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31413,7 +31430,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31429,7 +31446,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31455,7 +31472,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31470,7 +31487,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31484,7 +31501,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31498,7 +31515,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31510,7 +31527,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31524,7 +31541,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31536,7 +31553,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31548,7 +31565,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31562,7 +31579,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31576,7 +31593,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32877,7 +32894,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -32895,7 +32912,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -32917,7 +32934,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -32937,7 +32954,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -32957,7 +32974,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -32975,7 +32992,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -32993,7 +33010,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -33011,7 +33028,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33027,7 +33044,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34468,7 +34485,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34489,7 +34506,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34507,7 +34524,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34525,7 +34542,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34543,7 +34560,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34564,7 +34581,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34575,7 +34592,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34585,7 +34602,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34606,7 +34623,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34624,7 +34641,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34642,7 +34659,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34660,7 +34677,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34678,7 +34695,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34696,7 +34713,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34716,7 +34733,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34737,7 +34754,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34756,7 +34773,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34777,7 +34794,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34797,7 +34814,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34815,7 +34832,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34835,7 +34852,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34855,7 +34872,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -34905,7 +34922,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -34925,7 +34942,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -34943,7 +34960,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -34961,7 +34978,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -34979,7 +34996,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -34999,7 +35016,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -35017,7 +35034,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35035,7 +35052,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35053,7 +35070,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35071,7 +35088,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35089,7 +35106,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35107,7 +35124,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35125,7 +35142,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35145,7 +35162,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35163,7 +35180,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35181,7 +35198,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35199,7 +35216,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35219,7 +35236,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35239,7 +35256,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35260,7 +35277,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35280,7 +35297,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35298,7 +35315,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35318,7 +35335,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36568,7 +36585,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36586,7 +36603,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36606,7 +36623,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36621,7 +36638,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36636,7 +36653,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36651,7 +36668,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36660,10 +36677,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36675,14 +36692,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36693,7 +36710,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36713,7 +36730,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36731,7 +36748,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36749,7 +36766,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36769,7 +36786,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36789,7 +36806,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36825,7 +36842,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36843,7 +36860,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36861,7 +36878,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36879,7 +36896,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -36919,7 +36936,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -36937,7 +36954,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -36957,7 +36974,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -36975,7 +36992,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -36998,7 +37015,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -37019,7 +37036,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37038,7 +37055,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37058,7 +37075,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37080,7 +37097,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37116,7 +37133,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37136,7 +37153,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37156,7 +37173,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37174,7 +37191,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37192,7 +37209,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37210,7 +37227,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37230,7 +37247,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37250,7 +37267,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37270,7 +37287,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37279,10 +37296,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37294,7 +37311,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37312,7 +37329,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37324,7 +37341,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37336,7 +37353,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37351,7 +37368,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37375,7 +37392,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37389,7 +37406,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37401,7 +37418,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37415,7 +37432,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37429,7 +37446,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37441,7 +37458,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37453,7 +37470,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37465,7 +37482,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37477,7 +37494,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37489,7 +37506,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37501,7 +37518,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37513,7 +37530,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37527,7 +37544,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37539,7 +37556,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37551,7 +37568,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37565,7 +37582,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37577,7 +37594,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37589,7 +37606,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37601,7 +37618,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37613,7 +37630,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37664,7 +37681,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37715,7 +37732,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37768,7 +37785,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37821,7 +37838,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37872,7 +37889,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -37923,7 +37940,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -37974,7 +37991,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38027,7 +38044,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38078,7 +38095,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38131,7 +38148,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38182,7 +38199,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38233,7 +38250,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38286,7 +38303,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38337,7 +38354,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38390,7 +38407,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38492,7 +38509,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38596,7 +38613,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38754,7 +38771,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38807,7 +38824,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -38909,7 +38926,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -38962,7 +38979,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -38971,7 +38988,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39071,7 +39088,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39122,7 +39139,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39175,7 +39192,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39228,7 +39245,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39332,7 +39349,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39430,7 +39447,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39618,7 +39635,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42617,7 +42634,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42634,7 +42651,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42651,7 +42668,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42668,7 +42685,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42687,7 +42704,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42704,7 +42721,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42721,7 +42738,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42738,7 +42755,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42757,7 +42774,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42774,7 +42791,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42791,7 +42808,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42808,7 +42825,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42825,7 +42842,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42844,7 +42861,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42861,7 +42878,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42878,7 +42895,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43463,14 +43480,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43483,17 +43500,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43503,7 +43520,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43521,7 +43538,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43537,7 +43554,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43553,7 +43570,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43569,7 +43586,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43585,7 +43602,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43603,17 +43620,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43623,7 +43640,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43641,17 +43658,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43663,17 +43680,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43685,7 +43702,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43693,7 +43710,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43703,7 +43720,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43720,7 +43737,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43737,7 +43754,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43756,7 +43773,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43774,14 +43791,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43794,14 +43811,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43812,7 +43829,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43828,14 +43845,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43846,7 +43863,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43864,7 +43881,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43873,7 +43890,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43884,7 +43901,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -43900,7 +43917,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -43916,7 +43933,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -43932,7 +43949,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -43948,7 +43965,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -43966,7 +43983,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -43982,7 +43999,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -43998,7 +44015,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -44014,7 +44031,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44030,7 +44047,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44064,14 +44081,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44084,7 +44101,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44100,7 +44117,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44116,7 +44133,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44150,7 +44167,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44166,7 +44183,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44184,7 +44201,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44202,7 +44219,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44220,13 +44237,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44237,7 +44254,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44251,7 +44268,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44265,7 +44282,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44279,7 +44296,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44291,7 +44308,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44305,7 +44322,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44319,7 +44336,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44333,7 +44350,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44347,7 +44364,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44361,7 +44378,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44373,7 +44390,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44390,7 +44407,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44402,7 +44419,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44416,7 +44433,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44433,7 +44450,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44450,13 +44467,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44465,7 +44482,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44479,7 +44496,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44497,7 +44514,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44511,13 +44528,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44528,7 +44545,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44542,7 +44559,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44556,7 +44573,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44570,7 +44587,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44582,7 +44599,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44600,7 +44617,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44614,13 +44631,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44631,7 +44648,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44643,7 +44660,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44657,13 +44674,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44672,7 +44689,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44684,7 +44701,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44698,7 +44715,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44710,7 +44727,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44722,7 +44739,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44734,7 +44751,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44748,13 +44765,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44765,7 +44782,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44779,7 +44796,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44793,7 +44810,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44831,7 +44848,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44845,7 +44862,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44859,7 +44876,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44889,7 +44906,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -44903,7 +44920,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -44917,7 +44934,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -44931,7 +44948,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -44945,7 +44962,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -44959,7 +44976,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -44973,7 +44990,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -44987,13 +45004,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45004,7 +45021,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -45018,7 +45035,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45033,7 +45050,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45047,7 +45064,7 @@
         <v>2455</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45061,7 +45078,7 @@
         <v>2469</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45075,7 +45092,7 @@
         <v>2475</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45089,7 +45106,7 @@
         <v>2485</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45103,7 +45120,7 @@
         <v>2520</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45117,7 +45134,7 @@
         <v>2535</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45131,7 +45148,7 @@
         <v>2544</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45145,7 +45162,7 @@
         <v>2582</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45163,7 +45180,7 @@
         <v>2651</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45177,7 +45194,7 @@
         <v>2652</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45191,7 +45208,7 @@
         <v>2739</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45205,7 +45222,7 @@
         <v>2745</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45219,7 +45236,7 @@
         <v>2769</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45233,7 +45250,7 @@
         <v>2806</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45552,7 +45569,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45721,7 +45738,7 @@
   <sheetPr/>
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
@@ -45784,7 +45801,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45801,7 +45818,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45820,7 +45837,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45839,7 +45856,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45859,7 +45876,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45879,7 +45896,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -45900,7 +45917,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -45920,7 +45937,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -45930,10 +45947,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -45965,7 +45982,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -45985,7 +46002,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46005,7 +46022,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46028,7 +46045,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46048,7 +46065,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46068,19 +46085,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46094,7 +46111,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46112,7 +46129,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46132,7 +46149,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46141,7 +46158,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46155,7 +46172,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46175,7 +46192,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46193,7 +46210,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46213,7 +46230,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46222,10 +46239,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46237,7 +46254,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46257,7 +46274,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46275,7 +46292,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46358,7 +46375,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46378,7 +46395,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46398,7 +46415,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46408,7 +46425,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46420,7 +46437,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46440,7 +46457,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46574,7 +46591,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46588,7 +46605,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46602,7 +46619,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46616,13 +46633,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46633,7 +46650,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46647,7 +46664,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46661,7 +46678,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46675,7 +46692,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -46871,7 +46888,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46893,13 +46910,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -46913,13 +46930,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46930,7 +46947,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -46944,7 +46961,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -46958,7 +46975,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46972,7 +46989,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -46995,7 +47012,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47004,7 +47021,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47055,7 +47072,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47076,14 +47093,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47099,7 +47116,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47134,7 +47151,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47143,7 +47160,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47180,7 +47197,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47201,7 +47218,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47211,7 +47228,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48670,7 +48687,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48685,13 +48702,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48732,7 +48749,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48747,7 +48764,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48807,7 +48824,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48820,7 +48837,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48845,7 +48862,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48858,7 +48875,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48871,7 +48888,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48884,7 +48901,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -48899,7 +48916,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -48914,7 +48931,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -48927,7 +48944,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -48942,7 +48959,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Sovled problem 2303 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="13"/>
+    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3460" uniqueCount="1601">
   <si>
     <t>Date</t>
   </si>
@@ -4726,6 +4726,9 @@
   </si>
   <si>
     <t>Add Two Integers</t>
+  </si>
+  <si>
+    <t>Calculate Amount Paid in Taxes</t>
   </si>
   <si>
     <t>Smallest Even Multiple</t>
@@ -15380,7 +15383,7 @@
   <sheetPr/>
   <dimension ref="A1:AV288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+    <sheetView topLeftCell="A261" workbookViewId="0">
       <selection activeCell="C274" sqref="C274"/>
     </sheetView>
   </sheetViews>
@@ -43518,8 +43521,8 @@
   <sheetPr/>
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -45131,7 +45134,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" customFormat="1" ht="14.55"/>
+    <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A112" s="4">
+        <v>45173</v>
+      </c>
+      <c r="B112" s="12">
+        <v>2303</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A113" s="4">
         <v>45146</v>
@@ -45140,7 +45156,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45154,7 +45170,7 @@
         <v>2455</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45168,7 +45184,7 @@
         <v>2469</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45182,7 +45198,7 @@
         <v>2475</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45196,7 +45212,7 @@
         <v>2485</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45210,7 +45226,7 @@
         <v>2520</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45224,7 +45240,7 @@
         <v>2535</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45238,7 +45254,7 @@
         <v>2544</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45252,7 +45268,7 @@
         <v>2582</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45270,7 +45286,7 @@
         <v>2651</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45284,7 +45300,7 @@
         <v>2652</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45298,7 +45314,7 @@
         <v>2739</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45312,7 +45328,7 @@
         <v>2745</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45326,7 +45342,7 @@
         <v>2769</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45340,7 +45356,7 @@
         <v>2806</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45356,242 +45372,303 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
-    <cfRule type="cellIs" dxfId="3" priority="57" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="72" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" dxfId="1" priority="42" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="43" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="44" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="45" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="46" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="57" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="59" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="60" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="61" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F106">
+    <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
+      <formula>NOT(ISERROR(SEARCH("Apple",F106)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="32" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F106)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F106)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="38" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="39" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="40" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="35" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="34" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F112">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="3" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F112)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F112)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
+      <formula>NOT(ISERROR(SEARCH("Apple",F112)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:A44">
+    <cfRule type="cellIs" dxfId="1" priority="62" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="64" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="65" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="66" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:F48">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A131:E1048576 G131:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="68" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="69" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="70" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="71" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F88 F90:F105 F131:F1048576">
+    <cfRule type="containsText" dxfId="9" priority="46" operator="between" text="Apple">
+      <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="47" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="48" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="49" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="54" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="55" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="56" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G106:XFD106 A106:E106">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="42" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="43" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="44" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="45" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G107:XFD111 G113:XFD130 A113:E130 A107:E111">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="27" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="29" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="30" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F107:F111 F113:F130">
     <cfRule type="containsText" dxfId="9" priority="16" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="17" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F107)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="18" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F106)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="23" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="24" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="25" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F107)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="19" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="20" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="19" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="23" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="24" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="25" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:A44">
-    <cfRule type="cellIs" dxfId="1" priority="47" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="48" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="49" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="50" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="51" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:F48">
-    <cfRule type="cellIs" dxfId="0" priority="37" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A131:E1048576 G131:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="52" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="53" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="54" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="55" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="56" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F131:F1048576">
-    <cfRule type="containsText" dxfId="9" priority="31" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="32" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="33" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="34" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="35" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="36" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="38" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="39" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="40" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="41" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G106:XFD106 A106:E106">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="27" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="28" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="29" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="30" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD130 A113:E130 A107:E111">
+  <conditionalFormatting sqref="G112:XFD112 A112:E112">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F130">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F107)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="3" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F107)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -45659,7 +45736,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45891,7 +45968,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45908,7 +45985,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -45927,7 +46004,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -45946,7 +46023,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -45966,7 +46043,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -45986,7 +46063,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46007,7 +46084,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46027,7 +46104,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46037,10 +46114,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46072,7 +46149,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46092,7 +46169,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46112,7 +46189,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46135,7 +46212,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46155,7 +46232,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46175,19 +46252,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46201,7 +46278,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46219,7 +46296,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46239,7 +46316,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46248,7 +46325,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46262,7 +46339,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46282,7 +46359,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46300,7 +46377,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46320,7 +46397,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46329,10 +46406,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46344,7 +46421,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46364,7 +46441,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46382,7 +46459,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46465,7 +46542,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46485,7 +46562,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46505,7 +46582,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46515,7 +46592,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46527,7 +46604,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46547,7 +46624,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46681,7 +46758,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46695,7 +46772,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46709,7 +46786,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46723,13 +46800,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46740,7 +46817,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46754,7 +46831,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46768,7 +46845,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46782,7 +46859,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -47000,13 +47077,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -47020,13 +47097,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -47037,7 +47114,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -47051,7 +47128,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -47065,7 +47142,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -47079,7 +47156,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -47111,7 +47188,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47162,7 +47239,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47183,14 +47260,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47206,7 +47283,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47241,7 +47318,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47250,7 +47327,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47287,7 +47364,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47308,7 +47385,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47318,7 +47395,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48792,13 +48869,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48839,7 +48916,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48854,7 +48931,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48914,7 +48991,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -48927,7 +49004,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -48952,7 +49029,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -48965,7 +49042,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -48978,7 +49055,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -48991,7 +49068,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -49006,7 +49083,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -49021,7 +49098,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -49034,7 +49111,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -49049,7 +49126,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2243 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15000" windowHeight="5082" tabRatio="991" firstSheet="10" activeTab="20"/>
+    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3460" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3462" uniqueCount="1602">
   <si>
     <t>Date</t>
   </si>
@@ -3678,6 +3678,9 @@
   </si>
   <si>
     <t>Minimum Number of Operations to Convert Time</t>
+  </si>
+  <si>
+    <t>Calculate Digit Sum of a String</t>
   </si>
   <si>
     <t>Count Prefixes of a Given String</t>
@@ -27032,10 +27035,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I221"/>
+  <dimension ref="A1:I222"/>
   <sheetViews>
-    <sheetView topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="A221" sqref="A221"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29745,10 +29748,10 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="26">
-        <v>44700</v>
+        <v>45176</v>
       </c>
       <c r="B201" s="1">
-        <v>2255</v>
+        <v>2243</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>1166</v>
@@ -29762,7 +29765,7 @@
         <v>44700</v>
       </c>
       <c r="B202" s="1">
-        <v>2259</v>
+        <v>2255</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>1167</v>
@@ -29773,10 +29776,10 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="26">
-        <v>45153</v>
+        <v>44700</v>
       </c>
       <c r="B203" s="1">
-        <v>2264</v>
+        <v>2259</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>1168</v>
@@ -29786,11 +29789,11 @@
       </c>
     </row>
     <row r="204" spans="1:4">
-      <c r="A204" s="39">
-        <v>44726</v>
+      <c r="A204" s="26">
+        <v>45153</v>
       </c>
       <c r="B204" s="1">
-        <v>2278</v>
+        <v>2264</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>1169</v>
@@ -29801,10 +29804,10 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="39">
-        <v>45151</v>
+        <v>44726</v>
       </c>
       <c r="B205" s="1">
-        <v>2309</v>
+        <v>2278</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>1170</v>
@@ -29813,12 +29816,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" s="1" customFormat="1" spans="1:4">
-      <c r="A206" s="4">
-        <v>45149</v>
-      </c>
-      <c r="B206" s="12">
-        <v>2315</v>
+    <row r="206" spans="1:4">
+      <c r="A206" s="39">
+        <v>45151</v>
+      </c>
+      <c r="B206" s="1">
+        <v>2309</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>1171</v>
@@ -29827,32 +29830,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
-      <c r="A207" s="36"/>
+    <row r="207" s="1" customFormat="1" spans="1:4">
+      <c r="A207" s="4">
+        <v>45149</v>
+      </c>
+      <c r="B207" s="12">
+        <v>2315</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" s="36"/>
     </row>
-    <row r="209" spans="1:4">
-      <c r="A209" s="39">
-        <v>44838</v>
-      </c>
-      <c r="B209" s="1">
-        <v>2423</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>1172</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="209" spans="1:1">
+      <c r="A209" s="36"/>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="39">
-        <v>45169</v>
+        <v>44838</v>
       </c>
       <c r="B210" s="1">
-        <v>2490</v>
+        <v>2423</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1173</v>
@@ -29863,10 +29866,10 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="39">
-        <v>45150</v>
+        <v>45169</v>
       </c>
       <c r="B211" s="1">
-        <v>2496</v>
+        <v>2490</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1174</v>
@@ -29877,10 +29880,10 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="39">
-        <v>45160</v>
+        <v>45150</v>
       </c>
       <c r="B212" s="1">
-        <v>2586</v>
+        <v>2496</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>1175</v>
@@ -29891,10 +29894,10 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="39">
-        <v>45135</v>
+        <v>45160</v>
       </c>
       <c r="B213" s="1">
-        <v>2678</v>
+        <v>2586</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>1176</v>
@@ -29905,10 +29908,10 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="39">
-        <v>45140</v>
+        <v>45135</v>
       </c>
       <c r="B214" s="1">
-        <v>2697</v>
+        <v>2678</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>1177</v>
@@ -29919,10 +29922,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B215" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>1178</v>
@@ -29933,10 +29936,10 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B216" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>1179</v>
@@ -29947,40 +29950,40 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B217" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>1180</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B218" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C218" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>1181</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="39">
-        <v>45144</v>
+        <v>45131</v>
       </c>
       <c r="B219" s="1">
-        <v>2810</v>
-      </c>
-      <c r="C219" s="1" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C219" s="16" t="s">
         <v>1182</v>
       </c>
       <c r="D219" s="1" t="s">
@@ -29989,10 +29992,10 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="39">
-        <v>45159</v>
+        <v>45144</v>
       </c>
       <c r="B220" s="1">
-        <v>2828</v>
+        <v>2810</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>1183</v>
@@ -30003,15 +30006,29 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="39">
-        <v>45171</v>
+        <v>45159</v>
       </c>
       <c r="B221" s="1">
-        <v>2833</v>
+        <v>2828</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>1184</v>
       </c>
       <c r="D221" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="39">
+        <v>45171</v>
+      </c>
+      <c r="B222" s="1">
+        <v>2833</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30157,12 +30174,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F205">
+  <conditionalFormatting sqref="F206">
     <cfRule type="containsText" dxfId="5" priority="47" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="55" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F205)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="63" operator="between">
       <formula>"Amazon"</formula>
@@ -30193,15 +30210,15 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
+  <conditionalFormatting sqref="F207">
     <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Apple",F207)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="3" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F206)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
       <formula>"Amazon"</formula>
@@ -30232,12 +30249,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
+  <conditionalFormatting sqref="F208">
     <cfRule type="containsText" dxfId="5" priority="45" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="53" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F207)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="61" operator="between">
       <formula>"Amazon"</formula>
@@ -30268,12 +30285,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208">
+  <conditionalFormatting sqref="F209">
     <cfRule type="containsText" dxfId="5" priority="44" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="52" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F208)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="60" operator="between">
       <formula>"Amazon"</formula>
@@ -30304,12 +30321,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F217">
+  <conditionalFormatting sqref="F218">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -30340,7 +30357,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D218">
+  <conditionalFormatting sqref="D219">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30362,12 +30379,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F218">
+  <conditionalFormatting sqref="F219">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -30398,12 +30415,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F219">
+  <conditionalFormatting sqref="F220">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -30434,7 +30451,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A216">
+  <conditionalFormatting sqref="A210:A217">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30468,12 +30485,12 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F209:F216">
+  <conditionalFormatting sqref="F210:F217">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="27" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F209)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="28" operator="between">
       <formula>"Amazon"</formula>
@@ -30504,7 +30521,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E204 A189:E193 G195:XFD204 A195:E196 G220:XFD1048576 A220:E1048576">
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E205 A195:E196 A189:E193 G195:XFD205 A221:E1048576 G221:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30526,7 +30543,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F204 F220:F1048576">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F205 F221:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30606,7 +30623,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G205:XFD205 A205:E205">
+  <conditionalFormatting sqref="G206:XFD206 A206:E206">
     <cfRule type="cellIs" dxfId="0" priority="119" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30624,55 +30641,55 @@
       <formula>"Medium"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="151" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G206:XFD206 A206:E206">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:XFD207 A207:E207">
-    <cfRule type="cellIs" dxfId="0" priority="117" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="125" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="133" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="141" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="149" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G208:XFD208 A208:E208">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="133" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="141" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="149" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G209:XFD209 A209:E209">
     <cfRule type="cellIs" dxfId="0" priority="116" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30694,7 +30711,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G209:XFD216 B209:E216">
+  <conditionalFormatting sqref="G210:XFD217 B210:E217">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30716,7 +30733,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G217:XFD217 A217:E217">
+  <conditionalFormatting sqref="G218:XFD218 A218:E218">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30738,7 +30755,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G218:XFD218 E218 A218:C218">
+  <conditionalFormatting sqref="G219:XFD219 A219:C219 E219">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30760,7 +30777,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G219:XFD219 A219:E219">
+  <conditionalFormatting sqref="G220:XFD220 A220:E220">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30855,7 +30872,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30878,7 +30895,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30898,7 +30915,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30918,7 +30935,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30938,7 +30955,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30956,7 +30973,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30974,7 +30991,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -30992,7 +31009,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -31012,7 +31029,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -31030,7 +31047,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -31048,7 +31065,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -31066,7 +31083,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -31084,7 +31101,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31158,7 +31175,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31176,7 +31193,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31196,7 +31213,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31208,7 +31225,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31221,7 +31238,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31241,7 +31258,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31264,7 +31281,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31285,7 +31302,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31306,7 +31323,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31326,7 +31343,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31344,7 +31361,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31362,7 +31379,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31380,7 +31397,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31398,7 +31415,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31434,7 +31451,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31454,7 +31471,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31463,7 +31480,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31474,7 +31491,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31492,7 +31509,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31514,7 +31531,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31523,7 +31540,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31539,7 +31556,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31565,7 +31582,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31580,7 +31597,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31594,7 +31611,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31608,7 +31625,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31620,7 +31637,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31634,7 +31651,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31646,7 +31663,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31658,7 +31675,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31672,7 +31689,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31686,7 +31703,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -32987,7 +33004,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -33005,7 +33022,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -33027,7 +33044,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -33047,7 +33064,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33067,7 +33084,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -33085,7 +33102,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -33103,7 +33120,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -33121,7 +33138,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33137,7 +33154,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34578,7 +34595,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34599,7 +34616,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34617,7 +34634,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34635,7 +34652,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34653,7 +34670,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34674,7 +34691,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34685,7 +34702,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34695,7 +34712,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34716,7 +34733,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34734,7 +34751,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34752,7 +34769,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34770,7 +34787,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34788,7 +34805,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34806,7 +34823,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34826,7 +34843,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34847,7 +34864,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34866,7 +34883,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34887,7 +34904,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34907,7 +34924,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34925,7 +34942,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34945,7 +34962,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34965,7 +34982,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35015,7 +35032,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35035,7 +35052,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35053,7 +35070,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -35071,7 +35088,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35089,7 +35106,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -35109,7 +35126,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -35127,7 +35144,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35145,7 +35162,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35163,7 +35180,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35181,7 +35198,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35199,7 +35216,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35217,7 +35234,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35235,7 +35252,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35255,7 +35272,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35273,7 +35290,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35291,7 +35308,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35309,7 +35326,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35329,7 +35346,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35349,7 +35366,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35370,7 +35387,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35390,7 +35407,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35408,7 +35425,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35428,7 +35445,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36678,7 +36695,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36696,7 +36713,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36716,7 +36733,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36731,7 +36748,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36746,7 +36763,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36761,7 +36778,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36770,10 +36787,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36785,14 +36802,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36803,7 +36820,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36823,7 +36840,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36841,7 +36858,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36859,7 +36876,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36879,7 +36896,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36899,7 +36916,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36935,7 +36952,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36953,7 +36970,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36971,7 +36988,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -36989,7 +37006,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -37029,7 +37046,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -37047,7 +37064,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -37067,7 +37084,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -37085,7 +37102,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -37108,7 +37125,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -37129,7 +37146,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37148,7 +37165,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37168,7 +37185,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37190,7 +37207,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37226,7 +37243,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37246,7 +37263,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37266,7 +37283,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37284,7 +37301,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37302,7 +37319,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37320,7 +37337,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37340,7 +37357,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37360,7 +37377,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37380,7 +37397,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37389,10 +37406,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37404,7 +37421,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37422,7 +37439,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37434,7 +37451,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37446,7 +37463,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37461,7 +37478,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37485,7 +37502,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37499,7 +37516,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37511,7 +37528,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37525,7 +37542,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37539,7 +37556,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37551,7 +37568,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37563,7 +37580,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37575,7 +37592,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37587,7 +37604,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37599,7 +37616,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37611,7 +37628,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37623,7 +37640,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37637,7 +37654,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37649,7 +37666,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37661,7 +37678,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37675,7 +37692,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37687,7 +37704,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37699,7 +37716,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37711,7 +37728,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37723,7 +37740,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37774,7 +37791,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37825,7 +37842,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37878,7 +37895,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37931,7 +37948,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -37982,7 +37999,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -38033,7 +38050,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -38084,7 +38101,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38137,7 +38154,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38188,7 +38205,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38241,7 +38258,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38292,7 +38309,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38343,7 +38360,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38396,7 +38413,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38447,7 +38464,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38500,7 +38517,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38602,7 +38619,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38706,7 +38723,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38864,7 +38881,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38917,7 +38934,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -39019,7 +39036,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -39072,7 +39089,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -39081,7 +39098,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39181,7 +39198,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39232,7 +39249,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39285,7 +39302,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39338,7 +39355,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39442,7 +39459,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39540,7 +39557,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39728,7 +39745,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42727,7 +42744,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42744,7 +42761,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42761,7 +42778,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42778,7 +42795,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42797,7 +42814,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42814,7 +42831,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42831,7 +42848,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42848,7 +42865,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42867,7 +42884,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42884,7 +42901,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42901,7 +42918,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42918,7 +42935,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42935,7 +42952,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42954,7 +42971,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42971,7 +42988,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -42988,7 +43005,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43521,7 +43538,7 @@
   <sheetPr/>
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
@@ -43573,14 +43590,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43593,17 +43610,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43613,7 +43630,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43631,7 +43648,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43647,7 +43664,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43663,7 +43680,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43679,7 +43696,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43695,7 +43712,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43713,17 +43730,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43733,7 +43750,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43751,17 +43768,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43773,17 +43790,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43795,7 +43812,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43803,7 +43820,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43813,7 +43830,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43830,7 +43847,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43847,7 +43864,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43866,7 +43883,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43884,14 +43901,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43904,14 +43921,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43922,7 +43939,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43938,14 +43955,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43956,7 +43973,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43974,7 +43991,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -43983,7 +44000,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -43994,7 +44011,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44010,7 +44027,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44026,7 +44043,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -44042,7 +44059,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -44058,7 +44075,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -44076,7 +44093,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -44092,7 +44109,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -44108,7 +44125,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -44124,7 +44141,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44140,7 +44157,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44174,14 +44191,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44194,7 +44211,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44210,7 +44227,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44226,7 +44243,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44260,7 +44277,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44276,7 +44293,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44294,7 +44311,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44312,7 +44329,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44330,13 +44347,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44347,7 +44364,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44361,7 +44378,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44375,7 +44392,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44389,7 +44406,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44401,7 +44418,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44415,7 +44432,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44429,7 +44446,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44443,7 +44460,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44457,7 +44474,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44471,7 +44488,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44483,7 +44500,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44500,7 +44517,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44512,7 +44529,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44526,7 +44543,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44543,7 +44560,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44560,13 +44577,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44575,7 +44592,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44589,7 +44606,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44607,7 +44624,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44621,13 +44638,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44638,7 +44655,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44652,7 +44669,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44666,7 +44683,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44680,7 +44697,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44692,7 +44709,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44710,7 +44727,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44724,13 +44741,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44741,7 +44758,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44753,7 +44770,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44767,13 +44784,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44782,7 +44799,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44794,7 +44811,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44808,7 +44825,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44820,7 +44837,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44832,7 +44849,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44844,7 +44861,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44858,13 +44875,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44875,7 +44892,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44889,7 +44906,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44903,7 +44920,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44941,7 +44958,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44955,7 +44972,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44969,7 +44986,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -44999,7 +45016,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -45013,7 +45030,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -45027,7 +45044,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -45041,7 +45058,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -45055,7 +45072,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -45069,7 +45086,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -45083,7 +45100,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -45097,13 +45114,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45114,7 +45131,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -45128,7 +45145,7 @@
         <v>2235</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45142,7 +45159,7 @@
         <v>2303</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -45156,7 +45173,7 @@
         <v>2413</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45170,7 +45187,7 @@
         <v>2455</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45184,7 +45201,7 @@
         <v>2469</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45198,7 +45215,7 @@
         <v>2475</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45212,7 +45229,7 @@
         <v>2485</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45226,7 +45243,7 @@
         <v>2520</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45240,7 +45257,7 @@
         <v>2535</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45254,7 +45271,7 @@
         <v>2544</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45268,7 +45285,7 @@
         <v>2582</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45286,7 +45303,7 @@
         <v>2651</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -45300,7 +45317,7 @@
         <v>2652</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45314,7 +45331,7 @@
         <v>2739</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45328,7 +45345,7 @@
         <v>2745</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45342,7 +45359,7 @@
         <v>2769</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45356,7 +45373,7 @@
         <v>2806</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45736,7 +45753,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45968,7 +45985,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -45985,7 +46002,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -46004,7 +46021,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46023,7 +46040,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -46043,7 +46060,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -46063,7 +46080,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46084,7 +46101,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46104,7 +46121,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46114,10 +46131,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46149,7 +46166,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46169,7 +46186,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46189,7 +46206,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46212,7 +46229,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46232,7 +46249,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46252,19 +46269,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46278,7 +46295,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46296,7 +46313,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46316,7 +46333,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46325,7 +46342,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46339,7 +46356,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46359,7 +46376,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46377,7 +46394,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46397,7 +46414,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46406,10 +46423,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46421,7 +46438,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46441,7 +46458,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46459,7 +46476,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46542,7 +46559,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46562,7 +46579,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46582,7 +46599,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46592,7 +46609,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46604,7 +46621,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46624,7 +46641,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46758,7 +46775,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46772,7 +46789,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46786,7 +46803,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46800,13 +46817,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46817,7 +46834,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46831,7 +46848,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46845,7 +46862,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46859,7 +46876,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -47055,7 +47072,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -47077,13 +47094,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -47097,13 +47114,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -47114,7 +47131,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -47128,7 +47145,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -47142,7 +47159,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -47156,7 +47173,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -47179,7 +47196,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47188,7 +47205,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47239,7 +47256,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47260,14 +47277,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47283,7 +47300,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47318,7 +47335,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47327,7 +47344,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47364,7 +47381,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47385,7 +47402,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47395,7 +47412,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48854,7 +48871,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48869,13 +48886,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48916,7 +48933,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48931,7 +48948,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -48991,7 +49008,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -49004,7 +49021,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -49029,7 +49046,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -49042,7 +49059,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -49055,7 +49072,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -49068,7 +49085,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -49083,7 +49100,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -49098,7 +49115,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -49111,7 +49128,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -49126,7 +49143,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2239 Category: Math Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="14"/>
+    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3462" uniqueCount="1602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="1603">
   <si>
     <t>Date</t>
   </si>
@@ -4726,6 +4726,9 @@
   </si>
   <si>
     <t>Largest Number After Digit Swaps by Parity</t>
+  </si>
+  <si>
+    <t>Find Closest Number to Zero</t>
   </si>
   <si>
     <t>Add Two Integers</t>
@@ -15386,7 +15389,7 @@
   <sheetPr/>
   <dimension ref="A1:AV288"/>
   <sheetViews>
-    <sheetView topLeftCell="A261" workbookViewId="0">
+    <sheetView topLeftCell="A276" workbookViewId="0">
       <selection activeCell="C274" sqref="C274"/>
     </sheetView>
   </sheetViews>
@@ -27037,7 +27040,7 @@
   <sheetPr/>
   <dimension ref="A1:I222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+    <sheetView topLeftCell="A191" workbookViewId="0">
       <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
@@ -43536,10 +43539,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="14.1"/>
@@ -45139,10 +45142,10 @@
     </row>
     <row r="111" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A111" s="4">
-        <v>45149</v>
+        <v>45176</v>
       </c>
       <c r="B111" s="12">
-        <v>2235</v>
+        <v>2239</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>1508</v>
@@ -45153,10 +45156,10 @@
     </row>
     <row r="112" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A112" s="4">
-        <v>45173</v>
+        <v>45149</v>
       </c>
       <c r="B112" s="12">
-        <v>2303</v>
+        <v>2235</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1509</v>
@@ -45167,10 +45170,10 @@
     </row>
     <row r="113" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A113" s="4">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="B113" s="12">
-        <v>2413</v>
+        <v>2303</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1510</v>
@@ -45181,10 +45184,10 @@
     </row>
     <row r="114" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A114" s="4">
-        <v>45167</v>
+        <v>45146</v>
       </c>
       <c r="B114" s="12">
-        <v>2455</v>
+        <v>2413</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1511</v>
@@ -45195,10 +45198,10 @@
     </row>
     <row r="115" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A115" s="4">
-        <v>45141</v>
+        <v>45167</v>
       </c>
       <c r="B115" s="12">
-        <v>2469</v>
+        <v>2455</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1512</v>
@@ -45212,7 +45215,7 @@
         <v>45141</v>
       </c>
       <c r="B116" s="12">
-        <v>2475</v>
+        <v>2469</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>1513</v>
@@ -45223,10 +45226,10 @@
     </row>
     <row r="117" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A117" s="4">
-        <v>45148</v>
+        <v>45141</v>
       </c>
       <c r="B117" s="12">
-        <v>2485</v>
+        <v>2475</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>1514</v>
@@ -45237,10 +45240,10 @@
     </row>
     <row r="118" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A118" s="4">
-        <v>45160</v>
+        <v>45148</v>
       </c>
       <c r="B118" s="12">
-        <v>2520</v>
+        <v>2485</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>1515</v>
@@ -45251,10 +45254,10 @@
     </row>
     <row r="119" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A119" s="4">
-        <v>45156</v>
+        <v>45160</v>
       </c>
       <c r="B119" s="12">
-        <v>2535</v>
+        <v>2520</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>1516</v>
@@ -45265,10 +45268,10 @@
     </row>
     <row r="120" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A120" s="4">
-        <v>45163</v>
+        <v>45156</v>
       </c>
       <c r="B120" s="12">
-        <v>2544</v>
+        <v>2535</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>1517</v>
@@ -45279,10 +45282,10 @@
     </row>
     <row r="121" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A121" s="4">
-        <v>45137</v>
+        <v>45163</v>
       </c>
       <c r="B121" s="12">
-        <v>2582</v>
+        <v>2544</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>1518</v>
@@ -45291,30 +45294,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="12"/>
-    </row>
-    <row r="123" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A123" s="4">
-        <v>45147</v>
-      </c>
-      <c r="B123" s="12">
-        <v>2651</v>
-      </c>
-      <c r="C123" s="1" t="s">
+    <row r="122" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A122" s="4">
+        <v>45137</v>
+      </c>
+      <c r="B122" s="12">
+        <v>2582</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>1519</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D122" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A123" s="4"/>
+      <c r="B123" s="12"/>
     </row>
     <row r="124" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A124" s="4">
-        <v>45145</v>
+        <v>45147</v>
       </c>
       <c r="B124" s="12">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>1520</v>
@@ -45325,10 +45328,10 @@
     </row>
     <row r="125" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A125" s="4">
-        <v>45131</v>
+        <v>45145</v>
       </c>
       <c r="B125" s="12">
-        <v>2739</v>
+        <v>2652</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>1521</v>
@@ -45338,11 +45341,11 @@
       </c>
     </row>
     <row r="126" s="1" customFormat="1" ht="12.85" spans="1:4">
-      <c r="A126" s="27">
-        <v>45133</v>
+      <c r="A126" s="4">
+        <v>45131</v>
       </c>
       <c r="B126" s="12">
-        <v>2745</v>
+        <v>2739</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>1522</v>
@@ -45353,10 +45356,10 @@
     </row>
     <row r="127" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A127" s="27">
-        <v>45143</v>
+        <v>45133</v>
       </c>
       <c r="B127" s="12">
-        <v>2769</v>
+        <v>2745</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>1523</v>
@@ -45367,10 +45370,10 @@
     </row>
     <row r="128" s="1" customFormat="1" ht="12.85" spans="1:4">
       <c r="A128" s="27">
-        <v>45167</v>
+        <v>45143</v>
       </c>
       <c r="B128" s="12">
-        <v>2806</v>
+        <v>2769</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>1524</v>
@@ -45379,13 +45382,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" s="1" customFormat="1" ht="12.85" spans="1:2">
-      <c r="A129" s="11"/>
-      <c r="B129" s="12"/>
+    <row r="129" s="1" customFormat="1" ht="12.85" spans="1:4">
+      <c r="A129" s="27">
+        <v>45167</v>
+      </c>
+      <c r="B129" s="12">
+        <v>2806</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="130" s="1" customFormat="1" ht="12.85" spans="1:2">
       <c r="A130" s="11"/>
       <c r="B130" s="12"/>
+    </row>
+    <row r="131" s="1" customFormat="1" ht="12.85" spans="1:2">
+      <c r="A131" s="11"/>
+      <c r="B131" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E2">
@@ -45455,43 +45472,43 @@
       <formula>"Amazon"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F112">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
+  <conditionalFormatting sqref="F113">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
+      <formula>NOT(ISERROR(SEARCH("Apple",F113)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F113)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="3" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F113)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>"Amazon"</formula>
       <formula>"Amazon"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="3" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F112)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F112)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="1" operator="between" text="Apple">
-      <formula>NOT(ISERROR(SEARCH("Apple",F112)))</formula>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:A44">
@@ -45522,7 +45539,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 A131:E1048576 G131:XFD1048576">
+  <conditionalFormatting sqref="B43:E45 A1:E42 A46:E88 G1:XFD88 G90:XFD105 A90:E105 G132:XFD1048576 A132:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="67" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45544,7 +45561,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F88 F90:F105 F131:F1048576">
+  <conditionalFormatting sqref="F1:F88 F90:F105 F132:F1048576">
     <cfRule type="containsText" dxfId="9" priority="46" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F1)))</formula>
     </cfRule>
@@ -45605,7 +45622,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G107:XFD111 G113:XFD130 A113:E130 A107:E111">
+  <conditionalFormatting sqref="G107:XFD112 A107:E112 G114:XFD131 A114:E131">
     <cfRule type="cellIs" dxfId="0" priority="26" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -45627,7 +45644,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:F111 F113:F130">
+  <conditionalFormatting sqref="F107:F112 F114:F131">
     <cfRule type="containsText" dxfId="9" priority="16" operator="between" text="Apple">
       <formula>NOT(ISERROR(SEARCH("Apple",F107)))</formula>
     </cfRule>
@@ -45666,26 +45683,26 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G112:XFD112 A112:E112">
+  <conditionalFormatting sqref="G113:XFD113 A113:E113">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>"Easy"</formula>
       <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -45753,7 +45770,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -45985,7 +46002,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46002,7 +46019,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -46021,7 +46038,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46040,7 +46057,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -46060,7 +46077,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -46080,7 +46097,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46101,7 +46118,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46121,7 +46138,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46131,10 +46148,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46166,7 +46183,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46186,7 +46203,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46206,7 +46223,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46229,7 +46246,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46249,7 +46266,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46269,19 +46286,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46295,7 +46312,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46313,7 +46330,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46333,7 +46350,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46342,7 +46359,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46356,7 +46373,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46376,7 +46393,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46394,7 +46411,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46414,7 +46431,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46423,10 +46440,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46438,7 +46455,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46458,7 +46475,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46476,7 +46493,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46559,7 +46576,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46579,7 +46596,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46599,7 +46616,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46609,7 +46626,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46621,7 +46638,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46641,7 +46658,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46775,7 +46792,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46789,7 +46806,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46803,7 +46820,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46817,13 +46834,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46834,7 +46851,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46848,7 +46865,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46862,7 +46879,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46876,7 +46893,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -47094,13 +47111,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -47114,13 +47131,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -47131,7 +47148,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -47145,7 +47162,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -47159,7 +47176,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -47173,7 +47190,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -47205,7 +47222,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47256,7 +47273,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47277,14 +47294,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47300,7 +47317,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47335,7 +47352,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47344,7 +47361,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47381,7 +47398,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47402,7 +47419,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47412,7 +47429,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48886,13 +48903,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48933,7 +48950,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48948,7 +48965,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -49008,7 +49025,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -49021,7 +49038,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -49046,7 +49063,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -49059,7 +49076,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -49072,7 +49089,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -49085,7 +49102,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -49100,7 +49117,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -49115,7 +49132,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -49128,7 +49145,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -49143,7 +49160,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2843 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="20"/>
+    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="1603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="1604">
   <si>
     <t>Date</t>
   </si>
@@ -3738,6 +3738,9 @@
   </si>
   <si>
     <t>Furthest Point From Origin</t>
+  </si>
+  <si>
+    <t>Count Symmetric Integers</t>
   </si>
   <si>
     <t>Add Two Numbers</t>
@@ -27038,10 +27041,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I222"/>
+  <dimension ref="A1:I223"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -30032,6 +30035,20 @@
         <v>1185</v>
       </c>
       <c r="D222" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="39">
+        <v>45178</v>
+      </c>
+      <c r="B223" s="1">
+        <v>2843</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D223" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30875,7 +30892,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30898,7 +30915,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30918,7 +30935,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30938,7 +30955,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30958,7 +30975,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30976,7 +30993,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -30994,7 +31011,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -31012,7 +31029,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -31032,7 +31049,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -31050,7 +31067,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -31068,7 +31085,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -31086,7 +31103,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -31104,7 +31121,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31178,7 +31195,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31196,7 +31213,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31216,7 +31233,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31228,7 +31245,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31241,7 +31258,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31261,7 +31278,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31284,7 +31301,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31305,7 +31322,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31326,7 +31343,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31346,7 +31363,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31364,7 +31381,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31382,7 +31399,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31400,7 +31417,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31418,7 +31435,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31454,7 +31471,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31474,7 +31491,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31483,7 +31500,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31494,7 +31511,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31512,7 +31529,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31534,7 +31551,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31543,7 +31560,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31559,7 +31576,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31585,7 +31602,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31600,7 +31617,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31614,7 +31631,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31628,7 +31645,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31640,7 +31657,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31654,7 +31671,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31666,7 +31683,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31678,7 +31695,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31692,7 +31709,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31706,7 +31723,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -33007,7 +33024,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -33025,7 +33042,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -33047,7 +33064,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -33067,7 +33084,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33087,7 +33104,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -33105,7 +33122,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -33123,7 +33140,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -33141,7 +33158,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33157,7 +33174,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34598,7 +34615,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34619,7 +34636,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34637,7 +34654,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34655,7 +34672,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34673,7 +34690,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34694,7 +34711,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34705,7 +34722,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34715,7 +34732,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34736,7 +34753,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34754,7 +34771,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34772,7 +34789,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34790,7 +34807,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34808,7 +34825,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34826,7 +34843,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34846,7 +34863,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34867,7 +34884,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34886,7 +34903,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34907,7 +34924,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34927,7 +34944,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34945,7 +34962,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34965,7 +34982,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -34985,7 +35002,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35035,7 +35052,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35055,7 +35072,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35073,7 +35090,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -35091,7 +35108,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35109,7 +35126,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -35129,7 +35146,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -35147,7 +35164,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35165,7 +35182,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35183,7 +35200,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35201,7 +35218,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35219,7 +35236,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35237,7 +35254,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35255,7 +35272,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35275,7 +35292,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35293,7 +35310,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35311,7 +35328,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35329,7 +35346,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35349,7 +35366,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35369,7 +35386,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35390,7 +35407,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35410,7 +35427,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35428,7 +35445,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35448,7 +35465,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36698,7 +36715,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36716,7 +36733,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36736,7 +36753,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36751,7 +36768,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36766,7 +36783,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36781,7 +36798,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36790,10 +36807,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36805,14 +36822,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36823,7 +36840,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36843,7 +36860,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36861,7 +36878,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36879,7 +36896,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36899,7 +36916,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36919,7 +36936,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36955,7 +36972,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36973,7 +36990,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -36991,7 +37008,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -37009,7 +37026,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -37049,7 +37066,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -37067,7 +37084,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -37087,7 +37104,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -37105,7 +37122,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -37128,7 +37145,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -37149,7 +37166,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37168,7 +37185,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37188,7 +37205,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37210,7 +37227,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37246,7 +37263,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37266,7 +37283,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37286,7 +37303,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37304,7 +37321,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37322,7 +37339,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37340,7 +37357,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37360,7 +37377,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37380,7 +37397,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37400,7 +37417,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37409,10 +37426,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37424,7 +37441,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37442,7 +37459,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37454,7 +37471,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37466,7 +37483,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37481,7 +37498,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37505,7 +37522,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37519,7 +37536,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37531,7 +37548,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37545,7 +37562,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37559,7 +37576,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37571,7 +37588,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37583,7 +37600,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37595,7 +37612,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37607,7 +37624,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37619,7 +37636,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37631,7 +37648,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37643,7 +37660,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37657,7 +37674,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37669,7 +37686,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37681,7 +37698,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37695,7 +37712,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37707,7 +37724,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37719,7 +37736,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37731,7 +37748,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37743,7 +37760,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37794,7 +37811,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37845,7 +37862,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37898,7 +37915,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37951,7 +37968,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -38002,7 +38019,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -38053,7 +38070,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -38104,7 +38121,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38157,7 +38174,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38208,7 +38225,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38261,7 +38278,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38312,7 +38329,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38363,7 +38380,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38416,7 +38433,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38467,7 +38484,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38520,7 +38537,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38622,7 +38639,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38726,7 +38743,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38884,7 +38901,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38937,7 +38954,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -39039,7 +39056,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -39092,7 +39109,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -39101,7 +39118,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39201,7 +39218,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39252,7 +39269,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39305,7 +39322,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39358,7 +39375,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39462,7 +39479,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39560,7 +39577,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39748,7 +39765,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42747,7 +42764,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42764,7 +42781,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42781,7 +42798,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42798,7 +42815,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42817,7 +42834,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42834,7 +42851,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42851,7 +42868,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42868,7 +42885,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42887,7 +42904,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42904,7 +42921,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42921,7 +42938,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42938,7 +42955,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42955,7 +42972,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42974,7 +42991,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -42991,7 +43008,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -43008,7 +43025,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43541,7 +43558,7 @@
   <sheetPr/>
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
@@ -43593,14 +43610,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43613,17 +43630,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43633,7 +43650,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43651,7 +43668,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43667,7 +43684,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43683,7 +43700,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43699,7 +43716,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43715,7 +43732,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43733,17 +43750,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43753,7 +43770,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43771,17 +43788,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43793,17 +43810,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43815,7 +43832,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43823,7 +43840,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43833,7 +43850,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43850,7 +43867,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43867,7 +43884,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43886,7 +43903,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43904,14 +43921,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43924,14 +43941,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43942,7 +43959,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43958,14 +43975,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43976,7 +43993,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -43994,7 +44011,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -44003,7 +44020,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -44014,7 +44031,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44030,7 +44047,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44046,7 +44063,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -44062,7 +44079,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -44078,7 +44095,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -44096,7 +44113,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -44112,7 +44129,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -44128,7 +44145,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -44144,7 +44161,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44160,7 +44177,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44194,14 +44211,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44214,7 +44231,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44230,7 +44247,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44246,7 +44263,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44280,7 +44297,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44296,7 +44313,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44314,7 +44331,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44332,7 +44349,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44350,13 +44367,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44367,7 +44384,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44381,7 +44398,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44395,7 +44412,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44409,7 +44426,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44421,7 +44438,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44435,7 +44452,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44449,7 +44466,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44463,7 +44480,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44477,7 +44494,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44491,7 +44508,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44503,7 +44520,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44520,7 +44537,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44532,7 +44549,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44546,7 +44563,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44563,7 +44580,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44580,13 +44597,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44595,7 +44612,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44609,7 +44626,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44627,7 +44644,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44641,13 +44658,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44658,7 +44675,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44672,7 +44689,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44686,7 +44703,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44700,7 +44717,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44712,7 +44729,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44730,7 +44747,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44744,13 +44761,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44761,7 +44778,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44773,7 +44790,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44787,13 +44804,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44802,7 +44819,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44814,7 +44831,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44828,7 +44845,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44840,7 +44857,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44852,7 +44869,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44864,7 +44881,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44878,13 +44895,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44895,7 +44912,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44909,7 +44926,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44923,7 +44940,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44961,7 +44978,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44975,7 +44992,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -44989,7 +45006,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -45019,7 +45036,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -45033,7 +45050,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -45047,7 +45064,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -45061,7 +45078,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -45075,7 +45092,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -45089,7 +45106,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -45103,7 +45120,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -45117,13 +45134,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45134,7 +45151,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -45148,7 +45165,7 @@
         <v>2239</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45162,7 +45179,7 @@
         <v>2235</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -45176,7 +45193,7 @@
         <v>2303</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45190,7 +45207,7 @@
         <v>2413</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45204,7 +45221,7 @@
         <v>2455</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45218,7 +45235,7 @@
         <v>2469</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45232,7 +45249,7 @@
         <v>2475</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45246,7 +45263,7 @@
         <v>2485</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45260,7 +45277,7 @@
         <v>2520</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45274,7 +45291,7 @@
         <v>2535</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45288,7 +45305,7 @@
         <v>2544</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45302,7 +45319,7 @@
         <v>2582</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -45320,7 +45337,7 @@
         <v>2651</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45334,7 +45351,7 @@
         <v>2652</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45348,7 +45365,7 @@
         <v>2739</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45362,7 +45379,7 @@
         <v>2745</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45376,7 +45393,7 @@
         <v>2769</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45390,7 +45407,7 @@
         <v>2806</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>11</v>
@@ -45770,7 +45787,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -46002,7 +46019,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46019,7 +46036,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -46038,7 +46055,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46057,7 +46074,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -46077,7 +46094,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -46097,7 +46114,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46118,7 +46135,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46138,7 +46155,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46148,10 +46165,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46183,7 +46200,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46203,7 +46220,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46223,7 +46240,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46246,7 +46263,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46266,7 +46283,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46286,19 +46303,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46312,7 +46329,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46330,7 +46347,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46350,7 +46367,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46359,7 +46376,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46373,7 +46390,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46393,7 +46410,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46411,7 +46428,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46431,7 +46448,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46440,10 +46457,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46455,7 +46472,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46475,7 +46492,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46493,7 +46510,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46576,7 +46593,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46596,7 +46613,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46616,7 +46633,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46626,7 +46643,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46638,7 +46655,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46658,7 +46675,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46792,7 +46809,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46806,7 +46823,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46820,7 +46837,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46834,13 +46851,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46851,7 +46868,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46865,7 +46882,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46879,7 +46896,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46893,7 +46910,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -47089,7 +47106,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -47111,13 +47128,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -47131,13 +47148,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -47148,7 +47165,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -47162,7 +47179,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -47176,7 +47193,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -47190,7 +47207,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -47213,7 +47230,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47222,7 +47239,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47273,7 +47290,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47294,14 +47311,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47317,7 +47334,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47352,7 +47369,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47361,7 +47378,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47398,7 +47415,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47419,7 +47436,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47429,7 +47446,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48888,7 +48905,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48903,13 +48920,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48950,7 +48967,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48965,7 +48982,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -49025,7 +49042,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -49038,7 +49055,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -49063,7 +49080,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -49076,7 +49093,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -49089,7 +49106,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -49102,7 +49119,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -49117,7 +49134,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -49132,7 +49149,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -49145,7 +49162,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -49160,7 +49177,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2815 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="1604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3468" uniqueCount="1605">
   <si>
     <t>Date</t>
   </si>
@@ -3732,6 +3732,9 @@
   </si>
   <si>
     <t>Faulty Keyboard</t>
+  </si>
+  <si>
+    <t>Max Pair Sum in an Array</t>
   </si>
   <si>
     <t>Check if a String Is an Acronym of Words</t>
@@ -27041,10 +27044,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I223"/>
+  <dimension ref="A1:I224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+      <selection activeCell="E221" sqref="$A221:$XFD221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -30012,10 +30015,10 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="39">
-        <v>45159</v>
+        <v>45178</v>
       </c>
       <c r="B221" s="1">
-        <v>2828</v>
+        <v>2815</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>1184</v>
@@ -30026,10 +30029,10 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="39">
-        <v>45171</v>
+        <v>45159</v>
       </c>
       <c r="B222" s="1">
-        <v>2833</v>
+        <v>2828</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>1185</v>
@@ -30040,15 +30043,29 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="39">
-        <v>45178</v>
+        <v>45171</v>
       </c>
       <c r="B223" s="1">
-        <v>2843</v>
+        <v>2833</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>1186</v>
       </c>
       <c r="D223" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="39">
+        <v>45178</v>
+      </c>
+      <c r="B224" s="1">
+        <v>2843</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D224" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30435,42 +30452,6 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F220">
-    <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="64" operator="between">
-      <formula>"Amazon"</formula>
-      <formula>"Amazon"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="72" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="80" operator="between">
-      <formula>"Lock"</formula>
-      <formula>"Lock"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="88" operator="between">
-      <formula>"Hard"</formula>
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="96" operator="between">
-      <formula>"Medium"</formula>
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="104" operator="between">
-      <formula>"Easy"</formula>
-      <formula>"Easy"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A210:A217">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
@@ -30541,7 +30522,43 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E205 A195:E196 A189:E193 G195:XFD205 A221:E1048576 G221:XFD1048576">
+  <conditionalFormatting sqref="F220:F221">
+    <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="48" operator="between" text="Amazon">
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="64" operator="between">
+      <formula>"Amazon"</formula>
+      <formula>"Amazon"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="80" operator="between">
+      <formula>"Lock"</formula>
+      <formula>"Lock"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="88" operator="between">
+      <formula>"Hard"</formula>
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="96" operator="between">
+      <formula>"Medium"</formula>
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="104" operator="between">
+      <formula>"Easy"</formula>
+      <formula>"Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E205 A195:E196 A189:E193 G195:XFD205 G222:XFD1048576 A222:E1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30563,7 +30580,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F205 F221:F1048576">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F205 F222:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30797,7 +30814,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G220:XFD220 A220:E220">
+  <conditionalFormatting sqref="G220:XFD221 A220:E221">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30892,7 +30909,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30915,7 +30932,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30935,7 +30952,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30955,7 +30972,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -30975,7 +30992,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -30993,7 +31010,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -31011,7 +31028,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -31029,7 +31046,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -31049,7 +31066,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -31067,7 +31084,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -31085,7 +31102,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -31103,7 +31120,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -31121,7 +31138,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31195,7 +31212,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31213,7 +31230,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31233,7 +31250,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31245,7 +31262,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31258,7 +31275,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31278,7 +31295,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31301,7 +31318,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31322,7 +31339,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31343,7 +31360,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31363,7 +31380,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31381,7 +31398,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31399,7 +31416,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31417,7 +31434,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31435,7 +31452,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31471,7 +31488,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31491,7 +31508,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31500,7 +31517,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31511,7 +31528,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31529,7 +31546,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31551,7 +31568,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31560,7 +31577,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31576,7 +31593,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31602,7 +31619,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31617,7 +31634,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31631,7 +31648,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31645,7 +31662,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31657,7 +31674,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31671,7 +31688,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31683,7 +31700,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31695,7 +31712,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31709,7 +31726,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31723,7 +31740,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -33024,7 +33041,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -33042,7 +33059,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -33064,7 +33081,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -33084,7 +33101,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33104,7 +33121,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -33122,7 +33139,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -33140,7 +33157,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -33158,7 +33175,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33174,7 +33191,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34615,7 +34632,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34636,7 +34653,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34654,7 +34671,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34672,7 +34689,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34690,7 +34707,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34711,7 +34728,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34722,7 +34739,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34732,7 +34749,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34753,7 +34770,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34771,7 +34788,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34789,7 +34806,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34807,7 +34824,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34825,7 +34842,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34843,7 +34860,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34863,7 +34880,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34884,7 +34901,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34903,7 +34920,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34924,7 +34941,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34944,7 +34961,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34962,7 +34979,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -34982,7 +34999,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35002,7 +35019,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35052,7 +35069,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35072,7 +35089,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35090,7 +35107,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -35108,7 +35125,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35126,7 +35143,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -35146,7 +35163,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -35164,7 +35181,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35182,7 +35199,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35200,7 +35217,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35218,7 +35235,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35236,7 +35253,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35254,7 +35271,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35272,7 +35289,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35292,7 +35309,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35310,7 +35327,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35328,7 +35345,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35346,7 +35363,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35366,7 +35383,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35386,7 +35403,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35407,7 +35424,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35427,7 +35444,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35445,7 +35462,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35465,7 +35482,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36715,7 +36732,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36733,7 +36750,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36753,7 +36770,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36768,7 +36785,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36783,7 +36800,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36798,7 +36815,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36807,10 +36824,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36822,14 +36839,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36840,7 +36857,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36860,7 +36877,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36878,7 +36895,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36896,7 +36913,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36916,7 +36933,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36936,7 +36953,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -36972,7 +36989,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -36990,7 +37007,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -37008,7 +37025,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -37026,7 +37043,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -37066,7 +37083,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -37084,7 +37101,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -37104,7 +37121,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -37122,7 +37139,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -37145,7 +37162,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -37166,7 +37183,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37185,7 +37202,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37205,7 +37222,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37227,7 +37244,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37263,7 +37280,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37283,7 +37300,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37303,7 +37320,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37321,7 +37338,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37339,7 +37356,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37357,7 +37374,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37377,7 +37394,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37397,7 +37414,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37417,7 +37434,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37426,10 +37443,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37441,7 +37458,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37459,7 +37476,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37471,7 +37488,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37483,7 +37500,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37498,7 +37515,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37522,7 +37539,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37536,7 +37553,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37548,7 +37565,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37562,7 +37579,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37576,7 +37593,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37588,7 +37605,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37600,7 +37617,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37612,7 +37629,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37624,7 +37641,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37636,7 +37653,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37648,7 +37665,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37660,7 +37677,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37674,7 +37691,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37686,7 +37703,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37698,7 +37715,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37712,7 +37729,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37724,7 +37741,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37736,7 +37753,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37748,7 +37765,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37760,7 +37777,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37811,7 +37828,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37862,7 +37879,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37915,7 +37932,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37968,7 +37985,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -38019,7 +38036,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -38070,7 +38087,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -38121,7 +38138,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38174,7 +38191,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38225,7 +38242,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38278,7 +38295,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38329,7 +38346,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38380,7 +38397,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38433,7 +38450,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38484,7 +38501,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38537,7 +38554,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38639,7 +38656,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38743,7 +38760,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38901,7 +38918,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38954,7 +38971,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -39056,7 +39073,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -39109,7 +39126,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -39118,7 +39135,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39218,7 +39235,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39269,7 +39286,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39322,7 +39339,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39375,7 +39392,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39479,7 +39496,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39577,7 +39594,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39765,7 +39782,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42764,7 +42781,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42781,7 +42798,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42798,7 +42815,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42815,7 +42832,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42834,7 +42851,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42851,7 +42868,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42868,7 +42885,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42885,7 +42902,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42904,7 +42921,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42921,7 +42938,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42938,7 +42955,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42955,7 +42972,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -42972,7 +42989,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -42991,7 +43008,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -43008,7 +43025,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -43025,7 +43042,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43610,14 +43627,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43630,17 +43647,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43650,7 +43667,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43668,7 +43685,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43684,7 +43701,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43700,7 +43717,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43716,7 +43733,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43732,7 +43749,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43750,17 +43767,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43770,7 +43787,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43788,17 +43805,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43810,17 +43827,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43832,7 +43849,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43840,7 +43857,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43850,7 +43867,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43867,7 +43884,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43884,7 +43901,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43903,7 +43920,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43921,14 +43938,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43941,14 +43958,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43959,7 +43976,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -43975,14 +43992,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -43993,7 +44010,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -44011,7 +44028,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -44020,7 +44037,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -44031,7 +44048,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44047,7 +44064,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44063,7 +44080,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -44079,7 +44096,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -44095,7 +44112,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -44113,7 +44130,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -44129,7 +44146,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -44145,7 +44162,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -44161,7 +44178,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44177,7 +44194,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44211,14 +44228,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44231,7 +44248,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44247,7 +44264,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44263,7 +44280,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44297,7 +44314,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44313,7 +44330,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44331,7 +44348,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44349,7 +44366,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44367,13 +44384,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44384,7 +44401,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44398,7 +44415,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44412,7 +44429,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44426,7 +44443,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44438,7 +44455,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44452,7 +44469,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44466,7 +44483,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44480,7 +44497,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44494,7 +44511,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44508,7 +44525,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44520,7 +44537,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44537,7 +44554,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44549,7 +44566,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44563,7 +44580,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44580,7 +44597,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44597,13 +44614,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44612,7 +44629,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44626,7 +44643,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44644,7 +44661,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44658,13 +44675,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44675,7 +44692,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44689,7 +44706,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44703,7 +44720,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44717,7 +44734,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44729,7 +44746,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44747,7 +44764,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44761,13 +44778,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44778,7 +44795,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44790,7 +44807,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44804,13 +44821,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44819,7 +44836,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44831,7 +44848,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44845,7 +44862,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44857,7 +44874,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44869,7 +44886,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44881,7 +44898,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44895,13 +44912,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44912,7 +44929,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44926,7 +44943,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44940,7 +44957,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -44978,7 +44995,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -44992,7 +45009,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -45006,7 +45023,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -45036,7 +45053,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -45050,7 +45067,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -45064,7 +45081,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -45078,7 +45095,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -45092,7 +45109,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -45106,7 +45123,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -45120,7 +45137,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -45134,13 +45151,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45151,7 +45168,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -45165,7 +45182,7 @@
         <v>2239</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45179,7 +45196,7 @@
         <v>2235</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -45193,7 +45210,7 @@
         <v>2303</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45207,7 +45224,7 @@
         <v>2413</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45221,7 +45238,7 @@
         <v>2455</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45235,7 +45252,7 @@
         <v>2469</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45249,7 +45266,7 @@
         <v>2475</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45263,7 +45280,7 @@
         <v>2485</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45277,7 +45294,7 @@
         <v>2520</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45291,7 +45308,7 @@
         <v>2535</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45305,7 +45322,7 @@
         <v>2544</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45319,7 +45336,7 @@
         <v>2582</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -45337,7 +45354,7 @@
         <v>2651</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45351,7 +45368,7 @@
         <v>2652</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45365,7 +45382,7 @@
         <v>2739</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45379,7 +45396,7 @@
         <v>2745</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45393,7 +45410,7 @@
         <v>2769</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45407,7 +45424,7 @@
         <v>2806</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>11</v>
@@ -45787,7 +45804,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -46019,7 +46036,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46036,7 +46053,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -46055,7 +46072,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46074,7 +46091,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -46094,7 +46111,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -46114,7 +46131,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46135,7 +46152,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46155,7 +46172,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46165,10 +46182,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46200,7 +46217,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46220,7 +46237,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46240,7 +46257,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46263,7 +46280,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46283,7 +46300,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46303,19 +46320,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46329,7 +46346,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46347,7 +46364,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46367,7 +46384,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46376,7 +46393,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46390,7 +46407,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46410,7 +46427,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46428,7 +46445,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46448,7 +46465,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46457,10 +46474,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46472,7 +46489,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46492,7 +46509,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46510,7 +46527,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46593,7 +46610,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46613,7 +46630,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46633,7 +46650,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46643,7 +46660,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46655,7 +46672,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -46675,7 +46692,7 @@
         <v>1630</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -46809,7 +46826,7 @@
         <v>1833</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -46823,7 +46840,7 @@
         <v>1874</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -46837,7 +46854,7 @@
         <v>1913</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -46851,13 +46868,13 @@
         <v>2165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -46868,7 +46885,7 @@
         <v>2418</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -46882,7 +46899,7 @@
         <v>2500</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -46896,7 +46913,7 @@
         <v>2733</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -46910,7 +46927,7 @@
         <v>2740</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -47106,7 +47123,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -47128,13 +47145,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>317</v>
@@ -47148,13 +47165,13 @@
         <v>359</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -47165,7 +47182,7 @@
         <v>362</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -47179,7 +47196,7 @@
         <v>705</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -47193,7 +47210,7 @@
         <v>706</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -47207,7 +47224,7 @@
         <v>716</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -47230,7 +47247,7 @@
         <v>901</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -47239,7 +47256,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="19"/>
@@ -47290,7 +47307,7 @@
         <v>1357</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -47311,14 +47328,14 @@
         <v>1476</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="1" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -47334,7 +47351,7 @@
         <v>1570</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -47369,7 +47386,7 @@
         <v>1756</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -47378,7 +47395,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="J17" s="20"/>
       <c r="K17" s="19"/>
@@ -47415,7 +47432,7 @@
         <v>1845</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -47436,7 +47453,7 @@
         <v>1865</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -47446,7 +47463,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="J21" s="14"/>
       <c r="K21" s="22"/>
@@ -48905,7 +48922,7 @@
         <v>525</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -48920,13 +48937,13 @@
         <v>528</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="12.85" spans="1:8">
@@ -48967,7 +48984,7 @@
         <v>974</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -48982,7 +48999,7 @@
         <v>1094</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -49042,7 +49059,7 @@
         <v>1442</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -49055,7 +49072,7 @@
         <v>1524</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -49080,7 +49097,7 @@
         <v>1590</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -49093,7 +49110,7 @@
         <v>1658</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -49106,7 +49123,7 @@
         <v>1788</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>16</v>
@@ -49119,7 +49136,7 @@
         <v>1915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -49134,7 +49151,7 @@
         <v>1983</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -49149,7 +49166,7 @@
         <v>2021</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -49162,7 +49179,7 @@
         <v>2025</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>16</v>
@@ -49177,7 +49194,7 @@
         <v>2067</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Solved problem 2696 Category: String Difficulty: Easy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="9"/>
+    <workbookView windowWidth="15205" windowHeight="5631" tabRatio="991" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="BFS" sheetId="19" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="1606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="1607">
   <si>
     <t>Date</t>
   </si>
@@ -3717,6 +3717,9 @@
   </si>
   <si>
     <t>Number of Senior Citizens</t>
+  </si>
+  <si>
+    <t>Minimum String Length After Removing Substrings</t>
   </si>
   <si>
     <t>Lexicographically Smallest Palindrome</t>
@@ -7652,7 +7655,7 @@
   <sheetPr/>
   <dimension ref="A1:AR118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
@@ -27055,10 +27058,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I224"/>
+  <dimension ref="A1:I225"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="E221" sqref="$A221:$XFD221"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A215" sqref="A215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.10810810810811" defaultRowHeight="12.85"/>
@@ -29942,10 +29945,10 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="39">
-        <v>45140</v>
+        <v>45179</v>
       </c>
       <c r="B215" s="1">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>1179</v>
@@ -29956,10 +29959,10 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="39">
-        <v>45145</v>
+        <v>45140</v>
       </c>
       <c r="B216" s="1">
-        <v>2710</v>
+        <v>2697</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>1180</v>
@@ -29970,10 +29973,10 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="39">
-        <v>45134</v>
+        <v>45145</v>
       </c>
       <c r="B217" s="1">
-        <v>2744</v>
+        <v>2710</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>1181</v>
@@ -29984,40 +29987,40 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="39">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B218" s="1">
-        <v>2785</v>
+        <v>2744</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>1182</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="39">
-        <v>45131</v>
+        <v>45133</v>
       </c>
       <c r="B219" s="1">
-        <v>2788</v>
-      </c>
-      <c r="C219" s="16" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>1183</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="39">
-        <v>45144</v>
+        <v>45131</v>
       </c>
       <c r="B220" s="1">
-        <v>2810</v>
-      </c>
-      <c r="C220" s="1" t="s">
+        <v>2788</v>
+      </c>
+      <c r="C220" s="16" t="s">
         <v>1184</v>
       </c>
       <c r="D220" s="1" t="s">
@@ -30026,10 +30029,10 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="39">
-        <v>45178</v>
+        <v>45144</v>
       </c>
       <c r="B221" s="1">
-        <v>2815</v>
+        <v>2810</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>1185</v>
@@ -30040,10 +30043,10 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="39">
-        <v>45159</v>
+        <v>45178</v>
       </c>
       <c r="B222" s="1">
-        <v>2828</v>
+        <v>2815</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>1186</v>
@@ -30054,10 +30057,10 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="39">
-        <v>45171</v>
+        <v>45159</v>
       </c>
       <c r="B223" s="1">
-        <v>2833</v>
+        <v>2828</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>1187</v>
@@ -30068,15 +30071,29 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" s="39">
-        <v>45178</v>
+        <v>45171</v>
       </c>
       <c r="B224" s="1">
-        <v>2843</v>
+        <v>2833</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>1188</v>
       </c>
       <c r="D224" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="39">
+        <v>45178</v>
+      </c>
+      <c r="B225" s="1">
+        <v>2843</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D225" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -30369,12 +30386,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F218">
+  <conditionalFormatting sqref="F219">
     <cfRule type="containsText" dxfId="5" priority="42" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="50" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F218)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="58" operator="between">
       <formula>"Amazon"</formula>
@@ -30405,7 +30422,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D219">
+  <conditionalFormatting sqref="D220">
     <cfRule type="cellIs" dxfId="0" priority="16" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30427,12 +30444,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F219">
+  <conditionalFormatting sqref="F220">
     <cfRule type="containsText" dxfId="5" priority="41" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="49" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="57" operator="between">
       <formula>"Amazon"</formula>
@@ -30463,7 +30480,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A210:A217">
+  <conditionalFormatting sqref="A210:A218">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30497,7 +30514,7 @@
       <formula>"Lock"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210:F217">
+  <conditionalFormatting sqref="F210:F218">
     <cfRule type="containsText" dxfId="5" priority="26" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F210)))</formula>
     </cfRule>
@@ -30533,12 +30550,12 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F220:F221">
+  <conditionalFormatting sqref="F221:F222">
     <cfRule type="containsText" dxfId="5" priority="40" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F221)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="48" operator="between" text="Amazon">
-      <formula>NOT(ISERROR(SEARCH("Amazon",F220)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Amazon",F221)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="56" operator="between">
       <formula>"Amazon"</formula>
@@ -30569,7 +30586,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E205 A195:E196 A189:E193 G195:XFD205 G222:XFD1048576 A222:E1048576">
+  <conditionalFormatting sqref="G1:XFD187 A172:E179 A1:E170 D171:E171 A171:B171 D180:E180 A180:B180 A181:E187 G189:XFD193 A197:B197 D197:E197 A198:E205 A195:E196 A189:E193 G195:XFD205 A223:E1048576 G223:XFD1048576">
     <cfRule type="cellIs" dxfId="0" priority="206" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30591,7 +30608,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F205 F222:F1048576">
+  <conditionalFormatting sqref="F1:F187 F189:F193 F195:F205 F223:F1048576">
     <cfRule type="containsText" dxfId="5" priority="195" operator="between" text="Amazon">
       <formula>NOT(ISERROR(SEARCH("Amazon",F1)))</formula>
     </cfRule>
@@ -30759,7 +30776,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G210:XFD217 B210:E217">
+  <conditionalFormatting sqref="G210:XFD218 B210:E218">
     <cfRule type="cellIs" dxfId="0" priority="35" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30781,7 +30798,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G218:XFD218 A218:E218">
+  <conditionalFormatting sqref="G219:XFD219 A219:E219">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30803,7 +30820,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G219:XFD219 A219:C219 E219">
+  <conditionalFormatting sqref="G220:XFD220 E220 A220:C220">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30825,7 +30842,7 @@
       <formula>"Easy"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G220:XFD221 A220:E221">
+  <conditionalFormatting sqref="G221:XFD222 A221:E222">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="between">
       <formula>"Lock"</formula>
       <formula>"Lock"</formula>
@@ -30920,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -30943,7 +30960,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -30963,7 +30980,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -30983,7 +31000,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -31003,7 +31020,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -31021,7 +31038,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>16</v>
@@ -31039,7 +31056,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -31057,7 +31074,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -31077,7 +31094,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>11</v>
@@ -31095,7 +31112,7 @@
         <v>92</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -31113,7 +31130,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -31131,7 +31148,7 @@
         <v>114</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>13</v>
@@ -31149,7 +31166,7 @@
         <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -31223,7 +31240,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -31241,7 +31258,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -31261,7 +31278,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
@@ -31273,7 +31290,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="J20" s="20"/>
       <c r="K20" s="19"/>
@@ -31286,7 +31303,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -31306,7 +31323,7 @@
         <v>206</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
@@ -31329,7 +31346,7 @@
         <v>234</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -31350,7 +31367,7 @@
         <v>237</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -31371,7 +31388,7 @@
         <v>328</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -31391,7 +31408,7 @@
         <v>369</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -31409,7 +31426,7 @@
         <v>382</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -31427,7 +31444,7 @@
         <v>445</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -31445,7 +31462,7 @@
         <v>725</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -31463,7 +31480,7 @@
         <v>817</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -31499,7 +31516,7 @@
         <v>986</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -31519,7 +31536,7 @@
         <v>1019</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -31528,7 +31545,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="19"/>
@@ -31539,7 +31556,7 @@
         <v>1171</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -31557,7 +31574,7 @@
         <v>1181</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>13</v>
@@ -31579,7 +31596,7 @@
         <v>1265</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -31588,7 +31605,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -31604,7 +31621,7 @@
         <v>1290</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -31630,7 +31647,7 @@
         <v>1474</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -31645,7 +31662,7 @@
         <v>1634</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -31659,7 +31676,7 @@
         <v>1669</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -31673,7 +31690,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -31685,7 +31702,7 @@
         <v>1836</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -31699,7 +31716,7 @@
         <v>2046</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -31711,7 +31728,7 @@
         <v>2058</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -31723,7 +31740,7 @@
         <v>2074</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -31737,7 +31754,7 @@
         <v>2130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -31751,7 +31768,7 @@
         <v>2181</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -33052,7 +33069,7 @@
         <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -33070,7 +33087,7 @@
         <v>281</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -33092,7 +33109,7 @@
         <v>346</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>11</v>
@@ -33112,7 +33129,7 @@
         <v>862</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -33132,7 +33149,7 @@
         <v>933</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
@@ -33150,7 +33167,7 @@
         <v>1424</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -33168,7 +33185,7 @@
         <v>1438</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>16</v>
@@ -33186,7 +33203,7 @@
         <v>1499</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -33202,7 +33219,7 @@
         <v>1696</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34643,7 +34660,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -34664,7 +34681,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -34682,7 +34699,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -34700,7 +34717,7 @@
         <v>84</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>16</v>
@@ -34718,7 +34735,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -34739,7 +34756,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -34750,7 +34767,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="20" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -34760,7 +34777,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -34781,7 +34798,7 @@
         <v>155</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
@@ -34799,7 +34816,7 @@
         <v>173</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -34817,7 +34834,7 @@
         <v>224</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
@@ -34835,7 +34852,7 @@
         <v>227</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -34853,7 +34870,7 @@
         <v>232</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -34871,7 +34888,7 @@
         <v>255</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>13</v>
@@ -34891,7 +34908,7 @@
         <v>272</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>16</v>
@@ -34912,7 +34929,7 @@
         <v>331</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>13</v>
@@ -34931,7 +34948,7 @@
         <v>341</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -34952,7 +34969,7 @@
         <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -34972,7 +34989,7 @@
         <v>394</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -34990,7 +35007,7 @@
         <v>439</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -35010,7 +35027,7 @@
         <v>456</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -35030,7 +35047,7 @@
         <v>503</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -35080,7 +35097,7 @@
         <v>636</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -35100,7 +35117,7 @@
         <v>682</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -35118,7 +35135,7 @@
         <v>726</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -35136,7 +35153,7 @@
         <v>735</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -35154,7 +35171,7 @@
         <v>736</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>16</v>
@@ -35174,7 +35191,7 @@
         <v>739</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -35192,7 +35209,7 @@
         <v>770</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -35210,7 +35227,7 @@
         <v>772</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>16</v>
@@ -35228,7 +35245,7 @@
         <v>853</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -35246,7 +35263,7 @@
         <v>856</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -35264,7 +35281,7 @@
         <v>872</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -35282,7 +35299,7 @@
         <v>895</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>16</v>
@@ -35300,7 +35317,7 @@
         <v>901</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>13</v>
@@ -35320,7 +35337,7 @@
         <v>921</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -35338,7 +35355,7 @@
         <v>946</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -35356,7 +35373,7 @@
         <v>1003</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -35374,7 +35391,7 @@
         <v>1019</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -35394,7 +35411,7 @@
         <v>1021</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>11</v>
@@ -35414,7 +35431,7 @@
         <v>1047</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -35435,7 +35452,7 @@
         <v>1063</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>16</v>
@@ -35455,7 +35472,7 @@
         <v>1130</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>13</v>
@@ -35473,7 +35490,7 @@
         <v>1190</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>13</v>
@@ -35493,7 +35510,7 @@
         <v>1209</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>13</v>
@@ -36743,7 +36760,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -36761,7 +36778,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
@@ -36781,7 +36798,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -36796,7 +36813,7 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -36811,7 +36828,7 @@
         <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -36826,7 +36843,7 @@
         <v>116</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -36835,10 +36852,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -36850,14 +36867,14 @@
         <v>124</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -36868,7 +36885,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>13</v>
@@ -36888,7 +36905,7 @@
         <v>145</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
@@ -36906,7 +36923,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -36924,7 +36941,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>13</v>
@@ -36944,7 +36961,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
@@ -36964,7 +36981,7 @@
         <v>235</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -37000,7 +37017,7 @@
         <v>297</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -37018,7 +37035,7 @@
         <v>307</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>13</v>
@@ -37036,7 +37053,7 @@
         <v>308</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>16</v>
@@ -37054,7 +37071,7 @@
         <v>315</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>16</v>
@@ -37094,7 +37111,7 @@
         <v>449</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -37112,7 +37129,7 @@
         <v>525</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -37132,7 +37149,7 @@
         <v>530</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -37150,7 +37167,7 @@
         <v>536</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -37173,7 +37190,7 @@
         <v>538</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -37194,7 +37211,7 @@
         <v>543</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>11</v>
@@ -37213,7 +37230,7 @@
         <v>545</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -37233,7 +37250,7 @@
         <v>548</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -37255,7 +37272,7 @@
         <v>559</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>11</v>
@@ -37291,7 +37308,7 @@
         <v>572</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>11</v>
@@ -37311,7 +37328,7 @@
         <v>589</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -37331,7 +37348,7 @@
         <v>590</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>11</v>
@@ -37349,7 +37366,7 @@
         <v>606</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -37367,7 +37384,7 @@
         <v>617</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>11</v>
@@ -37385,7 +37402,7 @@
         <v>623</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>13</v>
@@ -37405,7 +37422,7 @@
         <v>637</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -37425,7 +37442,7 @@
         <v>652</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>13</v>
@@ -37445,7 +37462,7 @@
         <v>653</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>11</v>
@@ -37454,10 +37471,10 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="K39" s="19"/>
     </row>
@@ -37469,7 +37486,7 @@
         <v>654</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>13</v>
@@ -37487,7 +37504,7 @@
         <v>655</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>13</v>
@@ -37499,7 +37516,7 @@
         <v>662</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -37511,7 +37528,7 @@
         <v>663</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -37526,7 +37543,7 @@
         <v>677</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -37550,7 +37567,7 @@
         <v>685</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
@@ -37564,7 +37581,7 @@
         <v>687</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -37576,7 +37593,7 @@
         <v>699</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>16</v>
@@ -37590,7 +37607,7 @@
         <v>700</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -37604,7 +37621,7 @@
         <v>783</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -37616,7 +37633,7 @@
         <v>814</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
@@ -37628,7 +37645,7 @@
         <v>850</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
@@ -37640,7 +37657,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>13</v>
@@ -37652,7 +37669,7 @@
         <v>866</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -37664,7 +37681,7 @@
         <v>889</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -37676,7 +37693,7 @@
         <v>897</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -37688,7 +37705,7 @@
         <v>919</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>13</v>
@@ -37702,7 +37719,7 @@
         <v>938</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -37714,7 +37731,7 @@
         <v>951</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -37726,7 +37743,7 @@
         <v>958</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
@@ -37740,7 +37757,7 @@
         <v>965</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -37752,7 +37769,7 @@
         <v>971</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
@@ -37764,7 +37781,7 @@
         <v>979</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>13</v>
@@ -37776,7 +37793,7 @@
         <v>987</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>13</v>
@@ -37788,7 +37805,7 @@
         <v>988</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>13</v>
@@ -37839,7 +37856,7 @@
         <v>993</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -37890,7 +37907,7 @@
         <v>998</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>13</v>
@@ -37943,7 +37960,7 @@
         <v>1008</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
@@ -37996,7 +38013,7 @@
         <v>1022</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -38047,7 +38064,7 @@
         <v>1026</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -38098,7 +38115,7 @@
         <v>1028</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>16</v>
@@ -38149,7 +38166,7 @@
         <v>1032</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>16</v>
@@ -38202,7 +38219,7 @@
         <v>1038</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -38253,7 +38270,7 @@
         <v>1065</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -38306,7 +38323,7 @@
         <v>1080</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -38357,7 +38374,7 @@
         <v>1104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -38408,7 +38425,7 @@
         <v>1120</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -38461,7 +38478,7 @@
         <v>1123</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -38512,7 +38529,7 @@
         <v>1145</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -38565,7 +38582,7 @@
         <v>1214</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>13</v>
@@ -38667,7 +38684,7 @@
         <v>1261</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -38771,7 +38788,7 @@
         <v>1339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
@@ -38929,7 +38946,7 @@
         <v>1430</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -38982,7 +38999,7 @@
         <v>1443</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -39084,7 +39101,7 @@
         <v>1457</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>13</v>
@@ -39137,7 +39154,7 @@
         <v>1469</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -39146,7 +39163,7 @@
         <v>24</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -39246,7 +39263,7 @@
         <v>1505</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
@@ -39297,7 +39314,7 @@
         <v>1506</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>13</v>
@@ -39350,7 +39367,7 @@
         <v>1516</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
@@ -39403,7 +39420,7 @@
         <v>1519</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>13</v>
@@ -39507,7 +39524,7 @@
         <v>1530</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -39605,7 +39622,7 @@
         <v>1676</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
@@ -39793,7 +39810,7 @@
         <v>2236</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -42792,7 +42809,7 @@
         <v>264</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -42809,7 +42826,7 @@
         <v>295</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -42826,7 +42843,7 @@
         <v>313</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -42843,7 +42860,7 @@
         <v>358</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -42862,7 +42879,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -42879,7 +42896,7 @@
         <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -42896,7 +42913,7 @@
         <v>407</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
@@ -42913,7 +42930,7 @@
         <v>632</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -42932,7 +42949,7 @@
         <v>703</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -42949,7 +42966,7 @@
         <v>846</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -42966,7 +42983,7 @@
         <v>855</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -42983,7 +43000,7 @@
         <v>857</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>16</v>
@@ -43000,7 +43017,7 @@
         <v>871</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -43019,7 +43036,7 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -43036,7 +43053,7 @@
         <v>1057</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -43053,7 +43070,7 @@
         <v>1383</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -43638,14 +43655,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="19"/>
@@ -43658,17 +43675,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="I3" s="19"/>
     </row>
@@ -43678,7 +43695,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -43696,7 +43713,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>11</v>
@@ -43712,7 +43729,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -43728,7 +43745,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>13</v>
@@ -43744,7 +43761,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>13</v>
@@ -43760,7 +43777,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>16</v>
@@ -43778,17 +43795,17 @@
         <v>89</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="14"/>
       <c r="G10" s="14" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -43798,7 +43815,7 @@
         <v>166</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>13</v>
@@ -43816,17 +43833,17 @@
         <v>168</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="14"/>
       <c r="G12" s="14" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -43838,17 +43855,17 @@
         <v>171</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="14"/>
       <c r="G13" s="14" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="I13" s="22"/>
     </row>
@@ -43860,7 +43877,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
@@ -43868,7 +43885,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="29"/>
       <c r="H14" s="14" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -43878,7 +43895,7 @@
         <v>223</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>13</v>
@@ -43895,7 +43912,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>16</v>
@@ -43912,7 +43929,7 @@
         <v>248</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>16</v>
@@ -43931,7 +43948,7 @@
         <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>11</v>
@@ -43949,14 +43966,14 @@
         <v>263</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="14" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="19"/>
@@ -43969,14 +43986,14 @@
         <v>292</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="14" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="19"/>
@@ -43987,7 +44004,7 @@
         <v>319</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>13</v>
@@ -44003,14 +44020,14 @@
         <v>326</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="29" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="19"/>
@@ -44021,7 +44038,7 @@
         <v>335</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>16</v>
@@ -44039,7 +44056,7 @@
         <v>338</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>13</v>
@@ -44048,7 +44065,7 @@
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
       <c r="I24" s="21" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -44059,7 +44076,7 @@
         <v>343</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -44075,7 +44092,7 @@
         <v>365</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -44091,7 +44108,7 @@
         <v>372</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>13</v>
@@ -44107,7 +44124,7 @@
         <v>382</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>13</v>
@@ -44123,7 +44140,7 @@
         <v>386</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>13</v>
@@ -44141,7 +44158,7 @@
         <v>390</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>13</v>
@@ -44157,7 +44174,7 @@
         <v>391</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>16</v>
@@ -44173,7 +44190,7 @@
         <v>398</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>13</v>
@@ -44189,7 +44206,7 @@
         <v>400</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -44205,7 +44222,7 @@
         <v>413</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>13</v>
@@ -44239,14 +44256,14 @@
         <v>441</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="14"/>
       <c r="G36" s="29" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="19"/>
@@ -44259,7 +44276,7 @@
         <v>453</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>11</v>
@@ -44275,7 +44292,7 @@
         <v>458</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>16</v>
@@ -44291,7 +44308,7 @@
         <v>469</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>13</v>
@@ -44325,7 +44342,7 @@
         <v>478</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>13</v>
@@ -44341,7 +44358,7 @@
         <v>497</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>13</v>
@@ -44359,7 +44376,7 @@
         <v>598</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>11</v>
@@ -44377,7 +44394,7 @@
         <v>628</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>11</v>
@@ -44395,13 +44412,13 @@
         <v>728</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44412,7 +44429,7 @@
         <v>812</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -44426,7 +44443,7 @@
         <v>883</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>11</v>
@@ -44440,7 +44457,7 @@
         <v>892</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -44454,7 +44471,7 @@
         <v>908</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -44466,7 +44483,7 @@
         <v>910</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
@@ -44480,7 +44497,7 @@
         <v>914</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -44494,7 +44511,7 @@
         <v>1009</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -44508,7 +44525,7 @@
         <v>1025</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -44522,7 +44539,7 @@
         <v>1079</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>13</v>
@@ -44536,7 +44553,7 @@
         <v>1103</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -44548,7 +44565,7 @@
         <v>1121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>16</v>
@@ -44565,7 +44582,7 @@
         <v>1128</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -44577,7 +44594,7 @@
         <v>1131</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
@@ -44591,7 +44608,7 @@
         <v>1134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -44608,7 +44625,7 @@
         <v>1150</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -44625,13 +44642,13 @@
         <v>1154</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44640,7 +44657,7 @@
         <v>1157</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>16</v>
@@ -44654,7 +44671,7 @@
         <v>1217</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -44672,7 +44689,7 @@
         <v>1232</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -44686,13 +44703,13 @@
         <v>1237</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44703,7 +44720,7 @@
         <v>1266</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -44717,7 +44734,7 @@
         <v>1281</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -44731,7 +44748,7 @@
         <v>1317</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -44745,7 +44762,7 @@
         <v>1323</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -44757,7 +44774,7 @@
         <v>1360</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -44775,7 +44792,7 @@
         <v>1390</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>13</v>
@@ -44789,13 +44806,13 @@
         <v>1432</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44806,7 +44823,7 @@
         <v>1442</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>13</v>
@@ -44818,7 +44835,7 @@
         <v>1447</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>13</v>
@@ -44832,13 +44849,13 @@
         <v>1486</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44847,7 +44864,7 @@
         <v>1492</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>13</v>
@@ -44859,7 +44876,7 @@
         <v>1497</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>13</v>
@@ -44873,7 +44890,7 @@
         <v>1512</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -44885,7 +44902,7 @@
         <v>1513</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>13</v>
@@ -44897,7 +44914,7 @@
         <v>1525</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>13</v>
@@ -44909,7 +44926,7 @@
         <v>1537</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>16</v>
@@ -44923,13 +44940,13 @@
         <v>1551</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -44940,7 +44957,7 @@
         <v>1688</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -44954,7 +44971,7 @@
         <v>1716</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -44968,7 +44985,7 @@
         <v>1742</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -45006,7 +45023,7 @@
         <v>1806</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>13</v>
@@ -45020,7 +45037,7 @@
         <v>1812</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -45034,7 +45051,7 @@
         <v>1837</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -45064,7 +45081,7 @@
         <v>1952</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -45078,7 +45095,7 @@
         <v>1980</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
@@ -45092,7 +45109,7 @@
         <v>2119</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -45106,7 +45123,7 @@
         <v>2113</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>13</v>
@@ -45120,7 +45137,7 @@
         <v>2139</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>13</v>
@@ -45134,7 +45151,7 @@
         <v>2169</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -45148,7 +45165,7 @@
         <v>2177</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>13</v>
@@ -45162,13 +45179,13 @@
         <v>2180</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="1" ht="12.85" spans="1:4">
@@ -45179,7 +45196,7 @@
         <v>2231</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -45193,7 +45210,7 @@
         <v>2239</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>11</v>
@@ -45207,7 +45224,7 @@
         <v>2235</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>11</v>
@@ -45221,7 +45238,7 @@
         <v>2303</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>11</v>
@@ -45235,7 +45252,7 @@
         <v>2413</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>11</v>
@@ -45249,7 +45266,7 @@
         <v>2455</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -45263,7 +45280,7 @@
         <v>2469</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -45277,7 +45294,7 @@
         <v>2475</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>11</v>
@@ -45291,7 +45308,7 @@
         <v>2485</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -45305,7 +45322,7 @@
         <v>2520</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>11</v>
@@ -45319,7 +45336,7 @@
         <v>2535</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -45333,7 +45350,7 @@
         <v>2544</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -45347,7 +45364,7 @@
         <v>2582</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -45365,7 +45382,7 @@
         <v>2651</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -45379,7 +45396,7 @@
         <v>2652</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -45393,7 +45410,7 @@
         <v>2739</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -45407,7 +45424,7 @@
         <v>2745</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -45421,7 +45438,7 @@
         <v>2769</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -45435,7 +45452,7 @@
         <v>2806</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>11</v>
@@ -45815,7 +45832,7 @@
         <v>1114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -46047,7 +46064,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -46064,7 +46081,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
@@ -46083,7 +46100,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -46102,7 +46119,7 @@
         <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -46122,7 +46139,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -46142,7 +46159,7 @@
         <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -46163,7 +46180,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -46183,7 +46200,7 @@
         <v>347</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -46193,10 +46210,10 @@
         <v>90</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="16"/>
@@ -46228,7 +46245,7 @@
         <v>406</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -46248,7 +46265,7 @@
         <v>451</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -46268,7 +46285,7 @@
         <v>692</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -46291,7 +46308,7 @@
         <v>912</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -46311,7 +46328,7 @@
         <v>937</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -46331,19 +46348,19 @@
         <v>973</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="20"/>
@@ -46357,7 +46374,7 @@
         <v>976</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>11</v>
@@ -46375,7 +46392,7 @@
         <v>1054</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -46395,7 +46412,7 @@
         <v>1086</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>11</v>
@@ -46404,7 +46421,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -46418,7 +46435,7 @@
         <v>1094</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>13</v>
@@ -46438,7 +46455,7 @@
         <v>1122</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>11</v>
@@ -46456,7 +46473,7 @@
         <v>1229</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>13</v>
@@ -46476,7 +46493,7 @@
         <v>1356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>11</v>
@@ -46485,10 +46502,10 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -46500,7 +46517,7 @@
         <v>1365</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>11</v>
@@ -46520,7 +46537,7 @@
         <v>1387</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>13</v>
@@ -46538,7 +46555,7 @@
         <v>1451</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>13</v>
@@ -46621,7 +46638,7 @@
         <v>1523</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>11</v>
@@ -46641,7 +46658,7 @@
         <v>1561</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>13</v>
@@ -46661,7 +46678,7 @@
         <v>1588</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>11</v>
@@ -46671,7 +46688,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="23"/>
       <c r="J34" s="14" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="K34" s="19"/>
     </row>
@@ -46683,7 +46700,7 @@
         <v>1608</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="D35" s="14" t